<commit_message>
added basic plotting functionality
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>program_identifier</t>
   </si>
@@ -393,21 +393,21 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="54.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="66.85546875" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="66.86328125" customWidth="1"/>
+    <col min="6" max="6" width="46.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -440,6 +440,9 @@
       <c r="C2">
         <v>1970</v>
       </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
       <c r="E2">
         <v>50</v>
       </c>
@@ -447,7 +450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -464,7 +467,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
fixed typo in estimates, added Best Up Information Program, updated Graphs
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>program_identifier</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>In 2000 Germany reduced the top tax rate from 53% to 42%</t>
+  </si>
+  <si>
+    <t>BestUpInformationWorkshop</t>
+  </si>
+  <si>
+    <t>Best Up College Information Workshop</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>A group of researchers  studied the effect of providing information about the benefits of college education to high school students one year prior to graduation.</t>
+  </si>
+  <si>
+    <t>mentoringBalu</t>
+  </si>
+  <si>
+    <t>Mentoring Program Balu und Du</t>
+  </si>
+  <si>
+    <t>Mentoring</t>
+  </si>
+  <si>
+    <t>Elementary School students were assigned mentors who should encourage the acquisition of new ideas and skills.</t>
   </si>
 </sst>
 </file>
@@ -390,24 +414,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.3984375" customWidth="1"/>
-    <col min="2" max="2" width="15.3984375" customWidth="1"/>
-    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="66.86328125" customWidth="1"/>
-    <col min="6" max="6" width="46.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="66.85546875" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -450,7 +474,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -467,7 +491,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -482,6 +506,46 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>2013</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>19</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>2011</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added headline to program.R files, added Mentoring Program "Balu und Du" based on Falk et. al. (2020)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -57,12 +57,6 @@
     <t>Top Tax Reform</t>
   </si>
   <si>
-    <t>Tax Reform 2000</t>
-  </si>
-  <si>
-    <t>Tax Reform 1990</t>
-  </si>
-  <si>
     <t>short_description</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
   </si>
   <si>
     <t>Elementary School students were assigned mentors who should encourage the acquisition of new ideas and skills.</t>
+  </si>
+  <si>
+    <t>Top Tax Reform 1990</t>
+  </si>
+  <si>
+    <t>Top Tax Reform 2000</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +448,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -479,7 +479,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>1990</v>
@@ -488,7 +488,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -496,7 +496,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>2000</v>
@@ -505,50 +505,51 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>2013</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Tuition Fees, unified returns to schooling assumption
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>program_identifier</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Best Up College Information Workshop</t>
   </si>
   <si>
-    <t>Information</t>
-  </si>
-  <si>
     <t>A group of researchers  studied the effect of providing information about the benefits of college education to high school students one year prior to graduation.</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>Mentoring Program Balu und Du</t>
   </si>
   <si>
-    <t>Mentoring</t>
-  </si>
-  <si>
     <t>Elementary School students were assigned mentors who should encourage the acquisition of new ideas and skills.</t>
   </si>
   <si>
@@ -94,6 +88,24 @@
   </si>
   <si>
     <t>Top Tax Reform 2000</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>tuitionFees</t>
+  </si>
+  <si>
+    <t>Tuition Fees</t>
+  </si>
+  <si>
+    <t>In 2006 and 2007 some German federal states introduced tuition fees of about 1000€ per year. All tuition fees in Germany have since been abolished again. Lower Saxony was the last state to scrap tuition fees in 2015.</t>
+  </si>
+  <si>
+    <t>Between 2007 and 2013 some German federal states shortened the length of the academic high school track "Gymnasium" from 9 to 8 years.</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +491,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>1990</v>
@@ -496,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>2000</v>
@@ -519,33 +531,73 @@
         <v>2013</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E5">
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>2011</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8">
+        <v>2008</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Long Training Active Labor Market Policies based on Lechner et. al. (2011)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>program_identifier</t>
   </si>
@@ -106,6 +106,18 @@
   </si>
   <si>
     <t>Between 2007 and 2013 some German federal states shortened the length of the academic high school track "Gymnasium" from 9 to 8 years.</t>
+  </si>
+  <si>
+    <t>longTraining</t>
+  </si>
+  <si>
+    <t>Long Training</t>
+  </si>
+  <si>
+    <t>Active Labor Market Policy</t>
+  </si>
+  <si>
+    <t>Long Training sponsored Training Program lasting longer than 6 months</t>
   </si>
 </sst>
 </file>
@@ -426,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,6 +612,26 @@
         <v>27</v>
       </c>
     </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>1993</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added class room training and short training (Trainingsmaßnahmen) based on Biewen. et. al. (2014)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>program_identifier</t>
   </si>
@@ -117,7 +117,53 @@
     <t>Active Labor Market Policy</t>
   </si>
   <si>
-    <t>Long Training sponsored Training Program lasting longer than 6 months</t>
+    <t>Government sponsored Training Program lasting longer than 6 months</t>
+  </si>
+  <si>
+    <t>shortTraining</t>
+  </si>
+  <si>
+    <t>Short Training</t>
+  </si>
+  <si>
+    <t>Government sponsored Training Program lasting less less then 6 months</t>
+  </si>
+  <si>
+    <t>practiceFirm</t>
+  </si>
+  <si>
+    <t>Practice Firm</t>
+  </si>
+  <si>
+    <t>Government sponsored training to obtain a new professional degree in a field other than the
+profession currently held</t>
+  </si>
+  <si>
+    <t>Government sponsored training that simulates a job</t>
+  </si>
+  <si>
+    <t>retraining</t>
+  </si>
+  <si>
+    <t>Retraining</t>
+  </si>
+  <si>
+    <t>classRoomTraining</t>
+  </si>
+  <si>
+    <t>Class Room Training</t>
+  </si>
+  <si>
+    <t>Trainingsmaßnahmen</t>
+  </si>
+  <si>
+    <t>Government sponsored short-term training programs "Trainingsmaßnahmen", which where introduced again in 1998 after being abolished in 1993</t>
+  </si>
+  <si>
+    <t>shortTrainingPost1998</t>
+  </si>
+  <si>
+    <t>Government sponsored training that lasts on average 7.5 months.</t>
   </si>
 </sst>
 </file>
@@ -438,24 +484,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="54.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="54.3984375" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" customWidth="1"/>
+    <col min="3" max="3" width="11.1328125" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="66.85546875" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="66.86328125" customWidth="1"/>
+    <col min="6" max="6" width="46.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -498,7 +544,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -515,7 +561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -532,7 +578,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -552,7 +598,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -572,7 +618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -592,7 +638,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -612,7 +658,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -626,10 +672,110 @@
         <v>31</v>
       </c>
       <c r="E9">
-        <v>35</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10">
+        <v>1993</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>1993</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12">
+        <v>1993</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13">
+        <v>2000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>2000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>37</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed shortTrainingPost1998 to trainingMeasures
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -160,10 +160,10 @@
     <t>Government sponsored short-term training programs "Trainingsmaßnahmen", which where introduced again in 1998 after being abolished in 1993</t>
   </si>
   <si>
-    <t>shortTrainingPost1998</t>
-  </si>
-  <si>
     <t>Government sponsored training that lasts on average 7.5 months.</t>
+  </si>
+  <si>
+    <t>trainingMeasures</t>
   </si>
 </sst>
 </file>
@@ -486,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -755,12 +755,12 @@
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
added bridging Allowance also based on Caliendo & Künn (2011)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
   <si>
     <t>program_identifier</t>
   </si>
@@ -154,9 +154,6 @@
     <t>Class Room Training</t>
   </si>
   <si>
-    <t>Trainingsmaßnahmen</t>
-  </si>
-  <si>
     <t>Government sponsored short-term training programs "Trainingsmaßnahmen", which where introduced again in 1998 after being abolished in 1993</t>
   </si>
   <si>
@@ -164,6 +161,30 @@
   </si>
   <si>
     <t>trainingMeasures</t>
+  </si>
+  <si>
+    <t>Training Measures</t>
+  </si>
+  <si>
+    <t>startupSubsidy</t>
+  </si>
+  <si>
+    <t>Start Up Subsidy</t>
+  </si>
+  <si>
+    <t>bridgingAllowance</t>
+  </si>
+  <si>
+    <t>Bridging Allowance</t>
+  </si>
+  <si>
+    <t>average_earnings_beneficiary</t>
+  </si>
+  <si>
+    <t>The bridging allowance "Überbrückungsgeld" was a subsidy equal to the potential unemployment benefit payed to start up founders who would otherwise have been eligible for unemployment benefits. The briding allowance was payed for 6 months.</t>
+  </si>
+  <si>
+    <t>The start up subsidy "Existenzgründungszuschuss" was a subsidy that was payed for 3 years to start up founders who received unemployment benefits before entering self-employment.</t>
   </si>
 </sst>
 </file>
@@ -484,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,9 +520,10 @@
     <col min="5" max="5" width="66.86328125" customWidth="1"/>
     <col min="6" max="6" width="46.73046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -521,10 +543,13 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -540,11 +565,11 @@
       <c r="E2">
         <v>50</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -560,8 +585,9 @@
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -577,8 +603,9 @@
       <c r="F4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -597,8 +624,9 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -617,8 +645,9 @@
       <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -637,8 +666,9 @@
       <c r="F7" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="57" x14ac:dyDescent="0.45">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -657,8 +687,9 @@
       <c r="F8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -677,8 +708,12 @@
       <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G9" s="1">
+        <v>1396</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -697,8 +732,12 @@
       <c r="F10" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G10" s="1">
+        <v>1396</v>
+      </c>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -717,8 +756,12 @@
       <c r="F11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="G11" s="1">
+        <v>1396</v>
+      </c>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -737,8 +780,12 @@
       <c r="F12" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G12" s="1">
+        <v>1396</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -755,15 +802,16 @@
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
       </c>
       <c r="C14">
         <v>2000</v>
@@ -775,8 +823,57 @@
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15">
+        <v>2003</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15">
+        <v>38.86</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1459.3779999999999</v>
+      </c>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>2003</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16">
+        <v>40.17</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="1">
+        <v>2189.3620000000001</v>
+      </c>
+      <c r="H16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added start up Grant "Gründungszuschuss" based on Caliendo et. al. (2015)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>program_identifier</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>The start up subsidy "Existenzgründungszuschuss" was a subsidy that was payed for 3 years to start up founders who received unemployment benefits before entering self-employment.</t>
+  </si>
+  <si>
+    <t>startupGrant</t>
+  </si>
+  <si>
+    <t>Start Up Grant</t>
+  </si>
+  <si>
+    <t>The start up Grant is the follow up program to the  bridging allowance "Überbrückungsgeld" and start up subsidy "Existenzgründungszuschuss" which were replaced in 2006. This subsidy pays the individual unemloyment benefit for 6 months and an additional 300 euros for up to 15 months.</t>
   </si>
 </sst>
 </file>
@@ -505,25 +514,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.3984375" customWidth="1"/>
-    <col min="2" max="2" width="15.3984375" customWidth="1"/>
-    <col min="3" max="3" width="11.1328125" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="66.86328125" customWidth="1"/>
-    <col min="6" max="6" width="46.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="66.85546875" customWidth="1"/>
+    <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,7 +558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -569,7 +578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -587,7 +596,7 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -605,7 +614,7 @@
       </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -626,7 +635,7 @@
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -647,7 +656,7 @@
       </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -668,7 +677,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -689,7 +698,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -713,7 +722,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -737,7 +746,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -761,7 +770,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -785,7 +794,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -806,7 +815,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -827,7 +836,7 @@
       </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="57" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -851,7 +860,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -874,6 +883,29 @@
         <v>2189.3620000000001</v>
       </c>
       <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17">
+        <v>2009</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17">
+        <v>40.969000000000001</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="1">
+        <v>2047.962</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Training Vouchers based on Doerr et al. (2014) & Huber et al. (2018)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>program_identifier</t>
   </si>
@@ -194,6 +194,15 @@
   </si>
   <si>
     <t>The start up Grant is the follow up program to the  bridging allowance "Überbrückungsgeld" and start up subsidy "Existenzgründungszuschuss" which were replaced in 2006. This subsidy pays the individual unemloyment benefit for 6 months and an additional 300 euros for up to 15 months.</t>
+  </si>
+  <si>
+    <t>trainingVoucher</t>
+  </si>
+  <si>
+    <t>Training Voucher</t>
+  </si>
+  <si>
+    <t>Training Vouchers "Bildungsgutscheine" are awarded to unemployed to allow them to participate in training programs usually lasting between several months and 3 years.</t>
   </si>
 </sst>
 </file>
@@ -514,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,6 +916,29 @@
         <v>2047.962</v>
       </c>
     </row>
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18">
+        <v>2003</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18">
+        <v>39.03</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1901.21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added Potential Speed Limit on A3 & A61
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
   <si>
     <t>program_identifier</t>
   </si>
@@ -203,6 +203,24 @@
   </si>
   <si>
     <t>Training Vouchers "Bildungsgutscheine" are awarded to unemployed to allow them to participate in training programs usually lasting between several months and 3 years.</t>
+  </si>
+  <si>
+    <t>speedLimitA3</t>
+  </si>
+  <si>
+    <t>Speed Limit A3</t>
+  </si>
+  <si>
+    <t>Potential Speed Limit of 130 kmph on German Autobahn A3</t>
+  </si>
+  <si>
+    <t>Potential Speed Limit of 130 kmph on German Autobahn A61</t>
+  </si>
+  <si>
+    <t>Speed Limit A61</t>
+  </si>
+  <si>
+    <t>speedLimitA61</t>
   </si>
 </sst>
 </file>
@@ -523,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,6 +957,34 @@
         <v>1901.21</v>
       </c>
     </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19">
+        <v>2015</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20">
+        <v>2015</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added one euro jobs, and two subsidized work programs based on Hohmeyer & Wolff (2010)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t>program_identifier</t>
   </si>
@@ -221,6 +221,33 @@
   </si>
   <si>
     <t>speedLimitA61</t>
+  </si>
+  <si>
+    <t>Job Creation Schemes</t>
+  </si>
+  <si>
+    <t>oneEuroJobs</t>
+  </si>
+  <si>
+    <t>jobCreationSchemes</t>
+  </si>
+  <si>
+    <t>One Euro Jobs "Ein Euro Jobs" are jobs which are assigned to long term unemployed to help them reintegrate into the labor market. These jobs are meant to be unpayed. However, the participants receive a compenstation of at leat one euro per hour worked.</t>
+  </si>
+  <si>
+    <t>One Euro Jobs</t>
+  </si>
+  <si>
+    <t>Job Creation Schemes "Arbeitsbeschaffungsmaßnahmen" are comprised of subsizied jobs aimed at  unemployed who would not be able to find a job otherwise. This measure is mostly employed in local labor markets with excess labor supply. The duration of the subsidy (between 900 and 1300€ payed to the employer) is usually limited to 12 months.</t>
+  </si>
+  <si>
+    <t>subsidizedJobOpportunities</t>
+  </si>
+  <si>
+    <t>Subsidized Job Opportunities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar to  Job Creation Schemes, Subsidized Job Opportunities "Arbeitsgelegenheiten" are jobs where the employer receives a subsidy. The focus of subsidized job opportunities lies on reintegration. The amount of subsidy payed to the employer is not fixed and the types of jobs that can be subsizied  is more broad. </t>
   </si>
 </sst>
 </file>
@@ -541,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,6 +1012,57 @@
         <v>64</v>
       </c>
     </row>
+    <row r="21" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21">
+        <v>2005</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22">
+        <v>2005</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23">
+        <v>2005</v>
+      </c>
+      <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated ALL programs to include additional return values which sum to  government_net_costs and willingness_to_pay respectively
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>program_identifier</t>
   </si>
@@ -248,16 +248,116 @@
   </si>
   <si>
     <t xml:space="preserve">Similar to  Job Creation Schemes, Subsidized Job Opportunities "Arbeitsgelegenheiten" are jobs where the employer receives a subsidy. The focus of subsidized job opportunities lies on reintegration. The amount of subsidy payed to the employer is not fixed and the types of jobs that can be subsizied  is more broad. </t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Papers</t>
+  </si>
+  <si>
+    <t>Chuck &amp; Norris (2014);Du und Ich (2012)</t>
+  </si>
+  <si>
+    <t>https://example.com;https://example.com</t>
+  </si>
+  <si>
+    <t>Atkinson &amp; Piketty (2010);Gottfried &amp; Schellhorn (2004)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ideas.repec.org/p/iaw/iawdip/15.html;https://ideas.repec.org/p/iaw/iawdip/15.html
+</t>
+  </si>
+  <si>
+    <t>Doerrenberg et. al. (2017);Clementi and Gallegati (2005)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://ideas.repec.org/p/arx/papers/physics-0504217.html
+</t>
+  </si>
+  <si>
+    <t>Peter et. al. (2018)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/diw/diwwpp/dp1770.html</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/ces/ceswps/_8382.html</t>
+  </si>
+  <si>
+    <t>Falk et. al. (2020)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/uwp/jhriss/v54y2019i2p468-502.html</t>
+  </si>
+  <si>
+    <t>Marcus &amp; Zambre (2019)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/arx/papers/1909.08299.html;https://ideas.repec.org/a/eee/ecoedu/v41y2014icp14-23.html</t>
+  </si>
+  <si>
+    <t>Gorgen &amp; Schienle (2019);Bruckmeier &amp; Wigger (2014)</t>
+  </si>
+  <si>
+    <t>Lechner et. al. (2011)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/bla/jeurec/v9y2011i4p742-784.html</t>
+  </si>
+  <si>
+    <t>Biewen et. al. (2014)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/ucp/jlabec/doi10.1086-677233.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caliendo &amp; Künn (2011) </t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/pubeco/v95y2011i3p311-331.html</t>
+  </si>
+  <si>
+    <t>Caliendo et. al. (2016)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/eecrev/v86y2016icp87-108.html</t>
+  </si>
+  <si>
+    <t>Doerr et. al. (2014);Huber et al. (2018)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iza/izadps/dp8454.html;https://ideas.repec.org/p/cpr/ceprdp/10650.html</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/zbw/fubsbe/201817.html</t>
+  </si>
+  <si>
+    <t>Thiedig (2018)</t>
+  </si>
+  <si>
+    <t>Hohmeyer &amp; Wolff (2010)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iab/iabdpa/201021.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -280,16 +380,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,9 +690,11 @@
     <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -611,8 +719,14 @@
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -631,8 +745,14 @@
       <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -648,9 +768,14 @@
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -667,8 +792,14 @@
         <v>14</v>
       </c>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -688,8 +819,14 @@
         <v>17</v>
       </c>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -709,8 +846,14 @@
         <v>20</v>
       </c>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -730,8 +873,14 @@
         <v>28</v>
       </c>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -751,8 +900,14 @@
         <v>27</v>
       </c>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -775,8 +930,14 @@
         <v>1396</v>
       </c>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -799,8 +960,14 @@
         <v>1396</v>
       </c>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -823,8 +990,14 @@
         <v>1396</v>
       </c>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -847,8 +1020,14 @@
         <v>1396</v>
       </c>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -868,8 +1047,14 @@
         <v>45</v>
       </c>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -889,8 +1074,14 @@
         <v>44</v>
       </c>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -913,8 +1104,14 @@
         <v>1459.3779999999999</v>
       </c>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>96</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -937,8 +1134,14 @@
         <v>2189.3620000000001</v>
       </c>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>96</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -960,8 +1163,14 @@
       <c r="G17" s="1">
         <v>2047.962</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -983,8 +1192,14 @@
       <c r="G18" s="1">
         <v>1901.21</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -997,8 +1212,14 @@
       <c r="F19" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>103</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1011,8 +1232,14 @@
       <c r="F20" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1028,8 +1255,14 @@
       <c r="F21" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1045,8 +1278,14 @@
       <c r="F22" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1062,9 +1301,33 @@
       <c r="F23" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="I23" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J8" r:id="rId6"/>
+    <hyperlink ref="J7" r:id="rId7"/>
+    <hyperlink ref="J13" r:id="rId8"/>
+    <hyperlink ref="J14" r:id="rId9"/>
+    <hyperlink ref="J17" r:id="rId10"/>
+    <hyperlink ref="J18" r:id="rId11"/>
+    <hyperlink ref="J19" r:id="rId12"/>
+    <hyperlink ref="J20" r:id="rId13"/>
+    <hyperlink ref="J21" r:id="rId14"/>
+    <hyperlink ref="J22" r:id="rId15"/>
+    <hyperlink ref="J23" r:id="rId16"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Long list of changes: - added Maternity Leave Reforms 79, 86, 92 - bicycle helmet law - fixed bug in getSchoolCost
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10875"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="124">
   <si>
     <t>program_identifier</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>In 1990 Germany reduced the top tax rate from 56% to 53%</t>
-  </si>
-  <si>
-    <t>In 2000 Germany reduced the top tax rate from 53% to 42%</t>
   </si>
   <si>
     <t>BestUpInformationWorkshop</t>
@@ -340,6 +337,64 @@
   </si>
   <si>
     <t>https://ideas.repec.org/p/iab/iabdpa/201021.html</t>
+  </si>
+  <si>
+    <t>Between 2001 and 2005 Germany reduced the top tax rate from 53% to 42%</t>
+  </si>
+  <si>
+    <t>Traffic Regulation</t>
+  </si>
+  <si>
+    <t>Sieg (2014);Elvik (2013)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ideas.repec.org/p/mut/wpaper/21.html;https://academic.microsoft.com/paper/2110952839
+</t>
+  </si>
+  <si>
+    <t>bicycleHelmet</t>
+  </si>
+  <si>
+    <t>Mandatory Bicycle Helmet Law</t>
+  </si>
+  <si>
+    <t>Potential introduction of a law which would mandate that every bicycle rider has to wear a helmet</t>
+  </si>
+  <si>
+    <t>maternityLeave79</t>
+  </si>
+  <si>
+    <t>maternityLeave86</t>
+  </si>
+  <si>
+    <t>maternityLeave92</t>
+  </si>
+  <si>
+    <t>Health Program</t>
+  </si>
+  <si>
+    <t>Maternity Leave Reform 1979</t>
+  </si>
+  <si>
+    <t>Maternity Leave Reform 1986</t>
+  </si>
+  <si>
+    <t>Maternity Leave Reform 1992</t>
+  </si>
+  <si>
+    <t>In 1979, the maternity leave coverage was extended  from 2 to 6 months. During these 6 months all entitled mothers received a maternal leave benefit of 750 Deutschmarks per month.</t>
+  </si>
+  <si>
+    <t>The 1986 maternity leave reform extended the period during which mothers had the right to return to their previous job and received maternity benefits from 6 to 10 months. At the same, the maternity benefit was reduced from 750 Deutschmarks to 600 Deutschmarks.</t>
+  </si>
+  <si>
+    <t>In contrast to the maternity leave reforms in 1979 and 1986, the maternity benefit amount as well as the period of entitlement remained unchanged. Instead, the mother's right to return to their previous job was prolonged to 36 months.</t>
+  </si>
+  <si>
+    <t>Dustmann &amp; Schönberg (2011)</t>
+  </si>
+  <si>
+    <t>https://academic.microsoft.com/paper/2075105139/</t>
   </si>
 </sst>
 </file>
@@ -674,16 +729,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="66.85546875" customWidth="1"/>
@@ -714,16 +769,16 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -746,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -757,7 +812,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>1990</v>
@@ -769,10 +824,10 @@
         <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -780,7 +835,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>2000</v>
@@ -789,523 +844,621 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
       </c>
       <c r="C5">
         <v>2013</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>2011</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
       <c r="C8">
         <v>2008</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8">
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
       </c>
       <c r="C9">
         <v>1993</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9">
         <v>35.200000000000003</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="1">
         <v>1396</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" t="s">
         <v>92</v>
-      </c>
-      <c r="J9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
       </c>
       <c r="C10">
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>34.799999999999997</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1">
         <v>1396</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" t="s">
         <v>92</v>
-      </c>
-      <c r="J10" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
       </c>
       <c r="C11">
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="1">
         <v>1396</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" t="s">
         <v>92</v>
-      </c>
-      <c r="J11" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
       </c>
       <c r="C12">
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12">
         <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="1">
         <v>1396</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" t="s">
         <v>92</v>
-      </c>
-      <c r="J12" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
         <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
       </c>
       <c r="C13">
         <v>2000</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
       </c>
       <c r="C14">
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
         <v>48</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
       </c>
       <c r="C15">
         <v>2003</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15">
         <v>38.86</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="1">
         <v>1459.3779999999999</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
       </c>
       <c r="C16">
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E16">
         <v>40.17</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="1">
         <v>2189.3620000000001</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
         <v>55</v>
-      </c>
-      <c r="B17" t="s">
-        <v>56</v>
       </c>
       <c r="C17">
         <v>2009</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17">
         <v>40.969000000000001</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G17" s="1">
         <v>2047.962</v>
       </c>
       <c r="I17" t="s">
+        <v>97</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
         <v>58</v>
-      </c>
-      <c r="B18" t="s">
-        <v>59</v>
       </c>
       <c r="C18">
         <v>2003</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E18">
         <v>39.03</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G18" s="1">
         <v>1901.21</v>
       </c>
       <c r="I18" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
         <v>61</v>
-      </c>
-      <c r="B19" t="s">
-        <v>62</v>
       </c>
       <c r="C19">
         <v>2015</v>
       </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
       <c r="F19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20">
         <v>2015</v>
       </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
       <c r="F20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>2005</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I21" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22">
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
         <v>73</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
       </c>
       <c r="C23">
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>105</v>
+    </row>
+    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24">
+        <v>2012</v>
+      </c>
+      <c r="D24" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I24" t="s">
+        <v>107</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25">
+        <v>1979</v>
+      </c>
+      <c r="D25" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25" t="s">
+        <v>122</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26">
+        <v>1986</v>
+      </c>
+      <c r="D26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I26" t="s">
+        <v>122</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27">
+        <v>1992</v>
+      </c>
+      <c r="D27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I27" t="s">
+        <v>122</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1326,8 +1479,12 @@
     <hyperlink ref="J21" r:id="rId14"/>
     <hyperlink ref="J22" r:id="rId15"/>
     <hyperlink ref="J23" r:id="rId16"/>
+    <hyperlink ref="J24" r:id="rId17"/>
+    <hyperlink ref="J27" r:id="rId18"/>
+    <hyperlink ref="J26" r:id="rId19"/>
+    <hyperlink ref="J25" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added home care subsidy
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
   <si>
     <t>program_identifier</t>
   </si>
@@ -395,6 +395,24 @@
   </si>
   <si>
     <t>https://academic.microsoft.com/paper/2075105139/</t>
+  </si>
+  <si>
+    <t>homeCareSubsidy</t>
+  </si>
+  <si>
+    <t>Home Care Subsidy</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>The home care subsidy "Betreuungsgeld" was introduced in 2013 and was meant to compensate parents who did not make use of subsidised childcare.</t>
+  </si>
+  <si>
+    <t>Collischon et al. (2020)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iza/izadps/dp13271.html</t>
   </si>
 </sst>
 </file>
@@ -729,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D23" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,6 +1477,32 @@
       </c>
       <c r="J27" s="2" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28">
+        <v>2013</v>
+      </c>
+      <c r="D28" t="s">
+        <v>126</v>
+      </c>
+      <c r="E28">
+        <v>31.36</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I28" t="s">
+        <v>128</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1483,8 +1527,9 @@
     <hyperlink ref="J27" r:id="rId18"/>
     <hyperlink ref="J26" r:id="rId19"/>
     <hyperlink ref="J25" r:id="rId20"/>
+    <hyperlink ref="J28" r:id="rId21"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added coronavirus lockdown and parental leave (Elterngeld)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="145">
   <si>
     <t>program_identifier</t>
   </si>
@@ -413,6 +413,51 @@
   </si>
   <si>
     <t>https://ideas.repec.org/p/iza/izadps/dp13271.html</t>
+  </si>
+  <si>
+    <t>parentalLeave2007</t>
+  </si>
+  <si>
+    <t>Parental Leave Reform 2007</t>
+  </si>
+  <si>
+    <t>In 2007, "Elterngeld" was introduced which replaced the fromer parental leave benefit "Erziehungsgeld". Under the new system, the amount of benefit is determined by the net income of the parent who is taking parental leave. For most parents the total benefit payment is higher even though the subsidy is payed for 12 months instead of previously 24 months.</t>
+  </si>
+  <si>
+    <t>Frodermann et al. (2020);Kluve &amp; Tamm (2013)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iza/izadps/dp12935.html;https://ideas.repec.org/a/spr/jopoec/v26y2013i3p983-1005.html</t>
+  </si>
+  <si>
+    <t>coronavirusLockdown</t>
+  </si>
+  <si>
+    <t>coronavirusLockdownR1</t>
+  </si>
+  <si>
+    <t>Coronavirus Lockdown R=0.6</t>
+  </si>
+  <si>
+    <t>Coronavirus Lockdown R=0.6 vs R = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a hypothetical no lockdown scenario which would have left the GDP unchanged and resulted in 560000 deaths.  </t>
+  </si>
+  <si>
+    <t>Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a too lash lockdown which would maintained R=1.</t>
+  </si>
+  <si>
+    <t>Dorn et. al (2020):Flaxman et al. (2020)</t>
+  </si>
+  <si>
+    <t>Dorn et. al (2020)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/ces/ifosdd/06.html</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/ces/ifosdd/06.html;https://academic.microsoft.com/paper/3032971139</t>
   </si>
 </sst>
 </file>
@@ -747,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,6 +1548,81 @@
       </c>
       <c r="J28" s="2" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29">
+        <v>2007</v>
+      </c>
+      <c r="D29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29">
+        <v>29.768270000000001</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2235.6489999999999</v>
+      </c>
+      <c r="I29" t="s">
+        <v>133</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30">
+        <v>2020</v>
+      </c>
+      <c r="D30" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I30" t="s">
+        <v>141</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31">
+        <v>2020</v>
+      </c>
+      <c r="D31" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I31" t="s">
+        <v>142</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1528,8 +1648,11 @@
     <hyperlink ref="J26" r:id="rId19"/>
     <hyperlink ref="J25" r:id="rId20"/>
     <hyperlink ref="J28" r:id="rId21"/>
+    <hyperlink ref="J29" r:id="rId22"/>
+    <hyperlink ref="J30" r:id="rId23"/>
+    <hyperlink ref="J31" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated CPI to include values before 1990, added two Bafög Reforms
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="155">
   <si>
     <t>program_identifier</t>
   </si>
@@ -458,6 +458,36 @@
   </si>
   <si>
     <t>https://ideas.repec.org/a/ces/ifosdd/06.html;https://academic.microsoft.com/paper/3032971139</t>
+  </si>
+  <si>
+    <t>bafoegRepayment</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/diw/diwwpp/dp444.html</t>
+  </si>
+  <si>
+    <t>Baumgartner &amp; Steiner (2004)</t>
+  </si>
+  <si>
+    <t>Bafög 50% Repayment Reform</t>
+  </si>
+  <si>
+    <t>Bafög Refrom 2001</t>
+  </si>
+  <si>
+    <t>bafoeg2001</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iza/izadps/dp2034.html</t>
+  </si>
+  <si>
+    <t>Baumgartner &amp; Steiner (2006)</t>
+  </si>
+  <si>
+    <t>Bafög is a means-tested public German student loan program. Until 1990 students had to repay the entire loan. After the reform about 50% of the loan was offered as a grant which does not have to be payed back.</t>
+  </si>
+  <si>
+    <t>Bafög is a means-tested public German student loan program. Eligible students only have to pay back about 50% of the loan. In 1990, the threshold of parents' income above which students are no longer eligible for Bafög was lowered.</t>
   </si>
 </sst>
 </file>
@@ -792,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1623,6 +1653,58 @@
       </c>
       <c r="J31" s="2" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" t="s">
+        <v>148</v>
+      </c>
+      <c r="C32">
+        <v>1990</v>
+      </c>
+      <c r="D32" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="I32" t="s">
+        <v>147</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C33">
+        <v>2001</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33">
+        <v>19.420999999999999</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I33" t="s">
+        <v>152</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1651,8 +1733,10 @@
     <hyperlink ref="J29" r:id="rId22"/>
     <hyperlink ref="J30" r:id="rId23"/>
     <hyperlink ref="J31" r:id="rId24"/>
+    <hyperlink ref="J32" r:id="rId25"/>
+    <hyperlink ref="J33" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Unemployment Insurance based on Schmieder et al. (2012) & Schmieder & von Wachter (2016)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="167">
   <si>
     <t>program_identifier</t>
   </si>
@@ -488,6 +488,42 @@
   </si>
   <si>
     <t>Bafög is a means-tested public German student loan program. Eligible students only have to pay back about 50% of the loan. In 1990, the threshold of parents' income above which students are no longer eligible for Bafög was lowered.</t>
+  </si>
+  <si>
+    <t>Social Insurance</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/oup/qjecon/v127y2012i2p701-752.html;https://ideas.repec.org/a/anr/reveco/v8y2016p547-581.html</t>
+  </si>
+  <si>
+    <t>A discountinuity at the age of 42 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 42 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>unemploymentBenefits42</t>
+  </si>
+  <si>
+    <t>Unemployment Benefits Age 42</t>
+  </si>
+  <si>
+    <t>Schmieder et al. (2012);Schmieder &amp; von Wachter (2016)</t>
+  </si>
+  <si>
+    <t>Unemployment Benefits Age 44</t>
+  </si>
+  <si>
+    <t>A discountinuity at the age of 44 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 44 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>4unemploymentBenefits44</t>
+  </si>
+  <si>
+    <t>4unemploymentBenefits49</t>
+  </si>
+  <si>
+    <t>Unemployment Benefits Age 49</t>
+  </si>
+  <si>
+    <t>A discountinuity at the age of 49 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 49 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
   </si>
 </sst>
 </file>
@@ -822,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,6 +1741,93 @@
       </c>
       <c r="J33" s="2" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>158</v>
+      </c>
+      <c r="B34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34">
+        <v>1993</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34">
+        <v>42</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1934.5</v>
+      </c>
+      <c r="I34" t="s">
+        <v>160</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35">
+        <v>1993</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35">
+        <v>44</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1928.4169999999999</v>
+      </c>
+      <c r="I35" t="s">
+        <v>160</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" t="s">
+        <v>165</v>
+      </c>
+      <c r="C36">
+        <v>1993</v>
+      </c>
+      <c r="D36" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36">
+        <v>42</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1925.375</v>
+      </c>
+      <c r="I36" t="s">
+        <v>160</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1735,8 +1858,11 @@
     <hyperlink ref="J31" r:id="rId24"/>
     <hyperlink ref="J32" r:id="rId25"/>
     <hyperlink ref="J33" r:id="rId26"/>
+    <hyperlink ref="J34" r:id="rId27"/>
+    <hyperlink ref="J35" r:id="rId28"/>
+    <hyperlink ref="J36" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added a DiD study (Petrunyk & Pfeifer (2018)) that evaluates unemployment benefit cuts for individuals who participated in a rehabilitation program
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="176">
   <si>
     <t>program_identifier</t>
   </si>
@@ -514,16 +514,43 @@
     <t>A discountinuity at the age of 44 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 44 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
   </si>
   <si>
-    <t>4unemploymentBenefits44</t>
-  </si>
-  <si>
-    <t>4unemploymentBenefits49</t>
-  </si>
-  <si>
     <t>Unemployment Benefits Age 49</t>
   </si>
   <si>
     <t>A discountinuity at the age of 49 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 49 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>unemploymentBenefits44</t>
+  </si>
+  <si>
+    <t>unemploymentBenefits49</t>
+  </si>
+  <si>
+    <t>unemploymentBenefits2002</t>
+  </si>
+  <si>
+    <t>Unemployment Benefits Age 45</t>
+  </si>
+  <si>
+    <t>A discountinuity at the age of 45 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 45 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/wly/japmet/v28y2013i4p604-627.html;https://ideas.repec.org/a/anr/reveco/v8y2016p547-581.html</t>
+  </si>
+  <si>
+    <t>Caliendo et al. (2013);Schmieder &amp; von Wachter (2016)</t>
+  </si>
+  <si>
+    <t>Unemployment Benefits Hartz Reform</t>
+  </si>
+  <si>
+    <t>Petrunyk &amp; Pfeifer (2018);Schmieder et al. (2012);Schmieder &amp; von Wachter (2016)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iza/izadps/dp11300.html;https://ideas.repec.org/a/oup/qjecon/v127y2012i2p701-752.html;https://ideas.repec.org/a/anr/reveco/v8y2016p547-581.html</t>
+  </si>
+  <si>
+    <t>In 2006 the unemployment benefit duration was cut as part of the Hartz reforms. In contrast to the other studies which evaluate unemployment benefits, identification is not based on discontinuities in the benefit scheme but rather on the fact that not all age groups were affected by the Hartz reform. The MVPF is calculated for individuals who underwent medical rehabilitation treatments.</t>
   </si>
 </sst>
 </file>
@@ -858,16 +885,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="47" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
     <col min="5" max="5" width="66.85546875" customWidth="1"/>
@@ -1774,7 +1801,7 @@
     </row>
     <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B35" t="s">
         <v>161</v>
@@ -1803,10 +1830,10 @@
     </row>
     <row r="36" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B36" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C36">
         <v>1993</v>
@@ -1818,7 +1845,7 @@
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
@@ -1828,6 +1855,61 @@
       </c>
       <c r="J36" s="2" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>167</v>
+      </c>
+      <c r="B37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37">
+        <v>2002</v>
+      </c>
+      <c r="D37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37">
+        <v>45</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1999.866</v>
+      </c>
+      <c r="I37" t="s">
+        <v>171</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B38" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38">
+        <v>2006</v>
+      </c>
+      <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" s="1">
+        <v>50.492400000000004</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I38" t="s">
+        <v>173</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1861,8 +1943,10 @@
     <hyperlink ref="J34" r:id="rId27"/>
     <hyperlink ref="J35" r:id="rId28"/>
     <hyperlink ref="J36" r:id="rId29"/>
+    <hyperlink ref="J37" r:id="rId30"/>
+    <hyperlink ref="J38" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Job Information Brochure based on Altmann et al. (2018)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="181">
   <si>
     <t>program_identifier</t>
   </si>
@@ -551,13 +551,28 @@
   </si>
   <si>
     <t>In 2006 the unemployment benefit duration was cut as part of the Hartz reforms. In contrast to the other studies which evaluate unemployment benefits, identification is not based on discontinuities in the benefit scheme but rather on the fact that not all age groups were affected by the Hartz reform. The MVPF is calculated for individuals who underwent medical rehabilitation treatments.</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/pubeco/v164y2018icp33-49.html</t>
+  </si>
+  <si>
+    <t>Altmann et al. (2018)</t>
+  </si>
+  <si>
+    <t>jobSearchInformation</t>
+  </si>
+  <si>
+    <t>Job Search Information Brochure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As part of a randomized field experiment a brochure that informs about the benefits of job search and the consequences of unemployment was sent to newly registered unemployed. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,6 +584,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -595,7 +617,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -604,6 +626,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -885,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,6 +1933,35 @@
       </c>
       <c r="J38" s="2" t="s">
         <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" t="s">
+        <v>179</v>
+      </c>
+      <c r="C39">
+        <v>2011</v>
+      </c>
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39">
+        <v>36.92</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1593.2249999999999</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1945,8 +1997,9 @@
     <hyperlink ref="J36" r:id="rId29"/>
     <hyperlink ref="J37" r:id="rId30"/>
     <hyperlink ref="J38" r:id="rId31"/>
+    <hyperlink ref="J39" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added negative Income Tax Experiment
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="198">
   <si>
     <t>program_identifier</t>
   </si>
@@ -596,13 +596,34 @@
   </si>
   <si>
     <t>Familiy Policy</t>
+  </si>
+  <si>
+    <t>unemploymentBenefits2006</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iza/izadps/dp2067.html</t>
+  </si>
+  <si>
+    <t>Spermann &amp; Strotmann (2006)</t>
+  </si>
+  <si>
+    <t>Spermann &amp; Strotmann (2006) evaluate the effects of what they call a negative income tax experiment. This is misleading because the experiment they are describing does not resemble what is typically considered a negative income tax as proposed by Milton Friedman. In the sense of Friedman, a negative income tax is a basic income that is gradually phased-out with increasing gross earnings. Instead, Spermann &amp; Strotmann (2006) consider a experiment where long-term unemployed receive a  subsidy on top of their gross wage. The subsidy increases with the wage and can reach a maximum of up to 643 Deutschmark.</t>
+  </si>
+  <si>
+    <t>Tax Reform</t>
+  </si>
+  <si>
+    <t>negativeIncomeTax</t>
+  </si>
+  <si>
+    <t>Negative Income Tax Experiment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -631,6 +652,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -653,7 +681,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -664,6 +692,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -945,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1948,7 +1977,7 @@
     </row>
     <row r="38" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="B38" t="s">
         <v>169</v>
@@ -2057,6 +2086,35 @@
       </c>
       <c r="J41" s="2" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>196</v>
+      </c>
+      <c r="B42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C42">
+        <v>2001</v>
+      </c>
+      <c r="D42" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42">
+        <v>39.612000000000002</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1278.2249999999999</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2095,8 +2153,9 @@
     <hyperlink ref="J39" r:id="rId32"/>
     <hyperlink ref="J40" r:id="rId33"/>
     <hyperlink ref="J41" r:id="rId34"/>
+    <hyperlink ref="J42" r:id="rId35"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
removed testProgram and added placementService based on Krug & Stephan (2017)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -36,16 +36,7 @@
     <t>notes</t>
   </si>
   <si>
-    <t>testProgram</t>
-  </si>
-  <si>
-    <t>Test if everything works as expected</t>
-  </si>
-  <si>
     <t>program_name</t>
-  </si>
-  <si>
-    <t>Test Program</t>
   </si>
   <si>
     <t>taxReform1990</t>
@@ -250,12 +241,6 @@
     <t>Papers</t>
   </si>
   <si>
-    <t>Chuck &amp; Norris (2014);Du und Ich (2012)</t>
-  </si>
-  <si>
-    <t>https://example.com;https://example.com</t>
-  </si>
-  <si>
     <t>Atkinson &amp; Piketty (2010);Gottfried &amp; Schellhorn (2004)</t>
   </si>
   <si>
@@ -617,6 +602,21 @@
   </si>
   <si>
     <t>Negative Income Tax Experiment</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/iza/izadps/dp7403.html</t>
+  </si>
+  <si>
+    <t>Krug &amp; Stephan (2017)</t>
+  </si>
+  <si>
+    <t>Intensive Placement Services for unemployed can either be provided by the employment agency itself or it can be outsourced to a private contractor. The former is more expensive, but unemployed tend to show better labor market outcomes.</t>
+  </si>
+  <si>
+    <t>Inhouse Placement Service</t>
+  </si>
+  <si>
+    <t>placementService</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +999,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1011,95 +1011,96 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C2">
-        <v>1970</v>
+        <v>1990</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>2013</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="C3">
-        <v>1990</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E4">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>80</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1107,104 +1108,107 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" t="s">
-        <v>82</v>
+      <c r="I5" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>85</v>
+      <c r="I6" t="s">
+        <v>82</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
       <c r="C7">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E7">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>182</v>
       </c>
       <c r="E8">
-        <v>21</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1396</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>89</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
+      </c>
+      <c r="J8" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1218,10 +1222,10 @@
         <v>1993</v>
       </c>
       <c r="D9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E9">
-        <v>35.200000000000003</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>30</v>
@@ -1231,13 +1235,13 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1248,200 +1252,199 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E10">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
       </c>
       <c r="G10" s="1">
         <v>1396</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C11">
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E11">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="G11" s="1">
         <v>1396</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="J11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s">
-        <v>39</v>
-      </c>
       <c r="C12">
-        <v>1993</v>
+        <v>2000</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E12">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1396</v>
+        <v>40</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>2000</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E13">
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
       <c r="C14">
-        <v>2000</v>
+        <v>2003</v>
       </c>
       <c r="D14" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E14">
-        <v>37</v>
+        <v>38.86</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1459.3779999999999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
         <v>46</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
       </c>
       <c r="C15">
         <v>2003</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E15">
-        <v>38.86</v>
+        <v>40.17</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G15" s="1">
-        <v>1459.3779999999999</v>
+        <v>2189.3620000000001</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C16">
-        <v>2003</v>
+        <v>2009</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E16">
-        <v>40.17</v>
+        <v>40.969000000000001</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G16" s="1">
-        <v>2189.3620000000001</v>
-      </c>
-      <c r="H16" s="1"/>
+        <v>2047.962</v>
+      </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1449,28 +1452,28 @@
         <v>54</v>
       </c>
       <c r="C17">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E17">
-        <v>40.969000000000001</v>
+        <v>39.03</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G17" s="1">
-        <v>2047.962</v>
+        <v>1901.21</v>
       </c>
       <c r="I17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1478,30 +1481,24 @@
         <v>57</v>
       </c>
       <c r="C18">
-        <v>2003</v>
+        <v>2015</v>
       </c>
       <c r="D18" t="s">
-        <v>187</v>
-      </c>
-      <c r="E18">
-        <v>39.03</v>
+        <v>100</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G18" s="1">
-        <v>1901.21</v>
-      </c>
       <c r="I18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
         <v>60</v>
@@ -1510,67 +1507,67 @@
         <v>2015</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
       <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
+        <v>2005</v>
+      </c>
+      <c r="D20" t="s">
+        <v>182</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" t="s">
+        <v>97</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>63</v>
       </c>
-      <c r="C20">
-        <v>2015</v>
-      </c>
-      <c r="D20" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" t="s">
-        <v>101</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>67</v>
-      </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>2005</v>
       </c>
       <c r="D21" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="I21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>69</v>
@@ -1579,122 +1576,125 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="I22" t="s">
+        <v>97</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23">
+        <v>2012</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23">
-        <v>2005</v>
-      </c>
-      <c r="D23" t="s">
-        <v>187</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24">
+        <v>1979</v>
+      </c>
+      <c r="D24" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I24" t="s">
+        <v>116</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25">
+        <v>1986</v>
+      </c>
+      <c r="D25" t="s">
+        <v>185</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25" t="s">
+        <v>116</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>108</v>
       </c>
-      <c r="B24" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24">
-        <v>2012</v>
-      </c>
-      <c r="D24" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I24" t="s">
-        <v>106</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
+        <v>112</v>
+      </c>
+      <c r="C26">
+        <v>1992</v>
+      </c>
+      <c r="D26" t="s">
+        <v>185</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C25">
-        <v>1979</v>
-      </c>
-      <c r="D25" t="s">
-        <v>190</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="I26" t="s">
+        <v>116</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>118</v>
       </c>
-      <c r="I25" t="s">
-        <v>121</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B26" t="s">
-        <v>116</v>
-      </c>
-      <c r="C26">
-        <v>1986</v>
-      </c>
-      <c r="D26" t="s">
-        <v>190</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="B27" t="s">
         <v>119</v>
       </c>
-      <c r="I26" t="s">
-        <v>121</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" t="s">
-        <v>117</v>
-      </c>
       <c r="C27">
-        <v>1992</v>
+        <v>2013</v>
       </c>
       <c r="D27" t="s">
-        <v>190</v>
+        <v>185</v>
+      </c>
+      <c r="E27">
+        <v>31.36</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>120</v>
@@ -1706,7 +1706,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -1714,17 +1714,20 @@
         <v>124</v>
       </c>
       <c r="C28">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="D28" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E28">
-        <v>31.36</v>
+        <v>29.768270000000001</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="G28" s="1">
+        <v>2235.6489999999999</v>
+      </c>
       <c r="I28" t="s">
         <v>126</v>
       </c>
@@ -1732,79 +1735,76 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>128</v>
       </c>
       <c r="B29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29">
+        <v>2020</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I29" t="s">
+        <v>134</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>129</v>
       </c>
-      <c r="C29">
-        <v>2007</v>
-      </c>
-      <c r="D29" t="s">
-        <v>190</v>
-      </c>
-      <c r="E29">
-        <v>29.768270000000001</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29" s="1">
-        <v>2235.6489999999999</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="B30" t="s">
         <v>131</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>133</v>
-      </c>
-      <c r="B30" t="s">
-        <v>135</v>
       </c>
       <c r="C30">
         <v>2020</v>
       </c>
       <c r="D30" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B31" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C31">
-        <v>2020</v>
+        <v>1990</v>
       </c>
       <c r="D31" t="s">
-        <v>114</v>
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <v>19.809999999999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="I31" t="s">
         <v>140</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -1812,19 +1812,19 @@
         <v>143</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C32">
-        <v>1990</v>
+        <v>2001</v>
       </c>
       <c r="D32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E32">
-        <v>19.809999999999999</v>
+        <v>19.420999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="I32" t="s">
         <v>145</v>
@@ -1833,288 +1833,291 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33">
+        <v>1993</v>
+      </c>
+      <c r="D33" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33">
+        <v>42</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1934.5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>152</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="B33" t="s">
-        <v>147</v>
-      </c>
-      <c r="C33">
-        <v>2001</v>
-      </c>
-      <c r="D33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33">
-        <v>19.420999999999999</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I33" t="s">
-        <v>150</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B34" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E34">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>154</v>
       </c>
       <c r="G34" s="1">
-        <v>1934.5</v>
+        <v>1928.4169999999999</v>
       </c>
       <c r="I34" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E35">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G35" s="1">
-        <v>1928.4169999999999</v>
+        <v>1925.375</v>
       </c>
       <c r="I35" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B36" t="s">
         <v>160</v>
       </c>
       <c r="C36">
-        <v>1993</v>
+        <v>2002</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E36">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>161</v>
       </c>
       <c r="G36" s="1">
-        <v>1925.375</v>
+        <v>1999.866</v>
       </c>
       <c r="I36" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37" t="s">
         <v>164</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37">
+        <v>2006</v>
+      </c>
+      <c r="D37" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" s="1">
+        <v>50.492400000000004</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I37" t="s">
         <v>165</v>
       </c>
-      <c r="C37">
-        <v>2002</v>
-      </c>
-      <c r="D37" t="s">
-        <v>188</v>
-      </c>
-      <c r="E37">
-        <v>45</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="J37" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="G37" s="1">
-        <v>1999.866</v>
-      </c>
-      <c r="I37" t="s">
-        <v>168</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B38" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C38">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="D38" t="s">
-        <v>188</v>
-      </c>
-      <c r="E38" s="1">
-        <v>50.492400000000004</v>
+        <v>182</v>
+      </c>
+      <c r="E38">
+        <v>36.92</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I38" t="s">
-        <v>170</v>
+      <c r="G38" s="1">
+        <v>1593.2249999999999</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>173</v>
+      </c>
+      <c r="B39" t="s">
+        <v>174</v>
+      </c>
+      <c r="C39">
+        <v>2006</v>
+      </c>
+      <c r="D39" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39">
+        <v>37.71</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B39" t="s">
+      <c r="G39" s="1">
+        <v>2624.9580000000001</v>
+      </c>
+      <c r="I39" t="s">
         <v>176</v>
       </c>
-      <c r="C39">
-        <v>2011</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="J39" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>184</v>
+      </c>
+      <c r="B40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C40">
+        <v>2004</v>
+      </c>
+      <c r="D40" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40">
+        <v>37.630000000000003</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G40">
+        <v>2731</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" t="s">
+        <v>192</v>
+      </c>
+      <c r="C41">
+        <v>2001</v>
+      </c>
+      <c r="D41" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41">
+        <v>39.612000000000002</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1278.2249999999999</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E39">
-        <v>36.92</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G39" s="1">
-        <v>1593.2249999999999</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>178</v>
-      </c>
-      <c r="B40" t="s">
-        <v>179</v>
-      </c>
-      <c r="C40">
-        <v>2006</v>
-      </c>
-      <c r="D40" t="s">
-        <v>187</v>
-      </c>
-      <c r="E40">
-        <v>37.71</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="G40" s="1">
-        <v>2624.9580000000001</v>
-      </c>
-      <c r="I40" t="s">
-        <v>181</v>
-      </c>
-      <c r="J40" s="2" t="s">
+    </row>
+    <row r="42" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>197</v>
+      </c>
+      <c r="B42" t="s">
+        <v>196</v>
+      </c>
+      <c r="C42">
+        <v>2009</v>
+      </c>
+      <c r="D42" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" t="s">
-        <v>185</v>
-      </c>
-      <c r="C41">
-        <v>2004</v>
-      </c>
-      <c r="D41" t="s">
-        <v>114</v>
-      </c>
-      <c r="E41">
-        <v>37.630000000000003</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="G41">
-        <v>2731</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="210" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>196</v>
-      </c>
-      <c r="B42" t="s">
-        <v>197</v>
-      </c>
-      <c r="C42">
-        <v>2001</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="E42">
+        <v>50.181100000000001</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="E42">
-        <v>39.612000000000002</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1">
+        <v>1543.018</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="G42" s="1">
-        <v>1278.2249999999999</v>
-      </c>
-      <c r="I42" s="6" t="s">
+      <c r="J42" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2123,11 +2126,11 @@
     <hyperlink ref="J3" r:id="rId2"/>
     <hyperlink ref="J4" r:id="rId3"/>
     <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J6" r:id="rId5"/>
-    <hyperlink ref="J8" r:id="rId6"/>
-    <hyperlink ref="J7" r:id="rId7"/>
+    <hyperlink ref="J7" r:id="rId5"/>
+    <hyperlink ref="J6" r:id="rId6"/>
+    <hyperlink ref="J12" r:id="rId7"/>
     <hyperlink ref="J13" r:id="rId8"/>
-    <hyperlink ref="J14" r:id="rId9"/>
+    <hyperlink ref="J16" r:id="rId9"/>
     <hyperlink ref="J17" r:id="rId10"/>
     <hyperlink ref="J18" r:id="rId11"/>
     <hyperlink ref="J19" r:id="rId12"/>
@@ -2135,10 +2138,10 @@
     <hyperlink ref="J21" r:id="rId14"/>
     <hyperlink ref="J22" r:id="rId15"/>
     <hyperlink ref="J23" r:id="rId16"/>
-    <hyperlink ref="J24" r:id="rId17"/>
-    <hyperlink ref="J27" r:id="rId18"/>
-    <hyperlink ref="J26" r:id="rId19"/>
-    <hyperlink ref="J25" r:id="rId20"/>
+    <hyperlink ref="J26" r:id="rId17"/>
+    <hyperlink ref="J25" r:id="rId18"/>
+    <hyperlink ref="J24" r:id="rId19"/>
+    <hyperlink ref="J27" r:id="rId20"/>
     <hyperlink ref="J28" r:id="rId21"/>
     <hyperlink ref="J29" r:id="rId22"/>
     <hyperlink ref="J30" r:id="rId23"/>

</xml_diff>

<commit_message>
fixed a couple of small issues. (Wrong meta assumptions, missing price info ...)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -427,9 +427,6 @@
     <t>Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a too lash lockdown which would maintained R=1.</t>
   </si>
   <si>
-    <t>Dorn et. al (2020):Flaxman et al. (2020)</t>
-  </si>
-  <si>
     <t>Dorn et. al (2020)</t>
   </si>
   <si>
@@ -451,9 +448,6 @@
     <t>Bafög 50% Repayment Reform</t>
   </si>
   <si>
-    <t>Bafög Refrom 2001</t>
-  </si>
-  <si>
     <t>bafoeg2001</t>
   </si>
   <si>
@@ -617,6 +611,12 @@
   </si>
   <si>
     <t>placementService</t>
+  </si>
+  <si>
+    <t>Bafög Reform 2001</t>
+  </si>
+  <si>
+    <t>Dorn et. al (2020);Flaxman et al. (2020)</t>
   </si>
 </sst>
 </file>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1192,7 @@
         <v>1993</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E8">
         <v>35.200000000000003</v>
@@ -1222,7 +1222,7 @@
         <v>1993</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E9">
         <v>34.799999999999997</v>
@@ -1252,7 +1252,7 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E10">
         <v>36</v>
@@ -1282,7 +1282,7 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E11">
         <v>31</v>
@@ -1312,7 +1312,7 @@
         <v>2000</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E12">
         <v>37</v>
@@ -1339,7 +1339,7 @@
         <v>2000</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E13">
         <v>37</v>
@@ -1366,7 +1366,7 @@
         <v>2003</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E14">
         <v>38.86</v>
@@ -1396,7 +1396,7 @@
         <v>2003</v>
       </c>
       <c r="D15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E15">
         <v>40.17</v>
@@ -1426,7 +1426,7 @@
         <v>2009</v>
       </c>
       <c r="D16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E16">
         <v>40.969000000000001</v>
@@ -1455,7 +1455,7 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E17">
         <v>39.03</v>
@@ -1530,7 +1530,7 @@
         <v>2005</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>67</v>
@@ -1553,7 +1553,7 @@
         <v>2005</v>
       </c>
       <c r="D21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>65</v>
@@ -1576,7 +1576,7 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>70</v>
@@ -1622,7 +1622,7 @@
         <v>1979</v>
       </c>
       <c r="D24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>113</v>
@@ -1645,7 +1645,7 @@
         <v>1986</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>114</v>
@@ -1668,7 +1668,7 @@
         <v>1992</v>
       </c>
       <c r="D26" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>115</v>
@@ -1691,7 +1691,7 @@
         <v>2013</v>
       </c>
       <c r="D27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E27">
         <v>31.36</v>
@@ -1717,7 +1717,7 @@
         <v>2007</v>
       </c>
       <c r="D28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E28">
         <v>29.768270000000001</v>
@@ -1752,10 +1752,10 @@
         <v>132</v>
       </c>
       <c r="I29" t="s">
-        <v>134</v>
+        <v>197</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1775,18 +1775,18 @@
         <v>133</v>
       </c>
       <c r="I30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C31">
         <v>1990</v>
@@ -1798,21 +1798,21 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="I31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B32" t="s">
-        <v>142</v>
+        <v>196</v>
       </c>
       <c r="C32">
         <v>2001</v>
@@ -1824,221 +1824,221 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="I32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C33">
         <v>1993</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E33">
         <v>42</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G33" s="1">
         <v>1934.5</v>
       </c>
       <c r="I33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E34">
         <v>44</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G34" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E35">
         <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G35" s="1">
         <v>1925.375</v>
       </c>
       <c r="I35" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B36" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C36">
         <v>2002</v>
       </c>
       <c r="D36" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E36">
         <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G36" s="1">
         <v>1999.866</v>
       </c>
       <c r="I36" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B37" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C37">
         <v>2006</v>
       </c>
       <c r="D37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E37" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C38">
         <v>2011</v>
       </c>
       <c r="D38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E38">
         <v>36.92</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G38" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B39" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C39">
         <v>2006</v>
       </c>
       <c r="D39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E39">
         <v>37.71</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G39" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I39" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C40">
         <v>2004</v>
@@ -2050,74 +2050,74 @@
         <v>37.630000000000003</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G40">
         <v>2731</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C41">
         <v>2001</v>
       </c>
       <c r="D41" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E41">
         <v>39.612000000000002</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G41" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B42" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C42">
         <v>2009</v>
       </c>
       <c r="D42" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E42">
         <v>50.181100000000001</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G42" s="1">
         <v>1543.018</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Latex Table export. Added citationkeys to programs. A couple of small fixes
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="228">
   <si>
     <t>program_identifier</t>
   </si>
@@ -244,10 +244,6 @@
     <t>Atkinson &amp; Piketty (2010);Gottfried &amp; Schellhorn (2004)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ideas.repec.org/p/iaw/iawdip/15.html;https://ideas.repec.org/p/iaw/iawdip/15.html
-</t>
-  </si>
-  <si>
     <t>Doerrenberg et. al. (2017);Clementi and Gallegati (2005)</t>
   </si>
   <si>
@@ -303,12 +299,6 @@
     <t>https://ideas.repec.org/a/eee/eecrev/v86y2016icp87-108.html</t>
   </si>
   <si>
-    <t>Doerr et. al. (2014);Huber et al. (2018)</t>
-  </si>
-  <si>
-    <t>https://ideas.repec.org/p/iza/izadps/dp8454.html;https://ideas.repec.org/p/cpr/ceprdp/10650.html</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/p/zbw/fubsbe/201817.html</t>
   </si>
   <si>
@@ -445,9 +435,6 @@
     <t>Baumgartner &amp; Steiner (2004)</t>
   </si>
   <si>
-    <t>Bafög 50% Repayment Reform</t>
-  </si>
-  <si>
     <t>bafoeg2001</t>
   </si>
   <si>
@@ -601,9 +588,6 @@
     <t>https://ideas.repec.org/p/iza/izadps/dp7403.html</t>
   </si>
   <si>
-    <t>Krug &amp; Stephan (2017)</t>
-  </si>
-  <si>
     <t>Intensive Placement Services for unemployed can either be provided by the employment agency itself or it can be outsourced to a private contractor. The former is more expensive, but unemployed tend to show better labor market outcomes.</t>
   </si>
   <si>
@@ -617,6 +601,112 @@
   </si>
   <si>
     <t>Dorn et. al (2020);Flaxman et al. (2020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ideas.repec.org/b/oxp/obooks/9780199286898.html;https://ideas.repec.org/p/iaw/iawdip/15.html
+</t>
+  </si>
+  <si>
+    <t>bibtexkeys</t>
+  </si>
+  <si>
+    <t>atkinson2010;gottfried2004</t>
+  </si>
+  <si>
+    <t>doerrenberg2017;clementi2005</t>
+  </si>
+  <si>
+    <t>peter2018</t>
+  </si>
+  <si>
+    <t>falk2020</t>
+  </si>
+  <si>
+    <t>marcus2019</t>
+  </si>
+  <si>
+    <t>lechner2011</t>
+  </si>
+  <si>
+    <t>biewen2014</t>
+  </si>
+  <si>
+    <t>caliendo2016</t>
+  </si>
+  <si>
+    <t>gorgen2019;bruckmeier2014</t>
+  </si>
+  <si>
+    <t>hohmeyer2010</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/sae/ilrrev/v70y2017i3p767-812.html;https://ideas.repec.org/p/iza/izadps/dp9138.html</t>
+  </si>
+  <si>
+    <t>doerr2014;huber2015</t>
+  </si>
+  <si>
+    <t>Doerr et. al. (2014);Huber et al. (2015)</t>
+  </si>
+  <si>
+    <t>thiedig2018</t>
+  </si>
+  <si>
+    <t>sieg2014;elvik2011</t>
+  </si>
+  <si>
+    <t>dustmann2012</t>
+  </si>
+  <si>
+    <t>collischon2020</t>
+  </si>
+  <si>
+    <t>kluve2013;frodermann2020</t>
+  </si>
+  <si>
+    <t>dorn2020;flaxman2020</t>
+  </si>
+  <si>
+    <t>dorn2020</t>
+  </si>
+  <si>
+    <t>baumgartner2004</t>
+  </si>
+  <si>
+    <t>baumgartner2006</t>
+  </si>
+  <si>
+    <t>schmieder2012;schmieder2016</t>
+  </si>
+  <si>
+    <t>caliendo2013;schmieder2016</t>
+  </si>
+  <si>
+    <t>petrunyk2018;schmieder2012;schmieder2016</t>
+  </si>
+  <si>
+    <t>altmann2018</t>
+  </si>
+  <si>
+    <t>pawlowski2019</t>
+  </si>
+  <si>
+    <t>spermann2006</t>
+  </si>
+  <si>
+    <t>caliendo2011b</t>
+  </si>
+  <si>
+    <t>caliendo2011a</t>
+  </si>
+  <si>
+    <t>Krug &amp; Stephan (2013)</t>
+  </si>
+  <si>
+    <t>krug2013</t>
+  </si>
+  <si>
+    <t>Bafög Repayment Reform</t>
   </si>
 </sst>
 </file>
@@ -681,7 +771,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -693,6 +783,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -974,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F25" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,9 +1085,10 @@
     <col min="8" max="8" width="15.7109375" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" customWidth="1"/>
     <col min="10" max="10" width="45.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1025,8 +1119,11 @@
       <c r="J1" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1046,10 +1143,13 @@
         <v>73</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="K2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1063,17 +1163,20 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1094,13 +1197,16 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1121,13 +1227,16 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1148,13 +1257,16 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1175,13 +1287,16 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1192,7 +1307,7 @@
         <v>1993</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E8">
         <v>35.200000000000003</v>
@@ -1205,13 +1320,16 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J8" t="s">
         <v>85</v>
       </c>
-      <c r="J8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1222,7 +1340,7 @@
         <v>1993</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E9">
         <v>34.799999999999997</v>
@@ -1235,13 +1353,16 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" t="s">
         <v>85</v>
       </c>
-      <c r="J9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1252,7 +1373,7 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E10">
         <v>36</v>
@@ -1265,13 +1386,16 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
+        <v>84</v>
+      </c>
+      <c r="J10" t="s">
         <v>85</v>
       </c>
-      <c r="J10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K10" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1282,7 +1406,7 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E11">
         <v>31</v>
@@ -1295,13 +1419,16 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" t="s">
         <v>85</v>
       </c>
-      <c r="J11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -1312,7 +1439,7 @@
         <v>2000</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E12">
         <v>37</v>
@@ -1322,13 +1449,16 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
+        <v>86</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1339,7 +1469,7 @@
         <v>2000</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E13">
         <v>37</v>
@@ -1349,13 +1479,16 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
+        <v>86</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1366,7 +1499,7 @@
         <v>2003</v>
       </c>
       <c r="D14" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E14">
         <v>38.86</v>
@@ -1379,13 +1512,16 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -1396,7 +1532,7 @@
         <v>2003</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E15">
         <v>40.17</v>
@@ -1409,13 +1545,16 @@
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
+        <v>88</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -1426,7 +1565,7 @@
         <v>2009</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E16">
         <v>40.969000000000001</v>
@@ -1438,13 +1577,16 @@
         <v>2047.962</v>
       </c>
       <c r="I16" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1455,7 +1597,7 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E17">
         <v>39.03</v>
@@ -1467,13 +1609,16 @@
         <v>1901.21</v>
       </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>207</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="K17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1484,19 +1629,22 @@
         <v>2015</v>
       </c>
       <c r="D18" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>58</v>
       </c>
       <c r="I18" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="K18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1507,19 +1655,22 @@
         <v>2015</v>
       </c>
       <c r="D19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>59</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="K19" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1530,19 +1681,22 @@
         <v>2005</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="I20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K20" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -1553,19 +1707,22 @@
         <v>2005</v>
       </c>
       <c r="D21" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="I21" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -1576,217 +1733,244 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>70</v>
       </c>
       <c r="I22" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="K22" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="K23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C24">
         <v>1979</v>
       </c>
       <c r="D24" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" t="s">
         <v>113</v>
       </c>
-      <c r="I24" t="s">
-        <v>116</v>
-      </c>
       <c r="J24" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="K24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C25">
         <v>1986</v>
       </c>
       <c r="D25" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I25" t="s">
-        <v>116</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C26">
         <v>1992</v>
       </c>
       <c r="D26" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" t="s">
+        <v>113</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="K26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>115</v>
       </c>
-      <c r="I26" t="s">
+      <c r="B27" t="s">
         <v>116</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" t="s">
-        <v>119</v>
       </c>
       <c r="C27">
         <v>2013</v>
       </c>
       <c r="D27" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E27">
         <v>31.36</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27" t="s">
+        <v>118</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="K27" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>120</v>
       </c>
-      <c r="I27" t="s">
+      <c r="B28" t="s">
         <v>121</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" t="s">
-        <v>124</v>
       </c>
       <c r="C28">
         <v>2007</v>
       </c>
       <c r="D28" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E28">
         <v>29.768270000000001</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G28" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="I28" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K28" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B29" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B29" t="s">
-        <v>130</v>
       </c>
       <c r="C29">
         <v>2020</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I29" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="K29" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C30">
         <v>2020</v>
       </c>
       <c r="D30" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I30" t="s">
+        <v>131</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>134</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>137</v>
-      </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>227</v>
       </c>
       <c r="C31">
         <v>1990</v>
@@ -1798,21 +1982,24 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="K31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B32" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C32">
         <v>2001</v>
@@ -1824,300 +2011,333 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I32" t="s">
+        <v>139</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" t="s">
         <v>145</v>
-      </c>
-      <c r="I32" t="s">
-        <v>143</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>148</v>
-      </c>
-      <c r="B33" t="s">
-        <v>149</v>
       </c>
       <c r="C33">
         <v>1993</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E33">
         <v>42</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G33" s="1">
         <v>1934.5</v>
       </c>
       <c r="I33" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="K33" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B34" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E34">
         <v>44</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G34" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I34" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="K34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E35">
         <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G35" s="1">
         <v>1925.375</v>
       </c>
       <c r="I35" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="K35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C36">
         <v>2002</v>
       </c>
       <c r="D36" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E36">
         <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G36" s="1">
         <v>1999.866</v>
       </c>
       <c r="I36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="K36" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C37">
         <v>2006</v>
       </c>
       <c r="D37" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E37" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I37" t="s">
+        <v>159</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" t="s">
         <v>165</v>
-      </c>
-      <c r="I37" t="s">
-        <v>163</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>168</v>
-      </c>
-      <c r="B38" t="s">
-        <v>169</v>
       </c>
       <c r="C38">
         <v>2011</v>
       </c>
       <c r="D38" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E38">
         <v>36.92</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G38" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I38" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>167</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>171</v>
-      </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C39">
         <v>2006</v>
       </c>
       <c r="D39" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E39">
         <v>37.71</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G39" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I39" t="s">
+        <v>170</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="K39" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40" t="s">
         <v>174</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>182</v>
-      </c>
-      <c r="B40" t="s">
-        <v>178</v>
       </c>
       <c r="C40">
         <v>2004</v>
       </c>
       <c r="D40" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E40">
         <v>37.630000000000003</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G40">
         <v>2731</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="210" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="K40" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C41">
         <v>2001</v>
       </c>
       <c r="D41" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E41">
         <v>39.612000000000002</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G41" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="K41" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B42" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C42">
         <v>2009</v>
       </c>
       <c r="D42" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E42">
         <v>50.181100000000001</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G42" s="1">
         <v>1543.018</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
+      </c>
+      <c r="K42" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added expectedPensionLetter based on Dolls et al. (2019)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="234">
   <si>
     <t>program_identifier</t>
   </si>
@@ -707,6 +707,24 @@
   </si>
   <si>
     <t>Bafög Repayment Reform</t>
+  </si>
+  <si>
+    <t>expectedPensionLetter</t>
+  </si>
+  <si>
+    <t>Pension Information</t>
+  </si>
+  <si>
+    <t>Since 2005 the German pension administration sends out letters designed to inform about one's future expected future pension payments. These letters also highlight the link between social security contriubtions and the resulting pension entitlement. To receive such a letter, the recipient had to be at least 27 years old. This age cutoff  thus generated quasi-random variation which allows evaluating the resulting effect on earnings and retirement savings.</t>
+  </si>
+  <si>
+    <t>dolls2019</t>
+  </si>
+  <si>
+    <t>Dolls et al. (2019)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/pubeco/v171y2019icp105-116.html</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="F38" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2338,6 +2356,38 @@
       </c>
       <c r="K42" t="s">
         <v>226</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>228</v>
+      </c>
+      <c r="B43" t="s">
+        <v>229</v>
+      </c>
+      <c r="C43">
+        <v>2005</v>
+      </c>
+      <c r="D43" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43">
+        <v>27</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2004.07</v>
+      </c>
+      <c r="I43" t="s">
+        <v>232</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="K43" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2377,8 +2427,9 @@
     <hyperlink ref="J40" r:id="rId33"/>
     <hyperlink ref="J41" r:id="rId34"/>
     <hyperlink ref="J42" r:id="rId35"/>
+    <hyperlink ref="J43" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId36"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added decentralization of job centers based on Mergele & Weber (2020)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="240">
   <si>
     <t>program_identifier</t>
   </si>
@@ -725,6 +725,24 @@
   </si>
   <si>
     <t>https://ideas.repec.org/a/eee/pubeco/v171y2019icp105-116.html</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/pubeco/v182y2020ics0047272719301756.html</t>
+  </si>
+  <si>
+    <t>mergele2020</t>
+  </si>
+  <si>
+    <t>Mergeke &amp; Weber (2020)</t>
+  </si>
+  <si>
+    <t>decentralizedEmploymentServices</t>
+  </si>
+  <si>
+    <t>Decentralization of Employment Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2012 several job centers which where under the supervision of the federal emlpoyment agency were decentralized. 41 out of 407 German districts were put in charge of their local job centers. </t>
   </si>
 </sst>
 </file>
@@ -1085,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F38" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2388,6 +2406,38 @@
       </c>
       <c r="K43" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>237</v>
+      </c>
+      <c r="B44" t="s">
+        <v>238</v>
+      </c>
+      <c r="C44">
+        <v>2012</v>
+      </c>
+      <c r="D44" t="s">
+        <v>176</v>
+      </c>
+      <c r="E44">
+        <v>44.531999999999996</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="G44" s="1">
+        <v>994.59460000000001</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K44" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2428,8 +2478,9 @@
     <hyperlink ref="J41" r:id="rId34"/>
     <hyperlink ref="J42" r:id="rId35"/>
     <hyperlink ref="J43" r:id="rId36"/>
+    <hyperlink ref="J44" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId37"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EEG added based on Abrell et al. (2019)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="250">
   <si>
     <t>program_identifier</t>
   </si>
@@ -743,6 +743,36 @@
   </si>
   <si>
     <t xml:space="preserve">In 2012 several job centers which where under the supervision of the federal emlpoyment agency were decentralized. 41 out of 407 German districts were put in charge of their local job centers. </t>
+  </si>
+  <si>
+    <t>eegWind</t>
+  </si>
+  <si>
+    <t>EEG Wind Energy Subsidy</t>
+  </si>
+  <si>
+    <t>Climate Policy</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/pubeco/v169y2019icp172-202.html</t>
+  </si>
+  <si>
+    <t>abrell2019</t>
+  </si>
+  <si>
+    <t>Abrell et al. (2019)</t>
+  </si>
+  <si>
+    <t>eegSolar</t>
+  </si>
+  <si>
+    <t>In Germany electricity produced from renewable sources is subsidized under the the "Erneuerbare Energien Gesetz".  Abrell et al. (2019) estimate the implied carbon emission abatement cost of wind Energy.</t>
+  </si>
+  <si>
+    <t>In Germany electricity produced from renewable sources is subsidized under the the "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of solar Energy.</t>
+  </si>
+  <si>
+    <t>EEG Solar Energy Subsidy</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2438,6 +2468,58 @@
       </c>
       <c r="K44" t="s">
         <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>240</v>
+      </c>
+      <c r="B45" t="s">
+        <v>241</v>
+      </c>
+      <c r="C45">
+        <v>2012</v>
+      </c>
+      <c r="D45" t="s">
+        <v>242</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I45" t="s">
+        <v>245</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="K45" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>246</v>
+      </c>
+      <c r="B46" t="s">
+        <v>249</v>
+      </c>
+      <c r="C46">
+        <v>2012</v>
+      </c>
+      <c r="D46" t="s">
+        <v>242</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="I46" t="s">
+        <v>245</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="K46" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2479,8 +2561,10 @@
     <hyperlink ref="J42" r:id="rId35"/>
     <hyperlink ref="J43" r:id="rId36"/>
     <hyperlink ref="J44" r:id="rId37"/>
+    <hyperlink ref="J45" r:id="rId38"/>
+    <hyperlink ref="J46" r:id="rId39"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated MetaAssumptions. These should now be complete. Filenames might get a bit long. Maybe a hash function needs to be added.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -1135,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed incorrect spelling of et al.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="248">
   <si>
     <t>program_identifier</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Elementary School students were assigned mentors who should encourage the acquisition of new ideas and skills.</t>
-  </si>
-  <si>
-    <t>Top Tax Reform 1990</t>
   </si>
   <si>
     <t>Top Tax Reform 2000</t>
@@ -244,25 +241,16 @@
     <t>Atkinson &amp; Piketty (2010);Gottfried &amp; Schellhorn (2004)</t>
   </si>
   <si>
-    <t>Doerrenberg et. al. (2017);Clementi and Gallegati (2005)</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://ideas.repec.org/p/arx/papers/physics-0504217.html
 </t>
   </si>
   <si>
-    <t>Peter et. al. (2018)</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/p/diw/diwwpp/dp1770.html</t>
   </si>
   <si>
     <t>https://ideas.repec.org/p/ces/ceswps/_8382.html</t>
   </si>
   <si>
-    <t>Falk et. al. (2020)</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/a/uwp/jhriss/v54y2019i2p468-502.html</t>
   </si>
   <si>
@@ -275,15 +263,9 @@
     <t>Gorgen &amp; Schienle (2019);Bruckmeier &amp; Wigger (2014)</t>
   </si>
   <si>
-    <t>Lechner et. al. (2011)</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/a/bla/jeurec/v9y2011i4p742-784.html</t>
   </si>
   <si>
-    <t>Biewen et. al. (2014)</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/a/ucp/jlabec/doi10.1086-677233.html</t>
   </si>
   <si>
@@ -291,9 +273,6 @@
   </si>
   <si>
     <t>https://ideas.repec.org/a/eee/pubeco/v95y2011i3p311-331.html</t>
-  </si>
-  <si>
-    <t>Caliendo et. al. (2016)</t>
   </si>
   <si>
     <t>https://ideas.repec.org/a/eee/eecrev/v86y2016icp87-108.html</t>
@@ -646,9 +625,6 @@
     <t>doerr2014;huber2015</t>
   </si>
   <si>
-    <t>Doerr et. al. (2014);Huber et al. (2015)</t>
-  </si>
-  <si>
     <t>thiedig2018</t>
   </si>
   <si>
@@ -773,6 +749,24 @@
   </si>
   <si>
     <t>EEG Solar Energy Subsidy</t>
+  </si>
+  <si>
+    <t>Peter et al. (2018)</t>
+  </si>
+  <si>
+    <t>Falk et al. (2020)</t>
+  </si>
+  <si>
+    <t>Lechner et al. (2011)</t>
+  </si>
+  <si>
+    <t>Biewen et al. (2014)</t>
+  </si>
+  <si>
+    <t>Caliendo et al. (2016)</t>
+  </si>
+  <si>
+    <t>Doerr et al. (2014);Huber et al. (2015)</t>
   </si>
 </sst>
 </file>
@@ -1135,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,19 +1168,19 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1194,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1990</v>
@@ -1206,13 +1200,13 @@
         <v>10</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="K2" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1220,7 +1214,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>2000</v>
@@ -1229,17 +1223,15 @@
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
+      <c r="I3" s="1"/>
       <c r="J3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1253,7 +1245,7 @@
         <v>2013</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>19</v>
@@ -1263,13 +1255,13 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>242</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1283,7 +1275,7 @@
         <v>2011</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1293,1233 +1285,1233 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>79</v>
+        <v>243</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
       </c>
       <c r="C7">
         <v>2008</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
       <c r="C8">
         <v>1993</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E8">
         <v>35.200000000000003</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1">
         <v>1396</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>84</v>
+        <v>244</v>
       </c>
       <c r="J8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
       </c>
       <c r="C9">
         <v>1993</v>
       </c>
       <c r="D9" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E9">
         <v>34.799999999999997</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1">
         <v>1396</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>244</v>
       </c>
       <c r="J9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
       </c>
       <c r="C10">
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E10">
         <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="1">
         <v>1396</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>244</v>
       </c>
       <c r="J10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
       </c>
       <c r="C11">
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E11">
         <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1">
         <v>1396</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>84</v>
+        <v>244</v>
       </c>
       <c r="J11" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
       </c>
       <c r="C12">
         <v>2000</v>
       </c>
       <c r="D12" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E12">
         <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>86</v>
+        <v>245</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
       </c>
       <c r="C13">
         <v>2000</v>
       </c>
       <c r="D13" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E13">
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>86</v>
+        <v>245</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
       </c>
       <c r="C14">
         <v>2003</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E14">
         <v>38.86</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="1">
         <v>1459.3779999999999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K14" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
         <v>45</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
       </c>
       <c r="C15">
         <v>2003</v>
       </c>
       <c r="D15" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E15">
         <v>40.17</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="1">
         <v>2189.3620000000001</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="K15" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
         <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
       </c>
       <c r="C16">
         <v>2009</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E16">
         <v>40.969000000000001</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="1">
         <v>2047.962</v>
       </c>
       <c r="I16" t="s">
-        <v>90</v>
+        <v>246</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="K16" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
         <v>53</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
       </c>
       <c r="C17">
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E17">
         <v>39.03</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G17" s="1">
         <v>1901.21</v>
       </c>
       <c r="I17" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="K17" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
         <v>56</v>
-      </c>
-      <c r="B18" t="s">
-        <v>57</v>
       </c>
       <c r="C18">
         <v>2015</v>
       </c>
       <c r="D18" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K18" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19">
         <v>2015</v>
       </c>
       <c r="D19" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I19" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="K19" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20">
         <v>2005</v>
       </c>
       <c r="D20" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I20" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="K20" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21">
         <v>2005</v>
       </c>
       <c r="D21" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I21" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="K21" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
         <v>68</v>
-      </c>
-      <c r="B22" t="s">
-        <v>69</v>
       </c>
       <c r="C22">
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="K22" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="K23" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C24">
         <v>1979</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I24" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K24" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C25">
         <v>1986</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="I25" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K25" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C26">
         <v>1992</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="I26" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="K26" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C27">
         <v>2013</v>
       </c>
       <c r="D27" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E27">
         <v>31.36</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="I27" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="K27" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C28">
         <v>2007</v>
       </c>
       <c r="D28" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E28">
         <v>29.768270000000001</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G28" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="I28" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="K28" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C29">
         <v>2020</v>
       </c>
       <c r="D29" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="I29" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="K29" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C30">
         <v>2020</v>
       </c>
       <c r="D30" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="I30" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="K30" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C31">
         <v>1990</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E31">
         <v>19.809999999999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I31" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="K31" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B32" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C32">
         <v>2001</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E32">
         <v>19.420999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="I32" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="K32" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C33">
         <v>1993</v>
       </c>
       <c r="D33" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E33">
         <v>42</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="G33" s="1">
         <v>1934.5</v>
       </c>
       <c r="I33" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K33" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B34" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E34">
         <v>44</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="G34" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I34" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K34" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E35">
         <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="G35" s="1">
         <v>1925.375</v>
       </c>
       <c r="I35" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="K35" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C36">
         <v>2002</v>
       </c>
       <c r="D36" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E36">
         <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="G36" s="1">
         <v>1999.866</v>
       </c>
       <c r="I36" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="K36" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B37" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C37">
         <v>2006</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E37" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I37" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K37" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C38">
         <v>2011</v>
       </c>
       <c r="D38" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E38">
         <v>36.92</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="G38" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="K38" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C39">
         <v>2006</v>
       </c>
       <c r="D39" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E39">
         <v>37.71</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="G39" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I39" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="K39" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C40">
         <v>2004</v>
       </c>
       <c r="D40" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E40">
         <v>37.630000000000003</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G40">
         <v>2731</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="K40" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B41" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C41">
         <v>2001</v>
       </c>
       <c r="D41" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E41">
         <v>39.612000000000002</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G41" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K41" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B42" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C42">
         <v>2009</v>
       </c>
       <c r="D42" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E42">
         <v>50.181100000000001</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G42" s="1">
         <v>1543.018</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="K42" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B43" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="C43">
         <v>2005</v>
       </c>
       <c r="D43" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E43">
         <v>27</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G43" s="1">
         <v>2004.07</v>
       </c>
       <c r="I43" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K43" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B44" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C44">
         <v>2012</v>
       </c>
       <c r="D44" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E44">
         <v>44.531999999999996</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G44" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="K44" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B45" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="I45" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="K45" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B46" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="I46" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="K46" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated programs.xlsx - This includes: *fixed typos and other errors in descriptions *added some further income information
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="252">
   <si>
     <t>program_identifier</t>
   </si>
@@ -45,24 +45,15 @@
     <t>taxReform2000</t>
   </si>
   <si>
-    <t>Top Tax Reform</t>
-  </si>
-  <si>
     <t>short_description</t>
   </si>
   <si>
-    <t>In 1990 Germany reduced the top tax rate from 56% to 53%</t>
-  </si>
-  <si>
     <t>BestUpInformationWorkshop</t>
   </si>
   <si>
     <t>Best Up College Information Workshop</t>
   </si>
   <si>
-    <t>A group of researchers  studied the effect of providing information about the benefits of college education to high school students one year prior to graduation.</t>
-  </si>
-  <si>
     <t>mentoringBalu</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
   </si>
   <si>
     <t>Short Training</t>
-  </si>
-  <si>
-    <t>Government sponsored Training Program lasting less less then 6 months</t>
   </si>
   <si>
     <t>practiceFirm</t>
@@ -136,9 +124,6 @@
     <t>Class Room Training</t>
   </si>
   <si>
-    <t>Government sponsored short-term training programs "Trainingsmaßnahmen", which where introduced again in 1998 after being abolished in 1993</t>
-  </si>
-  <si>
     <t>Government sponsored training that lasts on average 7.5 months.</t>
   </si>
   <si>
@@ -163,21 +148,12 @@
     <t>average_earnings_beneficiary</t>
   </si>
   <si>
-    <t>The bridging allowance "Überbrückungsgeld" was a subsidy equal to the potential unemployment benefit payed to start up founders who would otherwise have been eligible for unemployment benefits. The briding allowance was payed for 6 months.</t>
-  </si>
-  <si>
-    <t>The start up subsidy "Existenzgründungszuschuss" was a subsidy that was payed for 3 years to start up founders who received unemployment benefits before entering self-employment.</t>
-  </si>
-  <si>
     <t>startupGrant</t>
   </si>
   <si>
     <t>Start Up Grant</t>
   </si>
   <si>
-    <t>The start up Grant is the follow up program to the  bridging allowance "Überbrückungsgeld" and start up subsidy "Existenzgründungszuschuss" which were replaced in 2006. This subsidy pays the individual unemloyment benefit for 6 months and an additional 300 euros for up to 15 months.</t>
-  </si>
-  <si>
     <t>trainingVoucher</t>
   </si>
   <si>
@@ -214,22 +190,13 @@
     <t>jobCreationSchemes</t>
   </si>
   <si>
-    <t>One Euro Jobs "Ein Euro Jobs" are jobs which are assigned to long term unemployed to help them reintegrate into the labor market. These jobs are meant to be unpayed. However, the participants receive a compenstation of at leat one euro per hour worked.</t>
-  </si>
-  <si>
     <t>One Euro Jobs</t>
   </si>
   <si>
-    <t>Job Creation Schemes "Arbeitsbeschaffungsmaßnahmen" are comprised of subsizied jobs aimed at  unemployed who would not be able to find a job otherwise. This measure is mostly employed in local labor markets with excess labor supply. The duration of the subsidy (between 900 and 1300€ payed to the employer) is usually limited to 12 months.</t>
-  </si>
-  <si>
     <t>subsidizedJobOpportunities</t>
   </si>
   <si>
     <t>Subsidized Job Opportunities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Similar to  Job Creation Schemes, Subsidized Job Opportunities "Arbeitsgelegenheiten" are jobs where the employer receives a subsidy. The focus of subsidized job opportunities lies on reintegration. The amount of subsidy payed to the employer is not fixed and the types of jobs that can be subsizied  is more broad. </t>
   </si>
   <si>
     <t>Links</t>
@@ -290,12 +257,6 @@
     <t>https://ideas.repec.org/p/iab/iabdpa/201021.html</t>
   </si>
   <si>
-    <t>Between 2001 and 2005 Germany reduced the top tax rate from 53% to 42%</t>
-  </si>
-  <si>
-    <t>Traffic Regulation</t>
-  </si>
-  <si>
     <t>Sieg (2014);Elvik (2013)</t>
   </si>
   <si>
@@ -333,9 +294,6 @@
     <t>Maternity Leave Reform 1992</t>
   </si>
   <si>
-    <t>In 1979, the maternity leave coverage was extended  from 2 to 6 months. During these 6 months all entitled mothers received a maternal leave benefit of 750 Deutschmarks per month.</t>
-  </si>
-  <si>
     <t>The 1986 maternity leave reform extended the period during which mothers had the right to return to their previous job and received maternity benefits from 6 to 10 months. At the same, the maternity benefit was reduced from 750 Deutschmarks to 600 Deutschmarks.</t>
   </si>
   <si>
@@ -354,9 +312,6 @@
     <t>Home Care Subsidy</t>
   </si>
   <si>
-    <t>The home care subsidy "Betreuungsgeld" was introduced in 2013 and was meant to compensate parents who did not make use of subsidised childcare.</t>
-  </si>
-  <si>
     <t>Collischon et al. (2020)</t>
   </si>
   <si>
@@ -369,9 +324,6 @@
     <t>Parental Leave Reform 2007</t>
   </si>
   <si>
-    <t>In 2007, "Elterngeld" was introduced which replaced the fromer parental leave benefit "Erziehungsgeld". Under the new system, the amount of benefit is determined by the net income of the parent who is taking parental leave. For most parents the total benefit payment is higher even though the subsidy is payed for 12 months instead of previously 24 months.</t>
-  </si>
-  <si>
     <t>Frodermann et al. (2020);Kluve &amp; Tamm (2013)</t>
   </si>
   <si>
@@ -390,9 +342,6 @@
     <t>Coronavirus Lockdown R=0.6 vs R = 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a hypothetical no lockdown scenario which would have left the GDP unchanged and resulted in 560000 deaths.  </t>
-  </si>
-  <si>
     <t>Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a too lash lockdown which would maintained R=1.</t>
   </si>
   <si>
@@ -423,18 +372,12 @@
     <t>Baumgartner &amp; Steiner (2006)</t>
   </si>
   <si>
-    <t>Bafög is a means-tested public German student loan program. Until 1990 students had to repay the entire loan. After the reform about 50% of the loan was offered as a grant which does not have to be payed back.</t>
-  </si>
-  <si>
     <t>Bafög is a means-tested public German student loan program. Eligible students only have to pay back about 50% of the loan. In 1990, the threshold of parents' income above which students are no longer eligible for Bafög was lowered.</t>
   </si>
   <si>
     <t>https://ideas.repec.org/a/oup/qjecon/v127y2012i2p701-752.html;https://ideas.repec.org/a/anr/reveco/v8y2016p547-581.html</t>
   </si>
   <si>
-    <t>A discountinuity at the age of 42 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 42 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
-  </si>
-  <si>
     <t>unemploymentBenefits42</t>
   </si>
   <si>
@@ -447,15 +390,9 @@
     <t>Unemployment Benefits Age 44</t>
   </si>
   <si>
-    <t>A discountinuity at the age of 44 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 44 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
-  </si>
-  <si>
     <t>Unemployment Benefits Age 49</t>
   </si>
   <si>
-    <t>A discountinuity at the age of 49 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 49 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
-  </si>
-  <si>
     <t>unemploymentBenefits44</t>
   </si>
   <si>
@@ -468,9 +405,6 @@
     <t>Unemployment Benefits Age 45</t>
   </si>
   <si>
-    <t>A discountinuity at the age of 45 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 45 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/a/wly/japmet/v28y2013i4p604-627.html;https://ideas.repec.org/a/anr/reveco/v8y2016p547-581.html</t>
   </si>
   <si>
@@ -510,9 +444,6 @@
     <t>Relocation Assistance</t>
   </si>
   <si>
-    <t>Unemployed who cannot find a new job locally are eligible for relocation assistence which either covers the immediate costs of moving or subsidizes a secondary flat for up to six months.</t>
-  </si>
-  <si>
     <t>Caliendo et al. (2011)</t>
   </si>
   <si>
@@ -550,9 +481,6 @@
   </si>
   <si>
     <t>Spermann &amp; Strotmann (2006)</t>
-  </si>
-  <si>
-    <t>Spermann &amp; Strotmann (2006) evaluate the effects of what they call a negative income tax experiment. This is misleading because the experiment they are describing does not resemble what is typically considered a negative income tax as proposed by Milton Friedman. In the sense of Friedman, a negative income tax is a basic income that is gradually phased-out with increasing gross earnings. Instead, Spermann &amp; Strotmann (2006) consider a experiment where long-term unemployed receive a  subsidy on top of their gross wage. The subsidy increases with the wage and can reach a maximum of up to 643 Deutschmark.</t>
   </si>
   <si>
     <t>Tax Reform</t>
@@ -691,9 +619,6 @@
     <t>Pension Information</t>
   </si>
   <si>
-    <t>Since 2005 the German pension administration sends out letters designed to inform about one's future expected future pension payments. These letters also highlight the link between social security contriubtions and the resulting pension entitlement. To receive such a letter, the recipient had to be at least 27 years old. This age cutoff  thus generated quasi-random variation which allows evaluating the resulting effect on earnings and retirement savings.</t>
-  </si>
-  <si>
     <t>dolls2019</t>
   </si>
   <si>
@@ -718,9 +643,6 @@
     <t>Decentralization of Employment Services</t>
   </si>
   <si>
-    <t xml:space="preserve">In 2012 several job centers which where under the supervision of the federal emlpoyment agency were decentralized. 41 out of 407 German districts were put in charge of their local job centers. </t>
-  </si>
-  <si>
     <t>eegWind</t>
   </si>
   <si>
@@ -742,12 +664,6 @@
     <t>eegSolar</t>
   </si>
   <si>
-    <t>In Germany electricity produced from renewable sources is subsidized under the the "Erneuerbare Energien Gesetz".  Abrell et al. (2019) estimate the implied carbon emission abatement cost of wind Energy.</t>
-  </si>
-  <si>
-    <t>In Germany electricity produced from renewable sources is subsidized under the the "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of solar Energy.</t>
-  </si>
-  <si>
     <t>EEG Solar Energy Subsidy</t>
   </si>
   <si>
@@ -767,6 +683,102 @@
   </si>
   <si>
     <t>Doerr et al. (2014);Huber et al. (2015)</t>
+  </si>
+  <si>
+    <t>In 1990 Germany reduced the top income tax rate from 56% to 53%</t>
+  </si>
+  <si>
+    <t>Between 2001 and 2005 Germany reduced the top income tax rate from 53% to 42%</t>
+  </si>
+  <si>
+    <t>Government sponsored Training Program lasting less then 6 months</t>
+  </si>
+  <si>
+    <t>Government sponsored short-term training programs "Trainingsmaßnahmen", which were introduced again in 1998 after being abolished in 1993</t>
+  </si>
+  <si>
+    <t>A group of researchers studied the effect of providing information about the benefits of college education to high school students one year prior to graduation.</t>
+  </si>
+  <si>
+    <t>The startup Grant is the follow up program to the bridging allowance "Überbrückungsgeld" and startup subsidy "Existenzgründungszuschuss" which were replaced in 2006. This subsidy pays the individual unemloyment benefit for 6 months and an additional 300 euros for up to 15 months.</t>
+  </si>
+  <si>
+    <t>In 1979, the maternity leave coverage was extended from 2 to 6 months. During these 6 months all entitled mothers received a maternal leave benefit of 750 Deutschmarks per month.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a hypothetical no lockdown scenario which would have left the GDP unchanged and resulted in 560000 deaths. </t>
+  </si>
+  <si>
+    <t>One Euro Jobs "Ein Euro Jobs" are jobs which are assigned to long term unemployed to help them reintegrate into the labor market. These jobs are meant to be unpaid. However, the participants receive a compensation of at least one euro per hour worked.</t>
+  </si>
+  <si>
+    <t>The home care subsidy "Betreuungsgeld" was introduced in 2013 and was meant to compensate parents who did not make use of subsidized childcare.</t>
+  </si>
+  <si>
+    <t>The startup subsidy "Existenzgründungszuschuss" was a subsidy that was paid for 3 years to start up founders who received unemployment benefits before entering self-employment.</t>
+  </si>
+  <si>
+    <t>The bridging allowance "Überbrückungsgeld" was a subsidy equal to the potential unemployment benefit paid to start up founders who would otherwise have been eligible for unemployment benefits. The bridging allowance was paid for 6 months.</t>
+  </si>
+  <si>
+    <t>Job Creation Schemes "Arbeitsbeschaffungsmaßnahmen" are comprised of subsidized jobs aimed at unemployed who would not be able to find a job otherwise. This measure is mostly employed in local labor markets with excess labor supply. The duration of the subsidy (between 900 and 1300€ paid to the employer) is usually limited to 12 months.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar to Job Creation Schemes, Subsidized Job Opportunities "Arbeitsgelegenheiten" are jobs where the employer receives a subsidy. The focus of subsidized job opportunities lies on reintegration. The amount of subsidy paid to the employer is not fixed and the types of jobs that can be subsidized is more broad. </t>
+  </si>
+  <si>
+    <t>In 2007, "Elterngeld" was introduced which replaced the former parental leave benefit "Erziehungsgeld". Under the new system, the amount of benefit is determined by the net income of the parent who is taking parental leave. For most parents the total benefit payment is higher even though the subsidy is paid for 12 months instead of previously 24 months.</t>
+  </si>
+  <si>
+    <t>Bafög is a means-tested public German student loan program. Until 1990 students had to repay the entire loan. After the reform about 50% of the loan was offered as a grant which does not have to be paid back.</t>
+  </si>
+  <si>
+    <t>A discontinuity at the age of 42 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 42 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>A discontinuity at the age of 44 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 44 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>A discontinuity at the age of 49 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 49 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>A discontinuity at the age of 45 in the German federal unemployment insurance system can be exploited to estimate the efficiency costs associated with expanding unemployment insurance for 45 year olds in Germany. Together with results from the theoretical literature on unemployment benefits, it is possible to calculate the implied MVPF.</t>
+  </si>
+  <si>
+    <t>Unemployed who cannot find a new job locally are eligible for relocation assistance which either covers the immediate costs of moving or subsidizes a secondary flat for up to six months.</t>
+  </si>
+  <si>
+    <t>Spermann &amp; Strotmann (2006) evaluate the effects of what they call a negative income tax experiment. This is a bit misleading because the experiment they are describing does not resemble what is typically considered a negative income tax as proposed by Milton Friedman. In the sense of Friedman, a negative income tax is a basic income that is gradually phased-out with increasing gross earnings. Instead, Spermann &amp; Strotmann (2006) consider an experiment where long-term unemployed receive a subsidy on top of their gross wage. The subsidy increases with the wage and can reach a maximum of up to 643 Deutschmark.</t>
+  </si>
+  <si>
+    <t>Since 2005 the German pension administration sends out letters designed to inform about one's future expected future pension payments. These letters also highlight the link between social security contributions and the resulting pension entitlement. To receive such a letter, the recipient had to be at least 27 years old. This age cutoff thus generated quasi-random variation which allows evaluating the resulting effect on earnings and retirement savings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In 2012 several job centers which where under the supervision of the federal employment agency were decentralized. 41 out of 407 German districts were put in charge of their local job centers. </t>
+  </si>
+  <si>
+    <t>In Germany electricity produced from renewable sources is subsidized under the "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of wind Energy.</t>
+  </si>
+  <si>
+    <t>In Germany electricity produced from renewable sources is subsidized under the "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of solar Energy.</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Average earnings calculated from Destatis Fachserie 14 Reihe 7.1 Year 2001, Table 4.4</t>
+  </si>
+  <si>
+    <t>Calculated from Destatis "Lohn- und Einkommensteuerstatistik 1995" Table 4.1.3 assuming that top tax affected incomes above  160000DM. And then deflated to 1990.</t>
+  </si>
+  <si>
+    <t>Average age is the average age of the german poluation according to CIA World Fact Book 2018. Average Earnings is Gross National Income in 2012 (From Destatis) divided by 80 Million</t>
+  </si>
+  <si>
+    <t>Average age is the average age of the german poluation according to CIA World Fact Book 2018. Average Earnings is Gross National Income in 2012 (From Destatis) divided by 80 Million.</t>
+  </si>
+  <si>
+    <t>maybe insert average age of mothers. This should be available somewhere</t>
   </si>
 </sst>
 </file>
@@ -1129,8 +1141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1154,7 @@
     <col min="5" max="5" width="66.85546875" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" customWidth="1"/>
     <col min="10" max="10" width="45.140625" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" customWidth="1"/>
@@ -1165,25 +1177,25 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1194,1324 +1206,1364 @@
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>220</v>
+      </c>
+      <c r="G2" s="1">
+        <v>8868.6350000000002</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="K2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>2000</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>153</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="1"/>
+        <v>221</v>
+      </c>
+      <c r="G3" s="1">
+        <v>9056.3310000000001</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2013</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>224</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>2011</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6">
         <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>2008</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>1993</v>
       </c>
       <c r="D8" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E8">
         <v>35.200000000000003</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G8" s="1">
         <v>1396</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="J8" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9">
         <v>1993</v>
       </c>
       <c r="D9" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E9">
         <v>34.799999999999997</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>29</v>
+        <v>222</v>
       </c>
       <c r="G9" s="1">
         <v>1396</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="J9" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10">
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E10">
         <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1">
         <v>1396</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="J10" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E11">
         <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G11" s="1">
         <v>1396</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="J11" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>2000</v>
       </c>
       <c r="D12" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E12">
         <v>37</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C13">
         <v>2000</v>
       </c>
       <c r="D13" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E13">
         <v>37</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>223</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>2003</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E14">
         <v>38.86</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>48</v>
+        <v>230</v>
       </c>
       <c r="G14" s="1">
         <v>1459.3779999999999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K14" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>2003</v>
       </c>
       <c r="D15" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E15">
         <v>40.17</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>47</v>
+        <v>231</v>
       </c>
       <c r="G15" s="1">
         <v>2189.3620000000001</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K15" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>2009</v>
       </c>
       <c r="D16" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E16">
         <v>40.969000000000001</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
+        <v>225</v>
       </c>
       <c r="G16" s="1">
         <v>2047.962</v>
       </c>
       <c r="I16" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="K16" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C17">
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E17">
         <v>39.03</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G17" s="1">
         <v>1901.21</v>
       </c>
       <c r="I17" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="K17" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C18">
         <v>2015</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>208</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I18" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K18" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C19">
         <v>2015</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>208</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I19" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="K19" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C20">
         <v>2005</v>
       </c>
       <c r="D20" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="I20" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="K20" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C21">
         <v>2005</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>64</v>
+        <v>228</v>
       </c>
       <c r="I21" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="K21" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C22">
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>69</v>
+        <v>233</v>
       </c>
       <c r="I22" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="K22" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C23">
         <v>2012</v>
       </c>
       <c r="D23" t="s">
-        <v>90</v>
+        <v>246</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="I23" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="K23" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C24">
         <v>1979</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>103</v>
+        <v>226</v>
+      </c>
+      <c r="H24" t="s">
+        <v>251</v>
       </c>
       <c r="I24" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K24" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C25">
         <v>1986</v>
       </c>
       <c r="D25" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
+      </c>
+      <c r="H25" t="s">
+        <v>251</v>
       </c>
       <c r="I25" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K25" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C26">
         <v>1992</v>
       </c>
       <c r="D26" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
+      </c>
+      <c r="H26" t="s">
+        <v>251</v>
       </c>
       <c r="I26" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K26" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C27">
         <v>2013</v>
       </c>
       <c r="D27" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="E27">
         <v>31.36</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>110</v>
+        <v>229</v>
       </c>
       <c r="I27" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="K27" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C28">
         <v>2007</v>
       </c>
       <c r="D28" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
       <c r="E28">
         <v>29.768270000000001</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>115</v>
+        <v>234</v>
       </c>
       <c r="G28" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="I28" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="K28" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C29">
         <v>2020</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="I29" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="K29" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C30">
         <v>2020</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="I30" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="K30" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B31" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="C31">
         <v>1990</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E31">
         <v>19.809999999999999</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>133</v>
+        <v>235</v>
       </c>
       <c r="I31" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="K31" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="B32" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="C32">
         <v>2001</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E32">
         <v>19.420999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="I32" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="K32" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="C33">
         <v>1993</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="E33">
         <v>42</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>136</v>
+        <v>236</v>
       </c>
       <c r="G33" s="1">
         <v>1934.5</v>
       </c>
       <c r="I33" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="K33" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="E34">
         <v>44</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>141</v>
+        <v>237</v>
       </c>
       <c r="G34" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I34" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="K34" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="E35">
         <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>143</v>
+        <v>238</v>
       </c>
       <c r="G35" s="1">
         <v>1925.375</v>
       </c>
       <c r="I35" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="K35" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="C36">
         <v>2002</v>
       </c>
       <c r="D36" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="E36">
         <v>45</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>148</v>
+        <v>239</v>
       </c>
       <c r="G36" s="1">
         <v>1999.866</v>
       </c>
       <c r="I36" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="K36" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="B37" t="s">
-        <v>151</v>
+        <v>129</v>
       </c>
       <c r="C37">
         <v>2006</v>
       </c>
       <c r="D37" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="E37" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="I37" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="K37" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>157</v>
+        <v>135</v>
       </c>
       <c r="B38" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="C38">
         <v>2011</v>
       </c>
       <c r="D38" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E38">
         <v>36.92</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="G38" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="K38" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="C39">
         <v>2006</v>
       </c>
       <c r="D39" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E39">
         <v>37.71</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>162</v>
+        <v>240</v>
       </c>
       <c r="G39" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I39" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="K39" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="B40" t="s">
-        <v>167</v>
+        <v>144</v>
       </c>
       <c r="C40">
         <v>2004</v>
       </c>
       <c r="D40" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E40">
         <v>37.630000000000003</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="G40">
         <v>2731</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>165</v>
+        <v>142</v>
       </c>
       <c r="K40" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="B41" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
       <c r="C41">
         <v>2001</v>
       </c>
       <c r="D41" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="E41">
         <v>39.612000000000002</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="G41" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="K41" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="B42" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="C42">
         <v>2009</v>
       </c>
       <c r="D42" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E42">
         <v>50.181100000000001</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>181</v>
+        <v>157</v>
       </c>
       <c r="G42" s="1">
         <v>1543.018</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
       <c r="K42" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="B43" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="C43">
         <v>2005</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>246</v>
       </c>
       <c r="E43">
         <v>27</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>222</v>
+        <v>242</v>
       </c>
       <c r="G43" s="1">
         <v>2004.07</v>
       </c>
       <c r="I43" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>225</v>
+        <v>200</v>
       </c>
       <c r="K43" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>229</v>
+        <v>204</v>
       </c>
       <c r="B44" t="s">
-        <v>230</v>
+        <v>205</v>
       </c>
       <c r="C44">
         <v>2012</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="E44">
         <v>44.531999999999996</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="G44" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>228</v>
+        <v>203</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>226</v>
+        <v>201</v>
       </c>
       <c r="K44" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>232</v>
+        <v>206</v>
       </c>
       <c r="B45" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>234</v>
+        <v>208</v>
+      </c>
+      <c r="E45">
+        <v>47.1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>239</v>
+        <v>244</v>
+      </c>
+      <c r="G45" s="1">
+        <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
+        <v>2928.3125</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>250</v>
       </c>
       <c r="I45" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="K45" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="B46" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>234</v>
+        <v>208</v>
+      </c>
+      <c r="E46">
+        <v>47.1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
+      </c>
+      <c r="G46" s="1">
+        <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
+        <v>2928.3125</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="I46" t="s">
-        <v>237</v>
+        <v>211</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>235</v>
+        <v>209</v>
       </c>
       <c r="K46" t="s">
-        <v>236</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated programs.xlsx and fixed the copy command.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="263">
   <si>
     <t>program_identifier</t>
   </si>
@@ -809,6 +809,9 @@
   </si>
   <si>
     <t>https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/</t>
+  </si>
+  <si>
+    <t>Top Tax Reform 1990</t>
   </si>
 </sst>
 </file>
@@ -1171,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>262</v>
       </c>
       <c r="C2">
         <v>1990</v>

</xml_diff>

<commit_message>
removed coronavirus R=0.6 vs unrestricted, as this too unrealistic.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="257">
   <si>
     <t>program_identifier</t>
   </si>
@@ -320,15 +320,9 @@
     <t>https://ideas.repec.org/p/iza/izadps/dp12935.html;https://ideas.repec.org/a/spr/jopoec/v26y2013i3p983-1005.html</t>
   </si>
   <si>
-    <t>coronavirusLockdown</t>
-  </si>
-  <si>
     <t>coronavirusLockdownR1</t>
   </si>
   <si>
-    <t>Coronavirus Lockdown R=0.6</t>
-  </si>
-  <si>
     <t>Coronavirus Lockdown R=0.6 vs R = 1</t>
   </si>
   <si>
@@ -341,9 +335,6 @@
     <t>https://ideas.repec.org/a/ces/ifosdd/06.html</t>
   </si>
   <si>
-    <t>https://ideas.repec.org/a/ces/ifosdd/06.html;https://academic.microsoft.com/paper/3032971139</t>
-  </si>
-  <si>
     <t>bafoegRepayment</t>
   </si>
   <si>
@@ -495,9 +486,6 @@
   </si>
   <si>
     <t>Bafög Reform 2001</t>
-  </si>
-  <si>
-    <t>Dorn et. al (2020);Flaxman et al. (2020)</t>
   </si>
   <si>
     <t xml:space="preserve">https://ideas.repec.org/b/oxp/obooks/9780199286898.html;https://ideas.repec.org/p/iaw/iawdip/15.html
@@ -555,9 +543,6 @@
     <t>kluve2013;frodermann2020</t>
   </si>
   <si>
-    <t>dorn2020;flaxman2020</t>
-  </si>
-  <si>
     <t>dorn2020</t>
   </si>
   <si>
@@ -688,9 +673,6 @@
   </si>
   <si>
     <t>In 1979, the maternity leave coverage was extended from 2 to 6 months. During these 6 months all entitled mothers received a maternal leave benefit of 750 Deutschmarks per month.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a hypothetical no lockdown scenario which would have left the GDP unchanged and resulted in 560000 deaths. </t>
   </si>
   <si>
     <t>One Euro Jobs "Ein Euro Jobs" are jobs which are assigned to long term unemployed to help them reintegrate into the labor market. These jobs are meant to be unpaid. However, the participants receive a compensation of at least one euro per hour worked.</t>
@@ -1174,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,7 +1207,7 @@
         <v>57</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1233,127 +1215,127 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>59</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="K2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B4" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="J5" s="3" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1373,17 +1355,17 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1407,13 +1389,13 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>61</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1443,7 +1425,7 @@
         <v>62</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1473,7 +1455,7 @@
         <v>64</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1487,7 +1469,7 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
@@ -1500,13 +1482,13 @@
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J10" t="s">
         <v>66</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1520,26 +1502,26 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="G11" s="1">
         <v>1396</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J11" t="s">
         <v>66</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1553,7 +1535,7 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E12">
         <v>36</v>
@@ -1566,13 +1548,13 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J12" t="s">
         <v>66</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1586,7 +1568,7 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E13">
         <v>31</v>
@@ -1599,13 +1581,13 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="J13" t="s">
         <v>66</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1619,7 +1601,7 @@
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E14">
         <v>37</v>
@@ -1629,13 +1611,13 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>67</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1649,23 +1631,23 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>67</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1679,13 +1661,13 @@
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
@@ -1698,7 +1680,7 @@
         <v>69</v>
       </c>
       <c r="K16" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1712,13 +1694,13 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
@@ -1731,7 +1713,7 @@
         <v>69</v>
       </c>
       <c r="K17" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1745,25 +1727,25 @@
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
       </c>
       <c r="I18" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>70</v>
       </c>
       <c r="K18" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1777,7 +1759,7 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E19">
         <v>39.03</v>
@@ -1789,13 +1771,13 @@
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="K19" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1809,7 +1791,7 @@
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>47</v>
@@ -1821,7 +1803,7 @@
         <v>71</v>
       </c>
       <c r="K20" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1835,7 +1817,7 @@
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>48</v>
@@ -1847,7 +1829,7 @@
         <v>71</v>
       </c>
       <c r="K21" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -1861,10 +1843,10 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="I22" t="s">
         <v>73</v>
@@ -1873,7 +1855,7 @@
         <v>74</v>
       </c>
       <c r="K22" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1887,10 +1869,10 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="I23" t="s">
         <v>73</v>
@@ -1899,7 +1881,7 @@
         <v>74</v>
       </c>
       <c r="K23" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1913,10 +1895,10 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I24" t="s">
         <v>73</v>
@@ -1925,7 +1907,7 @@
         <v>74</v>
       </c>
       <c r="K24" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1939,7 +1921,7 @@
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>79</v>
@@ -1951,7 +1933,7 @@
         <v>76</v>
       </c>
       <c r="K25" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1965,13 +1947,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H26" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I26" t="s">
         <v>89</v>
@@ -1980,7 +1962,7 @@
         <v>90</v>
       </c>
       <c r="K26" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1994,13 +1976,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H27" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I27" t="s">
         <v>89</v>
@@ -2009,7 +1991,7 @@
         <v>90</v>
       </c>
       <c r="K27" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2023,13 +2005,13 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>88</v>
       </c>
       <c r="H28" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="I28" t="s">
         <v>89</v>
@@ -2038,7 +2020,7 @@
         <v>90</v>
       </c>
       <c r="K28" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2052,13 +2034,13 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="I29" t="s">
         <v>93</v>
@@ -2067,7 +2049,7 @@
         <v>94</v>
       </c>
       <c r="K29" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2081,13 +2063,13 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
@@ -2099,15 +2081,15 @@
         <v>98</v>
       </c>
       <c r="K30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2116,42 +2098,45 @@
         <v>83</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>222</v>
+        <v>101</v>
       </c>
       <c r="I31" t="s">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="J31" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="K31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32">
+        <v>1990</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I32" t="s">
         <v>106</v>
-      </c>
-      <c r="K31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32">
-        <v>2020</v>
-      </c>
-      <c r="D32" t="s">
-        <v>83</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="I32" t="s">
-        <v>104</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>105</v>
       </c>
       <c r="K32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2159,19 +2144,19 @@
         <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="C33">
-        <v>1990</v>
+        <v>2001</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
       </c>
       <c r="E33">
-        <v>19.809999999999999</v>
+        <v>19.420999999999999</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="I33" t="s">
         <v>109</v>
@@ -2180,193 +2165,196 @@
         <v>108</v>
       </c>
       <c r="K33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B34" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="C34">
-        <v>2001</v>
+        <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>141</v>
       </c>
       <c r="E34">
-        <v>19.420999999999999</v>
+        <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>113</v>
+        <v>225</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1934.5</v>
       </c>
       <c r="I34" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>111</v>
       </c>
       <c r="K34" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" t="s">
         <v>115</v>
-      </c>
-      <c r="B35" t="s">
-        <v>116</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E35">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G35" s="1">
-        <v>1934.5</v>
+        <v>1928.4169999999999</v>
       </c>
       <c r="I35" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K35" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C36">
         <v>1993</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E36">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G36" s="1">
-        <v>1928.4169999999999</v>
+        <v>1925.375</v>
       </c>
       <c r="I36" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K36" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>119</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37">
+        <v>2002</v>
+      </c>
+      <c r="D37" t="s">
+        <v>141</v>
+      </c>
+      <c r="E37">
+        <v>45</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1999.866</v>
+      </c>
+      <c r="I37" t="s">
+        <v>122</v>
+      </c>
+      <c r="J37" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B37" t="s">
-        <v>119</v>
-      </c>
-      <c r="C37">
-        <v>1993</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="K37" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>144</v>
-      </c>
-      <c r="E37">
-        <v>42</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="G37" s="1">
-        <v>1925.375</v>
-      </c>
-      <c r="I37" t="s">
-        <v>117</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K37" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>122</v>
       </c>
       <c r="B38" t="s">
         <v>123</v>
       </c>
       <c r="C38">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="D38" t="s">
-        <v>144</v>
-      </c>
-      <c r="E38">
-        <v>45</v>
+        <v>141</v>
+      </c>
+      <c r="E38" s="1">
+        <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1999.866</v>
+        <v>126</v>
       </c>
       <c r="I38" t="s">
+        <v>124</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="K38" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B39" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C39">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
-      </c>
-      <c r="E39" s="1">
-        <v>50.492400000000004</v>
+        <v>140</v>
+      </c>
+      <c r="E39">
+        <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="I39" t="s">
+        <v>131</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1593.2249999999999</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="K39" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2377,292 +2365,296 @@
         <v>133</v>
       </c>
       <c r="C40">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E40">
-        <v>36.92</v>
+        <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2624.9580000000001</v>
+      </c>
+      <c r="I40" t="s">
         <v>134</v>
       </c>
-      <c r="G40" s="1">
-        <v>1593.2249999999999</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="J40" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="K40" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41">
+        <v>2004</v>
+      </c>
+      <c r="D41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41">
+        <v>37.630000000000003</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G41">
+        <v>2731</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="J41" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C41">
-        <v>2006</v>
-      </c>
-      <c r="D41" t="s">
-        <v>143</v>
-      </c>
-      <c r="E41">
-        <v>37.71</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="G41" s="1">
-        <v>2624.9580000000001</v>
-      </c>
-      <c r="I41" t="s">
-        <v>137</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="K41" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42">
+        <v>2001</v>
+      </c>
+      <c r="D42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42">
+        <v>39.612000000000002</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G42" s="1">
+        <v>1278.2249999999999</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B42" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42">
-        <v>2004</v>
-      </c>
-      <c r="D42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42">
-        <v>37.630000000000003</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G42">
-        <v>2731</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="K42" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B43" t="s">
         <v>152</v>
       </c>
       <c r="C43">
-        <v>2001</v>
+        <v>2009</v>
       </c>
       <c r="D43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43">
+        <v>50.181100000000001</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1543.018</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="J43" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E43">
-        <v>39.612000000000002</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="G43" s="1">
-        <v>1278.2249999999999</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="K43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>156</v>
+        <v>187</v>
       </c>
       <c r="B44" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
       <c r="C44">
-        <v>2009</v>
+        <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>235</v>
       </c>
       <c r="E44">
-        <v>50.181100000000001</v>
+        <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>154</v>
+        <v>231</v>
       </c>
       <c r="G44" s="1">
-        <v>1543.018</v>
-      </c>
-      <c r="I44" s="4" t="s">
+        <v>2004.07</v>
+      </c>
+      <c r="I44" t="s">
+        <v>190</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="K44" t="s">
         <v>189</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="K44" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B45" t="s">
+        <v>196</v>
+      </c>
+      <c r="C45">
+        <v>2012</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45">
+        <v>44.531999999999996</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="G45" s="1">
+        <v>994.59460000000001</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J45" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B45" t="s">
+      <c r="K45" t="s">
         <v>193</v>
       </c>
-      <c r="C45">
-        <v>2005</v>
-      </c>
-      <c r="D45" t="s">
-        <v>241</v>
-      </c>
-      <c r="E45">
-        <v>27</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G45" s="1">
-        <v>2004.07</v>
-      </c>
-      <c r="I45" t="s">
-        <v>195</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K45" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B46" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>199</v>
       </c>
       <c r="E46">
-        <v>44.531999999999996</v>
+        <v>47.1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G46" s="1">
-        <v>994.59460000000001</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>199</v>
+        <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
+        <v>2928.3125</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" t="s">
+        <v>202</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="K46" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B47" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E47">
         <v>47.1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I47" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K47" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B48" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C48">
         <v>2012</v>
       </c>
       <c r="D48" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E48">
         <v>47.1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="G48" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="I48" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="K48" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2687,29 +2679,15 @@
     <hyperlink ref="J26" r:id="rId18"/>
     <hyperlink ref="J29" r:id="rId19"/>
     <hyperlink ref="J30" r:id="rId20"/>
-    <hyperlink ref="J31" r:id="rId21"/>
-    <hyperlink ref="J32" r:id="rId22"/>
-    <hyperlink ref="J33" r:id="rId23"/>
-    <hyperlink ref="J34" r:id="rId24"/>
-    <hyperlink ref="J35" r:id="rId25"/>
-    <hyperlink ref="J36" r:id="rId26"/>
-    <hyperlink ref="J37" r:id="rId27"/>
-    <hyperlink ref="J38" r:id="rId28"/>
-    <hyperlink ref="J39" r:id="rId29"/>
-    <hyperlink ref="J40" r:id="rId30"/>
-    <hyperlink ref="J41" r:id="rId31"/>
-    <hyperlink ref="J42" r:id="rId32"/>
-    <hyperlink ref="J43" r:id="rId33"/>
-    <hyperlink ref="J44" r:id="rId34"/>
-    <hyperlink ref="J45" r:id="rId35"/>
-    <hyperlink ref="J46" r:id="rId36"/>
-    <hyperlink ref="J47" r:id="rId37"/>
-    <hyperlink ref="J48" r:id="rId38"/>
-    <hyperlink ref="J4" r:id="rId39"/>
-    <hyperlink ref="J5" r:id="rId40"/>
-    <hyperlink ref="J3" r:id="rId41"/>
+    <hyperlink ref="J48" r:id="rId21"/>
+    <hyperlink ref="J4" r:id="rId22"/>
+    <hyperlink ref="J5" r:id="rId23"/>
+    <hyperlink ref="J3" r:id="rId24"/>
+    <hyperlink ref="J31" r:id="rId25" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="J32" r:id="rId26" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
+    <hyperlink ref="J33" r:id="rId27" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed error that caused EEG Solar to appear twice
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="257">
   <si>
     <t>program_identifier</t>
   </si>
@@ -1156,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2621,41 +2621,9 @@
         <v>201</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>203</v>
-      </c>
-      <c r="B48" t="s">
-        <v>204</v>
-      </c>
-      <c r="C48">
-        <v>2012</v>
-      </c>
-      <c r="D48" t="s">
-        <v>199</v>
-      </c>
-      <c r="E48">
-        <v>47.1</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="G48" s="1">
-        <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
-        <v>2928.3125</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I48" t="s">
-        <v>202</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="K48" t="s">
-        <v>201</v>
-      </c>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H48" s="1"/>
+      <c r="J48" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2679,15 +2647,14 @@
     <hyperlink ref="J26" r:id="rId18"/>
     <hyperlink ref="J29" r:id="rId19"/>
     <hyperlink ref="J30" r:id="rId20"/>
-    <hyperlink ref="J48" r:id="rId21"/>
-    <hyperlink ref="J4" r:id="rId22"/>
-    <hyperlink ref="J5" r:id="rId23"/>
-    <hyperlink ref="J3" r:id="rId24"/>
-    <hyperlink ref="J31" r:id="rId25" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="J32" r:id="rId26" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
-    <hyperlink ref="J33" r:id="rId27" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="J4" r:id="rId21"/>
+    <hyperlink ref="J5" r:id="rId22"/>
+    <hyperlink ref="J3" r:id="rId23"/>
+    <hyperlink ref="J31" r:id="rId24" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="J32" r:id="rId25" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
+    <hyperlink ref="J33" r:id="rId26" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated tex tables; finalized Education Policies
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -84,9 +84,6 @@
     <t>Long Training</t>
   </si>
   <si>
-    <t>Government sponsored Training Program lasting longer than 6 months</t>
-  </si>
-  <si>
     <t>shortTraining</t>
   </si>
   <si>
@@ -97,10 +94,6 @@
   </si>
   <si>
     <t>Practice Firm</t>
-  </si>
-  <si>
-    <t>Government sponsored training to obtain a new professional degree in a field other than the
-profession currently held</t>
   </si>
   <si>
     <t>Government sponsored training that simulates a job</t>
@@ -452,9 +445,6 @@
     <t>sportsExpenditure</t>
   </si>
   <si>
-    <t>Familiy Policy</t>
-  </si>
-  <si>
     <t>unemploymentBenefits2006</t>
   </si>
   <si>
@@ -660,9 +650,6 @@
     <t>In 1990 Germany reduced the top income tax rate from 56% to 53%</t>
   </si>
   <si>
-    <t>Government sponsored Training Program lasting less then 6 months</t>
-  </si>
-  <si>
     <t>Government sponsored short-term training programs "Trainingsmaßnahmen", which were introduced again in 1998 after being abolished in 1993</t>
   </si>
   <si>
@@ -778,9 +765,6 @@
   </si>
   <si>
     <t>Between 1999 and 2001 the German income top marginal income tax rate was reduced from 53% to 48.5%. This was the first step of a piece-wise reduction of the top-marginal tax rate in the 2000s.</t>
-  </si>
-  <si>
-    <t>In the year 2005, the top marginal tax rate was lowered once more from 45% to 42%. To date, this has been the final reform with the expection of an increased rate of 45% which has been levied since 2007 on incomes in excess of 250 000 euro per year.</t>
   </si>
   <si>
     <t>Doerrenberg et al. (2017);World Inequality Database (2020)</t>
@@ -794,6 +778,21 @@
   </si>
   <si>
     <t>Top Tax Reform 1990</t>
+  </si>
+  <si>
+    <t>Government sponsored training program lasting longer than 6 months</t>
+  </si>
+  <si>
+    <t>Government sponsored training program lasting less then 6 months</t>
+  </si>
+  <si>
+    <t>In the year 2005, the top marginal tax rate was lowered once more from 45% to 42%. To date, this has been the final reform with the exception of an increased rate of 45% which has been levied since 2007 on incomes in excess of 250 000 euro per year.</t>
+  </si>
+  <si>
+    <t>Family Policy</t>
+  </si>
+  <si>
+    <t>Government sponsored training to obtain a new professional degree in a field other than the profession currently held</t>
   </si>
 </sst>
 </file>
@@ -1156,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,19 +1194,19 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1215,127 +1214,127 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1355,17 +1354,17 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1389,13 +1388,13 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1419,13 +1418,13 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1449,13 +1448,13 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1469,653 +1468,653 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>252</v>
       </c>
       <c r="G10" s="1">
         <v>1396</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
       </c>
       <c r="C11">
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>212</v>
+        <v>253</v>
       </c>
       <c r="G11" s="1">
         <v>1396</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
       </c>
       <c r="C12">
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E12">
         <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G12" s="1">
         <v>1396</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13">
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>256</v>
       </c>
       <c r="G13" s="1">
         <v>1396</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14">
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E14">
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K17" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18">
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
       </c>
       <c r="I18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19">
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E19">
         <v>39.03</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G19" s="1">
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K21" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22">
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K22" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
         <v>52</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
       </c>
       <c r="C23">
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24">
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K24" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25">
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C26">
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>143</v>
+        <v>255</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H26" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K26" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27">
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>143</v>
+        <v>255</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" t="s">
+        <v>236</v>
+      </c>
+      <c r="I27" t="s">
         <v>87</v>
       </c>
-      <c r="H27" t="s">
-        <v>240</v>
-      </c>
-      <c r="I27" t="s">
-        <v>89</v>
-      </c>
       <c r="J27" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K27" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C28">
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>255</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H28" t="s">
+        <v>236</v>
+      </c>
+      <c r="I28" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H28" t="s">
-        <v>240</v>
-      </c>
-      <c r="I28" t="s">
-        <v>89</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="K28" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C29">
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>255</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K29" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C30">
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>255</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="I30" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K30" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31">
         <v>2020</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I31" t="s">
+        <v>100</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I31" t="s">
-        <v>102</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="K31" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C32">
         <v>1990</v>
@@ -2127,24 +2126,24 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="I32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K32" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C33">
         <v>2001</v>
@@ -2156,469 +2155,469 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I33" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K33" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E34">
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
       </c>
       <c r="I34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K34" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E35">
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K35" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C36">
         <v>1993</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E36">
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
       </c>
       <c r="I36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K36" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C37">
         <v>2002</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E37">
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
       </c>
       <c r="I37" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K37" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C38">
         <v>2006</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K38" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C39">
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E39">
         <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K39" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C40">
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E40">
         <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I40" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K40" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C41">
         <v>2004</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E41">
         <v>37.630000000000003</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G41">
         <v>2731</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K41" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B42" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C42">
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="K42" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C43">
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G43" s="1">
         <v>1543.018</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K43" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B44" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C44">
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E44">
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G44" s="1">
         <v>2004.07</v>
       </c>
       <c r="I44" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="K44" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B45" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K45" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B46" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E46">
         <v>47.1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I46" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K46" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B47" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E47">
         <v>47.1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="I47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K47" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
* added more results needed for the paper. * Some minor adjustments to various programs.
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -710,12 +710,6 @@
     <t xml:space="preserve">In 2012 several job centers which where under the supervision of the federal employment agency were decentralized. 41 out of 407 German districts were put in charge of their local job centers. </t>
   </si>
   <si>
-    <t>In Germany electricity produced from renewable sources is subsidized under the "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of wind Energy.</t>
-  </si>
-  <si>
-    <t>In Germany electricity produced from renewable sources is subsidized under the "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of solar Energy.</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -793,6 +787,12 @@
   </si>
   <si>
     <t>Government sponsored training to obtain a new professional degree in a field other than the profession currently held</t>
+  </si>
+  <si>
+    <t>In Germany electricity produced from renewable sources is subsidized under the renewable energy act "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of wind Energy.</t>
+  </si>
+  <si>
+    <t>In Germany electricity produced from renewable sources is subsidized under the renewable energy act  "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of solar Energy.</t>
   </si>
 </sst>
 </file>
@@ -1155,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,7 +1214,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C2">
         <v>1990</v>
@@ -1229,7 +1229,7 @@
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>57</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C3">
         <v>2001</v>
@@ -1255,30 +1255,30 @@
         <v>144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>250</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C4">
         <v>2004</v>
@@ -1287,30 +1287,30 @@
         <v>144</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>250</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C5">
         <v>2005</v>
@@ -1319,22 +1319,22 @@
         <v>144</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G10" s="1">
         <v>1672</v>
@@ -1507,7 +1507,7 @@
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G11" s="1">
         <v>1570</v>
@@ -1573,7 +1573,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
@@ -1920,7 +1920,7 @@
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>77</v>
@@ -1946,13 +1946,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>212</v>
       </c>
       <c r="H26" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I26" t="s">
         <v>87</v>
@@ -1975,13 +1975,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I27" t="s">
         <v>87</v>
@@ -2004,13 +2004,13 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>86</v>
       </c>
       <c r="H28" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I28" t="s">
         <v>87</v>
@@ -2033,7 +2033,7 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E29">
         <v>31.36</v>
@@ -2062,7 +2062,7 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
@@ -2495,7 +2495,7 @@
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E44">
         <v>27</v>
@@ -2565,14 +2565,14 @@
         <v>47.1</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>229</v>
+        <v>255</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="I46" t="s">
         <v>199</v>
@@ -2601,14 +2601,14 @@
         <v>47.1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>230</v>
+        <v>256</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I47" t="s">
         <v>199</v>
@@ -2652,8 +2652,10 @@
     <hyperlink ref="J31" r:id="rId24" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
     <hyperlink ref="J32" r:id="rId25" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
     <hyperlink ref="J33" r:id="rId26" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="J34" r:id="rId27"/>
+    <hyperlink ref="J37" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* changed wrong sign in csv visualization * renamed Family Policies to Parental Leave Reforms * renamed Labor Market Policies to other Labor Market Policies
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="265">
   <si>
     <t>program_identifier</t>
   </si>
@@ -763,9 +763,6 @@
   </si>
   <si>
     <t>In Germany electricity produced from renewable sources is subsidized under the renewable energy act  "Erneuerbare Energien Gesetz". Abrell et al. (2019) estimate the implied carbon emission abatement cost of solar Energy.</t>
-  </si>
-  <si>
-    <t>Age of people who die of covid19 is 81 according to RKI</t>
   </si>
   <si>
     <t>Destatis Online Database Table 12612-0015: Durchschnittliches Alter der Mutter bei der Geburt ihrer
@@ -813,6 +810,15 @@
   </si>
   <si>
     <t>Other Labor Market Policies</t>
+  </si>
+  <si>
+    <t>Hard to tell what the average age of beneficiaries is. Age of people who die of covid19 is 81 according to RKI. But most of the WTP is due to lower economic costs of a smaller R.</t>
+  </si>
+  <si>
+    <t>Hard to tell what the average age of beneficiaries is. Age of people who die of covid19 is 81 according to RKI. But most of the WTP is due to lower economic costs of a smaller R. Missing Value for now.</t>
+  </si>
+  <si>
+    <t>Parental Leave Reform</t>
   </si>
 </sst>
 </file>
@@ -1175,8 +1181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1246,7 @@
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
@@ -1252,7 +1258,7 @@
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>57</v>
@@ -1275,7 +1281,7 @@
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
@@ -1287,7 +1293,7 @@
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>236</v>
@@ -1310,7 +1316,7 @@
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
@@ -1322,7 +1328,7 @@
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>236</v>
@@ -1345,7 +1351,7 @@
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
@@ -1357,7 +1363,7 @@
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>236</v>
@@ -1500,7 +1506,7 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
@@ -1533,7 +1539,7 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
@@ -1566,7 +1572,7 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E12">
         <v>36</v>
@@ -1599,7 +1605,7 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E13">
         <v>31</v>
@@ -1632,7 +1638,7 @@
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E14">
         <v>37</v>
@@ -1665,7 +1671,7 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E15">
         <v>37</v>
@@ -1698,7 +1704,7 @@
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E16">
         <v>38.86</v>
@@ -1731,7 +1737,7 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E17">
         <v>40.17</v>
@@ -1764,7 +1770,7 @@
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
@@ -1796,7 +1802,7 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E19">
         <v>39.03</v>
@@ -1837,7 +1843,7 @@
         <v>45</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I20" t="s">
         <v>70</v>
@@ -1869,7 +1875,7 @@
         <v>46</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I21" t="s">
         <v>70</v>
@@ -1892,7 +1898,7 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
@@ -1921,7 +1927,7 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
@@ -1950,7 +1956,7 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
@@ -1988,7 +1994,7 @@
         <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I25" t="s">
         <v>73</v>
@@ -2011,13 +2017,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>209</v>
       </c>
       <c r="H26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I26" t="s">
         <v>87</v>
@@ -2040,13 +2046,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I27" t="s">
         <v>87</v>
@@ -2069,7 +2075,7 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="E28">
         <v>28.1</v>
@@ -2078,7 +2084,7 @@
         <v>86</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I28" t="s">
         <v>87</v>
@@ -2101,7 +2107,7 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="E29">
         <v>31.36</v>
@@ -2130,7 +2136,7 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>243</v>
+        <v>264</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
@@ -2151,12 +2157,12 @@
         <v>166</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2164,14 +2170,11 @@
       <c r="D31" t="s">
         <v>81</v>
       </c>
-      <c r="E31">
-        <v>81</v>
-      </c>
       <c r="F31" s="1" t="s">
         <v>98</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="I31" t="s">
         <v>99</v>
@@ -2409,7 +2412,7 @@
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E39">
         <v>36.92</v>
@@ -2441,7 +2444,7 @@
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E40">
         <v>37.71</v>
@@ -2505,7 +2508,7 @@
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
@@ -2537,7 +2540,7 @@
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
@@ -2569,7 +2572,7 @@
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E44">
         <v>27</v>
@@ -2601,7 +2604,7 @@
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
@@ -2646,7 +2649,7 @@
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I46" t="s">
         <v>196</v>
@@ -2682,7 +2685,7 @@
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I47" t="s">
         <v>196</v>

</xml_diff>

<commit_message>
*fixed bug where two programs would not be displayed in the willingnesst to pay and net cost figures * programs belonging to category "Other" are now displayed in grey
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="263">
   <si>
     <t>program_identifier</t>
   </si>
@@ -751,9 +751,6 @@
   </si>
   <si>
     <t>In the year 2005, the top marginal tax rate was lowered once more from 45% to 42%. To date, this has been the final reform with the exception of an increased rate of 45% which has been levied since 2007 on incomes in excess of 250 000 euro per year.</t>
-  </si>
-  <si>
-    <t>Family Policy</t>
   </si>
   <si>
     <t>Government sponsored training to obtain a new professional degree in a field other than the profession currently held</t>
@@ -810,9 +807,6 @@
   </si>
   <si>
     <t>Other Labor Market Policies</t>
-  </si>
-  <si>
-    <t>Hard to tell what the average age of beneficiaries is. Age of people who die of covid19 is 81 according to RKI. But most of the WTP is due to lower economic costs of a smaller R.</t>
   </si>
   <si>
     <t>Hard to tell what the average age of beneficiaries is. Age of people who die of covid19 is 81 according to RKI. But most of the WTP is due to lower economic costs of a smaller R. Missing Value for now.</t>
@@ -1181,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,7 +1240,7 @@
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
@@ -1258,7 +1252,7 @@
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>57</v>
@@ -1281,7 +1275,7 @@
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
@@ -1293,7 +1287,7 @@
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>236</v>
@@ -1316,7 +1310,7 @@
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
@@ -1328,7 +1322,7 @@
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>236</v>
@@ -1351,7 +1345,7 @@
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
@@ -1363,7 +1357,7 @@
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>236</v>
@@ -1506,7 +1500,7 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
@@ -1539,7 +1533,7 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
@@ -1572,7 +1566,7 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E12">
         <v>36</v>
@@ -1605,13 +1599,13 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
@@ -1638,7 +1632,7 @@
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E14">
         <v>37</v>
@@ -1671,7 +1665,7 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E15">
         <v>37</v>
@@ -1704,7 +1698,7 @@
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E16">
         <v>38.86</v>
@@ -1737,7 +1731,7 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E17">
         <v>40.17</v>
@@ -1770,7 +1764,7 @@
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
@@ -1802,7 +1796,7 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E19">
         <v>39.03</v>
@@ -1843,7 +1837,7 @@
         <v>45</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I20" t="s">
         <v>70</v>
@@ -1875,7 +1869,7 @@
         <v>46</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I21" t="s">
         <v>70</v>
@@ -1898,7 +1892,7 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
@@ -1927,7 +1921,7 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
@@ -1956,7 +1950,7 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
@@ -1994,7 +1988,7 @@
         <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I25" t="s">
         <v>73</v>
@@ -2017,13 +2011,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>209</v>
       </c>
       <c r="H26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I26" t="s">
         <v>87</v>
@@ -2046,13 +2040,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I27" t="s">
         <v>87</v>
@@ -2075,7 +2069,7 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E28">
         <v>28.1</v>
@@ -2084,7 +2078,7 @@
         <v>86</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I28" t="s">
         <v>87</v>
@@ -2107,7 +2101,7 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E29">
         <v>31.36</v>
@@ -2136,7 +2130,7 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
@@ -2162,7 +2156,7 @@
         <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2174,7 +2168,7 @@
         <v>98</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I31" t="s">
         <v>99</v>
@@ -2412,7 +2406,7 @@
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E39">
         <v>36.92</v>
@@ -2444,7 +2438,7 @@
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E40">
         <v>37.71</v>
@@ -2508,7 +2502,7 @@
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
@@ -2540,7 +2534,7 @@
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
@@ -2572,7 +2566,7 @@
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E44">
         <v>27</v>
@@ -2604,7 +2598,7 @@
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
@@ -2642,14 +2636,14 @@
         <v>50.49</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I46" t="s">
         <v>196</v>
@@ -2678,14 +2672,14 @@
         <v>50.49</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I47" t="s">
         <v>196</v>

</xml_diff>

<commit_message>
* added option to overwrite ETI * replaced relative risk aversion with ETI in web visualization * changed tax rate options
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -587,9 +587,6 @@
     <t>mergele2020</t>
   </si>
   <si>
-    <t>Mergeke &amp; Weber (2020)</t>
-  </si>
-  <si>
     <t>decentralizedEmploymentServices</t>
   </si>
   <si>
@@ -813,6 +810,9 @@
   </si>
   <si>
     <t>Parental Leave Reform</t>
+  </si>
+  <si>
+    <t>Mergele &amp; Weber (2020)</t>
   </si>
 </sst>
 </file>
@@ -1175,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,25 +1234,25 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>57</v>
@@ -1266,107 +1266,107 @@
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" t="s">
         <v>227</v>
-      </c>
-      <c r="B3" t="s">
-        <v>228</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
         <v>230</v>
-      </c>
-      <c r="B4" t="s">
-        <v>231</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" t="s">
         <v>232</v>
-      </c>
-      <c r="B5" t="s">
-        <v>233</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>237</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1386,11 +1386,11 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>58</v>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>59</v>
@@ -1500,20 +1500,20 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G10" s="1">
         <v>1672</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J10" t="s">
         <v>64</v>
@@ -1533,20 +1533,20 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G11" s="1">
         <v>1570</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
@@ -1566,7 +1566,7 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E12">
         <v>36</v>
@@ -1579,7 +1579,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J12" t="s">
         <v>64</v>
@@ -1599,20 +1599,20 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J13" t="s">
         <v>64</v>
@@ -1632,7 +1632,7 @@
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E14">
         <v>37</v>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>65</v>
@@ -1665,20 +1665,20 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G15" s="1">
         <v>1542.066</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>65</v>
@@ -1698,13 +1698,13 @@
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
@@ -1731,13 +1731,13 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
@@ -1764,19 +1764,19 @@
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
       </c>
       <c r="I18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>68</v>
@@ -1796,7 +1796,7 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E19">
         <v>39.03</v>
@@ -1808,7 +1808,7 @@
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>160</v>
@@ -1828,7 +1828,7 @@
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E20">
         <v>46.96</v>
@@ -1837,7 +1837,7 @@
         <v>45</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I20" t="s">
         <v>70</v>
@@ -1860,7 +1860,7 @@
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E21">
         <v>46.96</v>
@@ -1869,7 +1869,7 @@
         <v>46</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I21" t="s">
         <v>70</v>
@@ -1892,13 +1892,13 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I22" t="s">
         <v>71</v>
@@ -1921,13 +1921,13 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I23" t="s">
         <v>71</v>
@@ -1950,13 +1950,13 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I24" t="s">
         <v>71</v>
@@ -1979,7 +1979,7 @@
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E25">
         <v>46.96</v>
@@ -1988,7 +1988,7 @@
         <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I25" t="s">
         <v>73</v>
@@ -2011,13 +2011,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I26" t="s">
         <v>87</v>
@@ -2040,13 +2040,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I27" t="s">
         <v>87</v>
@@ -2069,7 +2069,7 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E28">
         <v>28.1</v>
@@ -2078,7 +2078,7 @@
         <v>86</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I28" t="s">
         <v>87</v>
@@ -2101,13 +2101,13 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I29" t="s">
         <v>91</v>
@@ -2130,13 +2130,13 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
@@ -2156,7 +2156,7 @@
         <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2168,7 +2168,7 @@
         <v>98</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I31" t="s">
         <v>99</v>
@@ -2197,7 +2197,7 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I32" t="s">
         <v>103</v>
@@ -2255,7 +2255,7 @@
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
@@ -2287,7 +2287,7 @@
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
@@ -2319,7 +2319,7 @@
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
@@ -2351,7 +2351,7 @@
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
@@ -2406,7 +2406,7 @@
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E39">
         <v>36.92</v>
@@ -2438,13 +2438,13 @@
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E40">
         <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G40" s="1">
         <v>2624.9580000000001</v>
@@ -2502,13 +2502,13 @@
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G42" s="1">
         <v>1278.2249999999999</v>
@@ -2534,7 +2534,7 @@
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
@@ -2566,13 +2566,13 @@
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E44">
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G44" s="1">
         <v>2004.07</v>
@@ -2589,28 +2589,28 @@
     </row>
     <row r="45" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>188</v>
+      </c>
+      <c r="B45" t="s">
         <v>189</v>
-      </c>
-      <c r="B45" t="s">
-        <v>190</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>188</v>
+        <v>262</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>186</v>
@@ -2621,74 +2621,74 @@
     </row>
     <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>190</v>
+      </c>
+      <c r="B46" t="s">
         <v>191</v>
-      </c>
-      <c r="B46" t="s">
-        <v>192</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E46">
         <v>50.49</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J46" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K46" t="s">
         <v>194</v>
-      </c>
-      <c r="K46" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>196</v>
+      </c>
+      <c r="B47" t="s">
         <v>197</v>
-      </c>
-      <c r="B47" t="s">
-        <v>198</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E47">
         <v>50.49</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J47" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="K47" t="s">
         <v>194</v>
-      </c>
-      <c r="K47" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed missing category for coronavirusRestrictions
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -313,12 +313,6 @@
     <t>https://ideas.repec.org/p/iza/izadps/dp12935.html;https://ideas.repec.org/a/spr/jopoec/v26y2013i3p983-1005.html</t>
   </si>
   <si>
-    <t>coronavirusLockdownR1</t>
-  </si>
-  <si>
-    <t>Coronavirus induced lockdown with a reproduction number of R=0.627 compared with a too lash lockdown which would maintained R=1.</t>
-  </si>
-  <si>
     <t>Dorn et. al (2020)</t>
   </si>
   <si>
@@ -788,9 +782,6 @@
     <t>Assume same age as for speed limit</t>
   </si>
   <si>
-    <t>Coronavirus Lockdown R=0.6 vs R=1</t>
-  </si>
-  <si>
     <t>Top Tax Reform</t>
   </si>
   <si>
@@ -813,6 +804,15 @@
   </si>
   <si>
     <t>Mergele &amp; Weber (2020)</t>
+  </si>
+  <si>
+    <t>coronavirusRestrictions</t>
+  </si>
+  <si>
+    <t>Coronavirus Restrictions</t>
+  </si>
+  <si>
+    <t>Coronavirus induced restrictions with a reproduction number of R=0.627 compared with a too lash measures which would maintained R=1.</t>
   </si>
 </sst>
 </file>
@@ -1175,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,7 +1226,7 @@
         <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
@@ -1234,139 +1234,139 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" t="s">
         <v>149</v>
-      </c>
-      <c r="K2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>237</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>237</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1386,17 +1386,17 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>58</v>
       </c>
       <c r="K6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1420,13 +1420,13 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>59</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
         <v>60</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1486,7 +1486,7 @@
         <v>62</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1500,26 +1500,26 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G10" s="1">
         <v>1672</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J10" t="s">
         <v>64</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1533,26 +1533,26 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G11" s="1">
         <v>1570</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J11" t="s">
         <v>64</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1566,7 +1566,7 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E12">
         <v>36</v>
@@ -1579,13 +1579,13 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J12" t="s">
         <v>64</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1599,26 +1599,26 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J13" t="s">
         <v>64</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1632,7 +1632,7 @@
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E14">
         <v>37</v>
@@ -1645,13 +1645,13 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1665,26 +1665,26 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G15" s="1">
         <v>1542.066</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1698,13 +1698,13 @@
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
@@ -1717,7 +1717,7 @@
         <v>67</v>
       </c>
       <c r="K16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1731,13 +1731,13 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
@@ -1750,7 +1750,7 @@
         <v>67</v>
       </c>
       <c r="K17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1764,25 +1764,25 @@
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
       </c>
       <c r="I18" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1796,7 +1796,7 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E19">
         <v>39.03</v>
@@ -1808,13 +1808,13 @@
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E20">
         <v>46.96</v>
@@ -1837,7 +1837,7 @@
         <v>45</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I20" t="s">
         <v>70</v>
@@ -1846,7 +1846,7 @@
         <v>69</v>
       </c>
       <c r="K20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1860,7 +1860,7 @@
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E21">
         <v>46.96</v>
@@ -1869,7 +1869,7 @@
         <v>46</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="I21" t="s">
         <v>70</v>
@@ -1878,7 +1878,7 @@
         <v>69</v>
       </c>
       <c r="K21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -1892,13 +1892,13 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="I22" t="s">
         <v>71</v>
@@ -1907,7 +1907,7 @@
         <v>72</v>
       </c>
       <c r="K22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1921,13 +1921,13 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I23" t="s">
         <v>71</v>
@@ -1936,7 +1936,7 @@
         <v>72</v>
       </c>
       <c r="K23" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1950,13 +1950,13 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I24" t="s">
         <v>71</v>
@@ -1965,7 +1965,7 @@
         <v>72</v>
       </c>
       <c r="K24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1979,7 +1979,7 @@
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E25">
         <v>46.96</v>
@@ -1988,7 +1988,7 @@
         <v>77</v>
       </c>
       <c r="H25" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I25" t="s">
         <v>73</v>
@@ -1997,7 +1997,7 @@
         <v>74</v>
       </c>
       <c r="K25" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2011,13 +2011,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I26" t="s">
         <v>87</v>
@@ -2026,7 +2026,7 @@
         <v>88</v>
       </c>
       <c r="K26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -2040,13 +2040,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>85</v>
       </c>
       <c r="H27" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="I27" t="s">
         <v>87</v>
@@ -2055,7 +2055,7 @@
         <v>88</v>
       </c>
       <c r="K27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E28">
         <v>28.1</v>
@@ -2078,7 +2078,7 @@
         <v>86</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I28" t="s">
         <v>87</v>
@@ -2087,7 +2087,7 @@
         <v>88</v>
       </c>
       <c r="K28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2101,13 +2101,13 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I29" t="s">
         <v>91</v>
@@ -2116,7 +2116,7 @@
         <v>92</v>
       </c>
       <c r="K29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2130,13 +2130,13 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
@@ -2148,15 +2148,15 @@
         <v>96</v>
       </c>
       <c r="K30" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>260</v>
       </c>
       <c r="B31" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2165,27 +2165,27 @@
         <v>81</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I31" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="I31" t="s">
-        <v>99</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="K31" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C32">
         <v>1990</v>
@@ -2197,24 +2197,24 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C33">
         <v>2001</v>
@@ -2226,245 +2226,245 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E34">
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
       </c>
       <c r="I34" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E35">
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C36">
         <v>1993</v>
       </c>
       <c r="D36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E36">
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
       </c>
       <c r="I36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K36" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C37">
         <v>2002</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E37">
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
       </c>
       <c r="I37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K37" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C38">
         <v>2006</v>
       </c>
       <c r="D38" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I38" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C39">
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E39">
         <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C40">
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E40">
         <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K40" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C41">
         <v>2004</v>
@@ -2476,219 +2476,219 @@
         <v>37.630000000000003</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G41">
         <v>2731</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="210" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C42">
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C43">
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G43" s="1">
         <v>1543.018</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K43" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C44">
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E44">
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G44" s="1">
         <v>2004.07</v>
       </c>
       <c r="I44" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K44" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E46">
         <v>50.49</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I46" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K46" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B47" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E47">
         <v>50.49</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K47" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
*ordered functions in functions.R. *added further comments
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -776,15 +776,6 @@
     <t>Potential introduction of a law which would mandate that every bicycle rider has to wear a helmet.</t>
   </si>
   <si>
-    <t>In 1979, the maternity leave coverage was extended from 2 to 6 months. During these 6 months all entitled mothers received a maternal leave benefit of 750 Deutschmarks per month. Among other outcomes, Dustmann &amp; Schönberg (2011), study the effects of the reform on earnings of affected mothers and the wages of their children at the age of 28.</t>
-  </si>
-  <si>
-    <t>The 1986 maternity leave reform extended the period during which mothers had the right to return to their previous job and received maternity benefits from 6 to 10 months. At the same, the maternity benefit was reduced from 750 Deutschmarks to 600 Deutschmarks.  Among other outcomes, Dustmann &amp; Schönberg (2011), study the effects of the reform on earnings of affected mothers and the graduation rates of their children from the academic high school track.</t>
-  </si>
-  <si>
-    <t>In contrast to the maternity leave reforms in 1979 and 1986, the maternity benefit amount as well as the period of entitlement remained unchanged. Instead, the mother's right to return to their previous job was prolonged to 36 months. Among other outcomes, Dustmann &amp; Schönberg (2011), study the effects of the reform on earnings of affected mothers and their childrens' attendce of the academic high school track at the age of 14.</t>
-  </si>
-  <si>
     <t>The home care subsidy "Betreuungsgeld" was introduced in 2013 and was meant to compensate parents who did not make use of subsidized childcare. It pays 100€ for up to 22 months.</t>
   </si>
   <si>
@@ -813,6 +804,15 @@
   </si>
   <si>
     <t>In 2012, several job centers that had been under the supervision of the federal employment agency were decentralized. 41 out of 407 German districts were put in charge of their local job centers. Mergele &amp; Weber (2020) find that decentralization increased unemployment durations led to a shift of costs to higher levels of government.</t>
+  </si>
+  <si>
+    <t>In 1979, the maternity leave coverage was extended from 2 to 6 months. During these 6 months all entitled mothers received a maternal leave benefit of 750 Deutschmarks per month. Among other outcomes, Dustmann &amp; Schönberg (2011) study the effects of the reform on earnings of affected mothers and the wages of their children at the age of 28.</t>
+  </si>
+  <si>
+    <t>The 1986 maternity leave reform extended the period during which mothers had the right to return to their previous job and received maternity benefits from 6 to 10 months. At the same, the maternity benefit was reduced from 750 Deutschmarks to 600 Deutschmarks.  Among other outcomes, Dustmann &amp; Schönberg (2011) study the effects of the reform on earnings of affected mothers and the graduation rates of their children from the academic high school track.</t>
+  </si>
+  <si>
+    <t>In contrast to the maternity leave reforms in 1979 and 1986, the maternity benefit amount as well as the period of entitlement remained unchanged. Instead, the mother's right to return to their previous job was prolonged to 36 months. Among other outcomes, Dustmann &amp; Schönberg (2011) study the effects of the reform on earnings of affected mothers and their childrens' attendce of the academic high school track at the age of 14.</t>
   </si>
 </sst>
 </file>
@@ -1175,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F46" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="F22" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,7 +2014,7 @@
         <v>237</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="H26" t="s">
         <v>223</v>
@@ -2043,7 +2043,7 @@
         <v>237</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="H27" t="s">
         <v>223</v>
@@ -2075,7 +2075,7 @@
         <v>28.1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>222</v>
@@ -2107,7 +2107,7 @@
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I29" t="s">
         <v>83</v>
@@ -2165,7 +2165,7 @@
         <v>75</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>236</v>
@@ -2255,7 +2255,7 @@
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
@@ -2287,7 +2287,7 @@
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
@@ -2319,7 +2319,7 @@
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
@@ -2351,7 +2351,7 @@
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
@@ -2383,7 +2383,7 @@
         <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I38" t="s">
         <v>111</v>
@@ -2412,7 +2412,7 @@
         <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G39" s="1">
         <v>1593.2249999999999</v>
@@ -2476,7 +2476,7 @@
         <v>37.630000000000003</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G41">
         <v>2731</v>
@@ -2604,7 +2604,7 @@
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>

</xml_diff>

<commit_message>
added compulsarySchooling based on Piopiunik (2014)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="266">
   <si>
     <t>program_identifier</t>
   </si>
@@ -807,6 +807,21 @@
   </si>
   <si>
     <t>Coronavirus induced restrictions with a reproduction number of R=0.627, which was the status quo in April 2020, compared to less restrictive measures which would increase R to 1.</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/bla/scandj/v116y2014i3p878-907.html</t>
+  </si>
+  <si>
+    <t>Piopiunik (2014)</t>
+  </si>
+  <si>
+    <t>Between 1946 and 1969 all German federal states extended the length of the least academic school track "Hauptschule" in Germany by one year. Piopiunik (2014) finds that this reform improved educational outcomes of sons whose mothers were affected by the compulsary schooling reform.</t>
+  </si>
+  <si>
+    <t>compulsarySchooling</t>
+  </si>
+  <si>
+    <t>Compulsary Schooling</t>
   </si>
 </sst>
 </file>
@@ -1169,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="C44" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,9 +2700,32 @@
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>264</v>
+      </c>
+      <c r="B48" t="s">
+        <v>265</v>
+      </c>
+      <c r="C48">
+        <v>1967</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48">
+        <v>16</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>263</v>
+      </c>
       <c r="H48" s="1"/>
-      <c r="J48" s="2"/>
+      <c r="I48" t="s">
+        <v>262</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>261</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2719,8 +2757,9 @@
     <hyperlink ref="J37" r:id="rId26"/>
     <hyperlink ref="J4" r:id="rId27"/>
     <hyperlink ref="J3" r:id="rId28"/>
+    <hyperlink ref="J48" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added tracking reform in Bavaria
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="270">
   <si>
     <t>program_identifier</t>
   </si>
@@ -822,6 +822,18 @@
   </si>
   <si>
     <t>Compulsary Schooling</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/ces/ifowps/_153.html</t>
+  </si>
+  <si>
+    <t>In 2000, the Bavarian parliament passed a reform that started tracking (i.e. students attending different levels of secondary education) in 4th instead of 6th grade. The reform only affected the basic and middle track (Hauptschule and Realschule). Piopiunik (2014) finds that the earlier tracking reduces PISA test scores by 13 points on average.</t>
+  </si>
+  <si>
+    <t>Tracking Bavaria</t>
+  </si>
+  <si>
+    <t>trackingBavaria</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" workbookViewId="0">
-      <selection activeCell="L48" sqref="L48"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2725,6 +2737,32 @@
       </c>
       <c r="J48" s="2" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>269</v>
+      </c>
+      <c r="B49" t="s">
+        <v>268</v>
+      </c>
+      <c r="C49">
+        <v>2003</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49">
+        <v>10</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="I49" t="s">
+        <v>262</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2758,8 +2796,9 @@
     <hyperlink ref="J4" r:id="rId27"/>
     <hyperlink ref="J3" r:id="rId28"/>
     <hyperlink ref="J48" r:id="rId29"/>
+    <hyperlink ref="J49" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added school Fees based on Riphahn (2012)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="275">
   <si>
     <t>program_identifier</t>
   </si>
@@ -834,6 +834,21 @@
   </si>
   <si>
     <t>trackingBavaria</t>
+  </si>
+  <si>
+    <t>schoolFees</t>
+  </si>
+  <si>
+    <t>School Fees</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/bla/scandj/v114y2012i1p148-176.html</t>
+  </si>
+  <si>
+    <t>Riphahn (2012)</t>
+  </si>
+  <si>
+    <t>After WW II, school fees were successively abolished in all German federal states. Riphahn (2012) finds that this increased attendance of the advanced school track  "Gymnasium" which starts after 4th grade.</t>
   </si>
 </sst>
 </file>
@@ -1194,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2763,6 +2778,32 @@
       </c>
       <c r="J49" s="2" t="s">
         <v>266</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" t="s">
+        <v>271</v>
+      </c>
+      <c r="C50">
+        <v>1957</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50">
+        <v>10</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -2797,8 +2838,9 @@
     <hyperlink ref="J3" r:id="rId28"/>
     <hyperlink ref="J48" r:id="rId29"/>
     <hyperlink ref="J49" r:id="rId30"/>
+    <hyperlink ref="J50" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added "Rock your Life" Mentoring program based on Resnjanskij et al. (2021)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="280">
   <si>
     <t>program_identifier</t>
   </si>
@@ -849,6 +849,21 @@
   </si>
   <si>
     <t>After WW II, school fees were successively abolished in all German federal states. Riphahn (2012) finds that this increased attendance of the advanced school track  "Gymnasium" which starts after 4th grade.</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/ces/ceswps/_8870.html</t>
+  </si>
+  <si>
+    <t>Resnjanskij et al. (2021)</t>
+  </si>
+  <si>
+    <t>rockYourLife</t>
+  </si>
+  <si>
+    <t>Mentoring Program Rock your Life</t>
+  </si>
+  <si>
+    <t>Rock your Life is a mentoring program, where university students take on mentees from the lowest-track secondary schools (Hauptschule). The program aims at providing career guidance, establishing career visions, and fostering self-esteem and trust in the mentees’ own skills and abilities</t>
   </si>
 </sst>
 </file>
@@ -1209,10 +1224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K50"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,6 +2819,32 @@
       </c>
       <c r="J50" s="2" t="s">
         <v>272</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>277</v>
+      </c>
+      <c r="B51" t="s">
+        <v>278</v>
+      </c>
+      <c r="C51">
+        <v>2017</v>
+      </c>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51">
+        <v>14</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="I51" t="s">
+        <v>276</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2839,8 +2880,9 @@
     <hyperlink ref="J48" r:id="rId29"/>
     <hyperlink ref="J49" r:id="rId30"/>
     <hyperlink ref="J50" r:id="rId31"/>
+    <hyperlink ref="J51" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Interim Degrees based on Obergruber & Zierow (2020)
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="285">
   <si>
     <t>program_identifier</t>
   </si>
@@ -864,6 +864,21 @@
   </si>
   <si>
     <t>Rock your Life is a mentoring program, where university students take on mentees from the lowest-track secondary schools (Hauptschule). The program aims at providing career guidance, establishing career visions, and fostering self-esteem and trust in the mentees’ own skills and abilities</t>
+  </si>
+  <si>
+    <t>interimDegrees</t>
+  </si>
+  <si>
+    <t>Interim Degrees</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/ecoedu/v75y2020ics0272775718307179.html</t>
+  </si>
+  <si>
+    <t>Obergruber &amp; Zierow (2020)</t>
+  </si>
+  <si>
+    <t>All German federal states introduced interim degrees, which award the degree of the middle track "Realschule" to everyone who completes the the 10th grade of the highest track of the German school system "Gymnasium". The idea behind this reform was provide a fallback option for students not being able to complete the high track. Obergruber &amp; Zierow (2020) find that this reform incentivized students to stay on the highest track.</t>
   </si>
 </sst>
 </file>
@@ -1224,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2845,6 +2860,32 @@
       </c>
       <c r="J51" s="2" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>280</v>
+      </c>
+      <c r="B52" t="s">
+        <v>281</v>
+      </c>
+      <c r="C52">
+        <v>1978</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52">
+        <v>16</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2881,8 +2922,9 @@
     <hyperlink ref="J49" r:id="rId30"/>
     <hyperlink ref="J50" r:id="rId31"/>
     <hyperlink ref="J51" r:id="rId32"/>
+    <hyperlink ref="J52" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* added option to export as JSON. This should make the web viz easier to extend and update. * Also there is less redundant data stored using the JSON approach * Changed two column names in programs.xlsx
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -153,12 +153,6 @@
     <t>Subsidized Job Opportunities</t>
   </si>
   <si>
-    <t>Links</t>
-  </si>
-  <si>
-    <t>Papers</t>
-  </si>
-  <si>
     <t>Atkinson &amp; Piketty (2010);Gottfried &amp; Schellhorn (2004)</t>
   </si>
   <si>
@@ -879,6 +873,12 @@
   </si>
   <si>
     <t>All German federal states introduced interim degrees, which award the degree of the middle track "Realschule" to everyone who completes the the 10th grade of the highest track of the German school system "Gymnasium". The idea behind this reform was provide a fallback option for students not being able to complete the high track. Obergruber &amp; Zierow (2020) find that this reform incentivized students to stay on the highest track.</t>
+  </si>
+  <si>
+    <t>sources</t>
+  </si>
+  <si>
+    <t>links</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,13 +1286,13 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>283</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>44</v>
+        <v>284</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
@@ -1300,139 +1300,139 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" t="s">
         <v>129</v>
-      </c>
-      <c r="K2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1452,17 +1452,17 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1482,17 +1482,17 @@
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1512,17 +1512,17 @@
         <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1542,17 +1542,17 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1566,26 +1566,26 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G10" s="1">
         <v>1672</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1599,26 +1599,26 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G11" s="1">
         <v>1570</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1632,26 +1632,26 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E12">
         <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G12" s="1">
         <v>1434</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1665,26 +1665,26 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1692,32 +1692,32 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C14">
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E14">
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G14" s="1">
         <v>1559.6189999999999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1731,26 +1731,26 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G15" s="1">
         <v>1542.066</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1758,32 +1758,32 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C16">
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1797,26 +1797,26 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1824,31 +1824,31 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C18">
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
       </c>
       <c r="I18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1862,25 +1862,25 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E19">
         <v>39.03</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G19" s="1">
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1894,25 +1894,25 @@
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E20">
         <v>46.96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1926,25 +1926,25 @@
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E21">
         <v>46.96</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -1958,22 +1958,22 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1987,22 +1987,22 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -2016,242 +2016,242 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="I24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25">
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E25">
         <v>46.96</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K25" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C26">
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27">
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K27" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28">
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E28">
         <v>28.1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29">
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I29" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C30">
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="I30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B31" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C31">
         <v>2020</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C32">
         <v>1990</v>
@@ -2263,24 +2263,24 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C33">
         <v>2001</v>
@@ -2292,477 +2292,477 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E34">
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
       </c>
       <c r="I34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E35">
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C36">
         <v>1993</v>
       </c>
       <c r="D36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E36">
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
       </c>
       <c r="I36" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C37">
         <v>2002</v>
       </c>
       <c r="D37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E37">
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
       </c>
       <c r="I37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K37" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C38">
         <v>2006</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I38" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C39">
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E39">
         <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40">
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E40">
         <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C41">
         <v>2004</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E41">
         <v>37.630000000000003</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G41">
         <v>2731</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K41" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C42">
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C43">
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G43" s="1">
         <v>1543.018</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C44">
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E44">
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G44" s="1">
         <v>2004.07</v>
       </c>
       <c r="I44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="K45" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E46">
         <v>50.49</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I46" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K46" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E47">
         <v>50.49</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I47" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K47" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B48" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C48">
         <v>1967</v>
@@ -2774,22 +2774,22 @@
         <v>16</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B49" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C49">
         <v>2003</v>
@@ -2801,21 +2801,21 @@
         <v>10</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I49" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B50" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C50">
         <v>1957</v>
@@ -2827,21 +2827,21 @@
         <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B51" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C51">
         <v>2017</v>
@@ -2853,21 +2853,21 @@
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I51" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B52" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C52">
         <v>1978</v>
@@ -2879,13 +2879,13 @@
         <v>16</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed wrong year in short description
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -289,9 +289,6 @@
     <t>Baumgartner &amp; Steiner (2006)</t>
   </si>
   <si>
-    <t>Bafög is a means-tested public German student loan program. Eligible students only have to pay back about 50% of the loan. In 1990, the threshold of parents' income above which students are no longer eligible for Bafög was lowered.</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/a/oup/qjecon/v127y2012i2p701-752.html;https://ideas.repec.org/a/anr/reveco/v8y2016p547-581.html</t>
   </si>
   <si>
@@ -879,6 +876,9 @@
   </si>
   <si>
     <t>links</t>
+  </si>
+  <si>
+    <t>Bafög is a means-tested public German student loan program. Eligible students only have to pay back about 50% of the loan. In 2001, the threshold of parents' income above which students are no longer eligible for Bafög was lowered.</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,13 +1286,13 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
@@ -1300,139 +1300,139 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" t="s">
         <v>186</v>
-      </c>
-      <c r="B3" t="s">
-        <v>187</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" t="s">
         <v>188</v>
-      </c>
-      <c r="B4" t="s">
-        <v>189</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" t="s">
         <v>190</v>
-      </c>
-      <c r="B5" t="s">
-        <v>191</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1452,17 +1452,17 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1482,17 +1482,17 @@
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
@@ -1522,7 +1522,7 @@
         <v>47</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
@@ -1552,7 +1552,7 @@
         <v>49</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1566,26 +1566,26 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G10" s="1">
         <v>1672</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J10" t="s">
         <v>51</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1599,26 +1599,26 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G11" s="1">
         <v>1570</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J11" t="s">
         <v>51</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1632,26 +1632,26 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E12">
         <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G12" s="1">
         <v>1434</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J12" t="s">
         <v>51</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1665,26 +1665,26 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J13" t="s">
         <v>51</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1692,32 +1692,32 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C14">
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E14">
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G14" s="1">
         <v>1559.6189999999999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1731,26 +1731,26 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G15" s="1">
         <v>1542.066</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1758,19 +1758,19 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C16">
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
@@ -1783,7 +1783,7 @@
         <v>54</v>
       </c>
       <c r="K16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1797,13 +1797,13 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
@@ -1816,7 +1816,7 @@
         <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1824,31 +1824,31 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C18">
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
       </c>
       <c r="I18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1862,25 +1862,25 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E19">
         <v>39.03</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G19" s="1">
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K19" t="s">
         <v>138</v>
-      </c>
-      <c r="K19" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1894,16 +1894,16 @@
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E20">
         <v>46.96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I20" t="s">
         <v>57</v>
@@ -1912,7 +1912,7 @@
         <v>56</v>
       </c>
       <c r="K20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1926,16 +1926,16 @@
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E21">
         <v>46.96</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I21" t="s">
         <v>57</v>
@@ -1944,7 +1944,7 @@
         <v>56</v>
       </c>
       <c r="K21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -1958,13 +1958,13 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I22" t="s">
         <v>58</v>
@@ -1973,7 +1973,7 @@
         <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1987,13 +1987,13 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I23" t="s">
         <v>58</v>
@@ -2002,7 +2002,7 @@
         <v>59</v>
       </c>
       <c r="K23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -2016,13 +2016,13 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I24" t="s">
         <v>58</v>
@@ -2031,7 +2031,7 @@
         <v>59</v>
       </c>
       <c r="K24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2045,16 +2045,16 @@
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E25">
         <v>46.96</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I25" t="s">
         <v>60</v>
@@ -2063,7 +2063,7 @@
         <v>61</v>
       </c>
       <c r="K25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2077,13 +2077,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H26" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I26" t="s">
         <v>71</v>
@@ -2092,7 +2092,7 @@
         <v>72</v>
       </c>
       <c r="K26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
@@ -2106,13 +2106,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I27" t="s">
         <v>71</v>
@@ -2121,7 +2121,7 @@
         <v>72</v>
       </c>
       <c r="K27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -2135,16 +2135,16 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E28">
         <v>28.1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I28" t="s">
         <v>71</v>
@@ -2153,7 +2153,7 @@
         <v>72</v>
       </c>
       <c r="K28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2167,13 +2167,13 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I29" t="s">
         <v>75</v>
@@ -2182,7 +2182,7 @@
         <v>76</v>
       </c>
       <c r="K29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2196,13 +2196,13 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
@@ -2214,15 +2214,15 @@
         <v>80</v>
       </c>
       <c r="K30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" t="s">
         <v>209</v>
-      </c>
-      <c r="B31" t="s">
-        <v>210</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2231,10 +2231,10 @@
         <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I31" t="s">
         <v>81</v>
@@ -2243,7 +2243,7 @@
         <v>82</v>
       </c>
       <c r="K31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
         <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C32">
         <v>1990</v>
@@ -2263,7 +2263,7 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I32" t="s">
         <v>85</v>
@@ -2272,7 +2272,7 @@
         <v>84</v>
       </c>
       <c r="K32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2280,7 +2280,7 @@
         <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33">
         <v>2001</v>
@@ -2292,7 +2292,7 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>89</v>
+        <v>284</v>
       </c>
       <c r="I33" t="s">
         <v>88</v>
@@ -2301,236 +2301,236 @@
         <v>87</v>
       </c>
       <c r="K33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
         <v>91</v>
-      </c>
-      <c r="B34" t="s">
-        <v>92</v>
       </c>
       <c r="C34">
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E34">
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
       </c>
       <c r="I34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K34" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35">
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35">
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="I35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36">
         <v>1993</v>
       </c>
       <c r="D36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E36">
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
       </c>
       <c r="I36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" t="s">
         <v>98</v>
-      </c>
-      <c r="B37" t="s">
-        <v>99</v>
       </c>
       <c r="C37">
         <v>2002</v>
       </c>
       <c r="D37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E37">
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
       </c>
       <c r="I37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38">
         <v>2006</v>
       </c>
       <c r="D38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I38" t="s">
+        <v>102</v>
+      </c>
+      <c r="J38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="J38" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="K38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" t="s">
         <v>107</v>
-      </c>
-      <c r="B39" t="s">
-        <v>108</v>
       </c>
       <c r="C39">
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E39">
         <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" t="s">
         <v>109</v>
-      </c>
-      <c r="B40" t="s">
-        <v>110</v>
       </c>
       <c r="C40">
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E40">
         <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I40" t="s">
+        <v>110</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="K40" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C41">
         <v>2004</v>
@@ -2542,227 +2542,227 @@
         <v>37.630000000000003</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G41">
         <v>2731</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
         <v>121</v>
-      </c>
-      <c r="B42" t="s">
-        <v>122</v>
       </c>
       <c r="C42">
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C43">
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G43" s="1">
         <v>1543.018</v>
       </c>
       <c r="I43" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K43" t="s">
         <v>156</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="K43" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
         <v>159</v>
-      </c>
-      <c r="B44" t="s">
-        <v>160</v>
       </c>
       <c r="C44">
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E44">
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G44" s="1">
         <v>2004.07</v>
       </c>
       <c r="I44" t="s">
+        <v>161</v>
+      </c>
+      <c r="J44" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>163</v>
-      </c>
       <c r="K44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" t="s">
         <v>166</v>
-      </c>
-      <c r="B45" t="s">
-        <v>167</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K45" t="s">
         <v>164</v>
-      </c>
-      <c r="K45" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" t="s">
         <v>168</v>
-      </c>
-      <c r="B46" t="s">
-        <v>169</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E46">
         <v>50.49</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J46" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K46" t="s">
         <v>171</v>
-      </c>
-      <c r="K46" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" t="s">
         <v>174</v>
-      </c>
-      <c r="B47" t="s">
-        <v>175</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E47">
         <v>50.49</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J47" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K47" t="s">
         <v>171</v>
-      </c>
-      <c r="K47" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>261</v>
+      </c>
+      <c r="B48" t="s">
         <v>262</v>
-      </c>
-      <c r="B48" t="s">
-        <v>263</v>
       </c>
       <c r="C48">
         <v>1967</v>
@@ -2774,22 +2774,22 @@
         <v>16</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C49">
         <v>2003</v>
@@ -2801,21 +2801,21 @@
         <v>10</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I49" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>267</v>
+      </c>
+      <c r="B50" t="s">
         <v>268</v>
-      </c>
-      <c r="B50" t="s">
-        <v>269</v>
       </c>
       <c r="C50">
         <v>1957</v>
@@ -2827,21 +2827,21 @@
         <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>274</v>
+      </c>
+      <c r="B51" t="s">
         <v>275</v>
-      </c>
-      <c r="B51" t="s">
-        <v>276</v>
       </c>
       <c r="C51">
         <v>2017</v>
@@ -2853,21 +2853,21 @@
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I51" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>277</v>
+      </c>
+      <c r="B52" t="s">
         <v>278</v>
-      </c>
-      <c r="B52" t="s">
-        <v>279</v>
       </c>
       <c r="C52">
         <v>1978</v>
@@ -2879,13 +2879,13 @@
         <v>16</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed wrong year in citation
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -352,9 +352,6 @@
     <t>Relocation Assistance</t>
   </si>
   <si>
-    <t>Caliendo et al. (2011)</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/a/eee/pubeco/v148y2017icp136-151.html</t>
   </si>
   <si>
@@ -879,6 +876,9 @@
   </si>
   <si>
     <t>Bafög is a means-tested public German student loan program. Eligible students only have to pay back about 50% of the loan. In 2001, the threshold of parents' income above which students are no longer eligible for Bafög was lowered.</t>
+  </si>
+  <si>
+    <t>Caliendo et al. (2017)</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,13 +1286,13 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>283</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
@@ -1300,139 +1300,139 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
         <v>185</v>
-      </c>
-      <c r="B3" t="s">
-        <v>186</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>254</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
         <v>187</v>
-      </c>
-      <c r="B4" t="s">
-        <v>188</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>254</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B5" t="s">
         <v>189</v>
-      </c>
-      <c r="B5" t="s">
-        <v>190</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>254</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1452,17 +1452,17 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>45</v>
       </c>
       <c r="K6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1482,17 +1482,17 @@
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1512,7 +1512,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
@@ -1522,7 +1522,7 @@
         <v>47</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
@@ -1552,7 +1552,7 @@
         <v>49</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1566,26 +1566,26 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G10" s="1">
         <v>1672</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J10" t="s">
         <v>51</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1599,26 +1599,26 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="1">
         <v>1570</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J11" t="s">
         <v>51</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1632,26 +1632,26 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E12">
         <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G12" s="1">
         <v>1434</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J12" t="s">
         <v>51</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1665,26 +1665,26 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J13" t="s">
         <v>51</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1692,32 +1692,32 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C14">
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E14">
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G14" s="1">
         <v>1559.6189999999999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1731,26 +1731,26 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G15" s="1">
         <v>1542.066</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1758,19 +1758,19 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C16">
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
@@ -1783,7 +1783,7 @@
         <v>54</v>
       </c>
       <c r="K16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1797,13 +1797,13 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
@@ -1816,7 +1816,7 @@
         <v>54</v>
       </c>
       <c r="K17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -1824,31 +1824,31 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C18">
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
       </c>
       <c r="I18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -1862,25 +1862,25 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E19">
         <v>39.03</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G19" s="1">
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K19" t="s">
         <v>137</v>
-      </c>
-      <c r="K19" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1894,16 +1894,16 @@
         <v>2015</v>
       </c>
       <c r="D20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E20">
         <v>46.96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I20" t="s">
         <v>57</v>
@@ -1912,7 +1912,7 @@
         <v>56</v>
       </c>
       <c r="K20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="180" x14ac:dyDescent="0.25">
@@ -1926,16 +1926,16 @@
         <v>2015</v>
       </c>
       <c r="D21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E21">
         <v>46.96</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I21" t="s">
         <v>57</v>
@@ -1944,7 +1944,7 @@
         <v>56</v>
       </c>
       <c r="K21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -1958,13 +1958,13 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I22" t="s">
         <v>58</v>
@@ -1973,7 +1973,7 @@
         <v>59</v>
       </c>
       <c r="K22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
@@ -1987,13 +1987,13 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I23" t="s">
         <v>58</v>
@@ -2002,7 +2002,7 @@
         <v>59</v>
       </c>
       <c r="K23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -2016,13 +2016,13 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I24" t="s">
         <v>58</v>
@@ -2031,7 +2031,7 @@
         <v>59</v>
       </c>
       <c r="K24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2045,16 +2045,16 @@
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E25">
         <v>46.96</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I25" t="s">
         <v>60</v>
@@ -2063,7 +2063,7 @@
         <v>61</v>
       </c>
       <c r="K25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2077,13 +2077,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I26" t="s">
         <v>71</v>
@@ -2092,7 +2092,7 @@
         <v>72</v>
       </c>
       <c r="K26" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
@@ -2106,13 +2106,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I27" t="s">
         <v>71</v>
@@ -2121,7 +2121,7 @@
         <v>72</v>
       </c>
       <c r="K27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -2135,16 +2135,16 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E28">
         <v>28.1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I28" t="s">
         <v>71</v>
@@ -2153,7 +2153,7 @@
         <v>72</v>
       </c>
       <c r="K28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2167,13 +2167,13 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I29" t="s">
         <v>75</v>
@@ -2182,7 +2182,7 @@
         <v>76</v>
       </c>
       <c r="K29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2196,13 +2196,13 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
@@ -2214,15 +2214,15 @@
         <v>80</v>
       </c>
       <c r="K30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" t="s">
         <v>208</v>
-      </c>
-      <c r="B31" t="s">
-        <v>209</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2231,10 +2231,10 @@
         <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I31" t="s">
         <v>81</v>
@@ -2243,7 +2243,7 @@
         <v>82</v>
       </c>
       <c r="K31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
         <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C32">
         <v>1990</v>
@@ -2263,7 +2263,7 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I32" t="s">
         <v>85</v>
@@ -2272,7 +2272,7 @@
         <v>84</v>
       </c>
       <c r="K32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -2280,7 +2280,7 @@
         <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C33">
         <v>2001</v>
@@ -2292,7 +2292,7 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I33" t="s">
         <v>88</v>
@@ -2301,7 +2301,7 @@
         <v>87</v>
       </c>
       <c r="K33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -2315,13 +2315,13 @@
         <v>1993</v>
       </c>
       <c r="D34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E34">
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
@@ -2333,7 +2333,7 @@
         <v>89</v>
       </c>
       <c r="K34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -2347,13 +2347,13 @@
         <v>1993</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E35">
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
@@ -2365,7 +2365,7 @@
         <v>89</v>
       </c>
       <c r="K35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="135" x14ac:dyDescent="0.25">
@@ -2379,13 +2379,13 @@
         <v>1993</v>
       </c>
       <c r="D36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E36">
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
@@ -2397,7 +2397,7 @@
         <v>89</v>
       </c>
       <c r="K36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="120" x14ac:dyDescent="0.25">
@@ -2411,13 +2411,13 @@
         <v>2002</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E37">
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
@@ -2429,12 +2429,12 @@
         <v>99</v>
       </c>
       <c r="K37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
         <v>101</v>
@@ -2443,13 +2443,13 @@
         <v>2006</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I38" t="s">
         <v>102</v>
@@ -2458,7 +2458,7 @@
         <v>103</v>
       </c>
       <c r="K38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2472,13 +2472,13 @@
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E39">
         <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G39" s="1">
         <v>1593.2249999999999</v>
@@ -2490,7 +2490,7 @@
         <v>104</v>
       </c>
       <c r="K39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2504,33 +2504,33 @@
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E40">
         <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I40" t="s">
+        <v>284</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J40" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="K40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41">
         <v>2004</v>
@@ -2542,227 +2542,227 @@
         <v>37.630000000000003</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G41">
         <v>2731</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" t="s">
         <v>120</v>
-      </c>
-      <c r="B42" t="s">
-        <v>121</v>
       </c>
       <c r="C42">
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C43">
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G43" s="1">
         <v>1543.018</v>
       </c>
       <c r="I43" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K43" t="s">
         <v>155</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="K43" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>157</v>
+      </c>
+      <c r="B44" t="s">
         <v>158</v>
-      </c>
-      <c r="B44" t="s">
-        <v>159</v>
       </c>
       <c r="C44">
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E44">
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G44" s="1">
         <v>2004.07</v>
       </c>
       <c r="I44" t="s">
+        <v>160</v>
+      </c>
+      <c r="J44" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J44" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="K44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>164</v>
+      </c>
+      <c r="B45" t="s">
         <v>165</v>
-      </c>
-      <c r="B45" t="s">
-        <v>166</v>
       </c>
       <c r="C45">
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J45" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="K45" t="s">
         <v>163</v>
-      </c>
-      <c r="K45" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B46" t="s">
         <v>167</v>
-      </c>
-      <c r="B46" t="s">
-        <v>168</v>
       </c>
       <c r="C46">
         <v>2012</v>
       </c>
       <c r="D46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E46">
         <v>50.49</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J46" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K46" t="s">
         <v>170</v>
-      </c>
-      <c r="K46" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" t="s">
         <v>173</v>
-      </c>
-      <c r="B47" t="s">
-        <v>174</v>
       </c>
       <c r="C47">
         <v>2012</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E47">
         <v>50.49</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="J47" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K47" t="s">
         <v>170</v>
-      </c>
-      <c r="K47" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>260</v>
+      </c>
+      <c r="B48" t="s">
         <v>261</v>
-      </c>
-      <c r="B48" t="s">
-        <v>262</v>
       </c>
       <c r="C48">
         <v>1967</v>
@@ -2774,22 +2774,22 @@
         <v>16</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C49">
         <v>2003</v>
@@ -2801,21 +2801,21 @@
         <v>10</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I49" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>266</v>
+      </c>
+      <c r="B50" t="s">
         <v>267</v>
-      </c>
-      <c r="B50" t="s">
-        <v>268</v>
       </c>
       <c r="C50">
         <v>1957</v>
@@ -2827,21 +2827,21 @@
         <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>273</v>
+      </c>
+      <c r="B51" t="s">
         <v>274</v>
-      </c>
-      <c r="B51" t="s">
-        <v>275</v>
       </c>
       <c r="C51">
         <v>2017</v>
@@ -2853,21 +2853,21 @@
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I51" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>276</v>
+      </c>
+      <c r="B52" t="s">
         <v>277</v>
-      </c>
-      <c r="B52" t="s">
-        <v>278</v>
       </c>
       <c r="C52">
         <v>1978</v>
@@ -2879,13 +2879,13 @@
         <v>16</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
*added Bildungsgutscheine *fixed wrong year in citation
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -560,9 +560,6 @@
     <t>Caliendo et al. (2016)</t>
   </si>
   <si>
-    <t>Doerr et al. (2014);Huber et al. (2015)</t>
-  </si>
-  <si>
     <t>One Euro Jobs "Ein Euro Jobs" are jobs which are assigned to long term unemployed to help them reintegrate into the labor market. These jobs are meant to be unpaid. However, the participants receive a compensation of at least one euro per hour worked.</t>
   </si>
   <si>
@@ -879,6 +876,9 @@
   </si>
   <si>
     <t>Caliendo et al. (2017)</t>
+  </si>
+  <si>
+    <t>Doerr et al. (2017);Huber et al. (2015)</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,10 +1286,10 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>126</v>
@@ -1300,25 +1300,25 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2">
         <v>1990</v>
       </c>
       <c r="D2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E2">
         <v>48.480624773955284</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>44</v>
@@ -1332,107 +1332,107 @@
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" t="s">
         <v>184</v>
-      </c>
-      <c r="B3" t="s">
-        <v>185</v>
       </c>
       <c r="C3">
         <v>2001</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E3">
         <v>48.922446097261144</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" t="s">
         <v>186</v>
-      </c>
-      <c r="B4" t="s">
-        <v>187</v>
       </c>
       <c r="C4">
         <v>2004</v>
       </c>
       <c r="D4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E4">
         <v>50.583095918192996</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" t="s">
         <v>188</v>
-      </c>
-      <c r="B5" t="s">
-        <v>189</v>
       </c>
       <c r="C5">
         <v>2005</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E5">
         <v>50.583095918192996</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>253</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -1452,7 +1452,7 @@
         <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
@@ -1482,7 +1482,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
@@ -1512,7 +1512,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
@@ -1542,7 +1542,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" t="s">
@@ -1566,13 +1566,13 @@
         <v>1993</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E10">
         <v>35.200000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G10" s="1">
         <v>1672</v>
@@ -1599,13 +1599,13 @@
         <v>1993</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11">
         <v>34.799999999999997</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G11" s="1">
         <v>1570</v>
@@ -1632,13 +1632,13 @@
         <v>1993</v>
       </c>
       <c r="D12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E12">
         <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G12" s="1">
         <v>1434</v>
@@ -1665,13 +1665,13 @@
         <v>1993</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E13">
         <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G13" s="1">
         <v>1558</v>
@@ -1692,19 +1692,19 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C14">
         <v>2000</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E14">
         <v>37</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G14" s="1">
         <v>1559.6189999999999</v>
@@ -1731,13 +1731,13 @@
         <v>2000</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E15">
         <v>37</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G15" s="1">
         <v>1542.066</v>
@@ -1758,19 +1758,19 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C16">
         <v>2003</v>
       </c>
       <c r="D16" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E16">
         <v>38.86</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G16" s="1">
         <v>1459.3779999999999</v>
@@ -1797,13 +1797,13 @@
         <v>2003</v>
       </c>
       <c r="D17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E17">
         <v>40.17</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G17" s="1">
         <v>2189.3620000000001</v>
@@ -1824,19 +1824,19 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C18">
         <v>2009</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E18">
         <v>40.969000000000001</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G18" s="1">
         <v>2047.962</v>
@@ -1862,19 +1862,19 @@
         <v>2003</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E19">
         <v>39.03</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G19" s="1">
         <v>1901.21</v>
       </c>
       <c r="I19" t="s">
-        <v>179</v>
+        <v>284</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>136</v>
@@ -1900,10 +1900,10 @@
         <v>46.96</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I20" t="s">
         <v>57</v>
@@ -1932,10 +1932,10 @@
         <v>46.96</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I21" t="s">
         <v>57</v>
@@ -1958,13 +1958,13 @@
         <v>2005</v>
       </c>
       <c r="D22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E22">
         <v>39.64795218424306</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I22" t="s">
         <v>58</v>
@@ -1987,13 +1987,13 @@
         <v>2005</v>
       </c>
       <c r="D23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I23" t="s">
         <v>58</v>
@@ -2016,13 +2016,13 @@
         <v>2005</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I24" t="s">
         <v>58</v>
@@ -2045,16 +2045,16 @@
         <v>2012</v>
       </c>
       <c r="D25" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E25">
         <v>46.96</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I25" t="s">
         <v>60</v>
@@ -2077,13 +2077,13 @@
         <v>1979</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H26" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I26" t="s">
         <v>71</v>
@@ -2106,13 +2106,13 @@
         <v>1986</v>
       </c>
       <c r="D27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I27" t="s">
         <v>71</v>
@@ -2135,16 +2135,16 @@
         <v>1992</v>
       </c>
       <c r="D28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E28">
         <v>28.1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I28" t="s">
         <v>71</v>
@@ -2167,13 +2167,13 @@
         <v>2013</v>
       </c>
       <c r="D29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E29">
         <v>31.36</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I29" t="s">
         <v>75</v>
@@ -2196,13 +2196,13 @@
         <v>2007</v>
       </c>
       <c r="D30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E30">
         <v>29.768270000000001</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G30" s="1">
         <v>2235.6489999999999</v>
@@ -2219,10 +2219,10 @@
     </row>
     <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" t="s">
         <v>207</v>
-      </c>
-      <c r="B31" t="s">
-        <v>208</v>
       </c>
       <c r="C31">
         <v>2020</v>
@@ -2231,10 +2231,10 @@
         <v>67</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I31" t="s">
         <v>81</v>
@@ -2263,7 +2263,7 @@
         <v>19.809999999999999</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I32" t="s">
         <v>85</v>
@@ -2292,7 +2292,7 @@
         <v>19.420999999999999</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I33" t="s">
         <v>88</v>
@@ -2321,7 +2321,7 @@
         <v>42</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G34" s="1">
         <v>1934.5</v>
@@ -2353,7 +2353,7 @@
         <v>44</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G35" s="1">
         <v>1928.4169999999999</v>
@@ -2385,7 +2385,7 @@
         <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G36" s="1">
         <v>1925.375</v>
@@ -2417,7 +2417,7 @@
         <v>45</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G37" s="1">
         <v>1999.866</v>
@@ -2449,7 +2449,7 @@
         <v>50.492400000000004</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I38" t="s">
         <v>102</v>
@@ -2472,13 +2472,13 @@
         <v>2011</v>
       </c>
       <c r="D39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E39">
         <v>36.92</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G39" s="1">
         <v>1593.2249999999999</v>
@@ -2504,19 +2504,19 @@
         <v>2006</v>
       </c>
       <c r="D40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E40">
         <v>37.71</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="I40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>110</v>
@@ -2542,7 +2542,7 @@
         <v>37.630000000000003</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G41">
         <v>2731</v>
@@ -2568,13 +2568,13 @@
         <v>2001</v>
       </c>
       <c r="D42" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E42">
         <v>39.612000000000002</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G42" s="1">
         <v>1278.2249999999999</v>
@@ -2600,13 +2600,13 @@
         <v>2009</v>
       </c>
       <c r="D43" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E43">
         <v>50.181100000000001</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G43" s="1">
         <v>1543.018</v>
@@ -2632,13 +2632,13 @@
         <v>2005</v>
       </c>
       <c r="D44" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E44">
         <v>27</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G44" s="1">
         <v>2004.07</v>
@@ -2664,19 +2664,19 @@
         <v>2012</v>
       </c>
       <c r="D45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E45">
         <v>44.531999999999996</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>162</v>
@@ -2702,14 +2702,14 @@
         <v>50.49</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I46" t="s">
         <v>171</v>
@@ -2738,14 +2738,14 @@
         <v>50.49</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I47" t="s">
         <v>171</v>
@@ -2759,10 +2759,10 @@
     </row>
     <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>259</v>
+      </c>
+      <c r="B48" t="s">
         <v>260</v>
-      </c>
-      <c r="B48" t="s">
-        <v>261</v>
       </c>
       <c r="C48">
         <v>1967</v>
@@ -2774,22 +2774,22 @@
         <v>16</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H48" s="1"/>
       <c r="I48" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C49">
         <v>2003</v>
@@ -2801,21 +2801,21 @@
         <v>10</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I49" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>265</v>
+      </c>
+      <c r="B50" t="s">
         <v>266</v>
-      </c>
-      <c r="B50" t="s">
-        <v>267</v>
       </c>
       <c r="C50">
         <v>1957</v>
@@ -2827,21 +2827,21 @@
         <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>272</v>
+      </c>
+      <c r="B51" t="s">
         <v>273</v>
-      </c>
-      <c r="B51" t="s">
-        <v>274</v>
       </c>
       <c r="C51">
         <v>2017</v>
@@ -2853,21 +2853,21 @@
         <v>14</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>275</v>
+      </c>
+      <c r="B52" t="s">
         <v>276</v>
-      </c>
-      <c r="B52" t="s">
-        <v>277</v>
       </c>
       <c r="C52">
         <v>1978</v>
@@ -2879,13 +2879,13 @@
         <v>16</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added German reform names to programs.xlsx
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="332">
   <si>
     <t>program_identifier</t>
   </si>
@@ -879,13 +879,154 @@
   </si>
   <si>
     <t>Doerr et al. (2017);Huber et al. (2015)</t>
+  </si>
+  <si>
+    <t>program_name_de</t>
+  </si>
+  <si>
+    <t>Einkommenssteuerreform 1990</t>
+  </si>
+  <si>
+    <t>Einkommenssteuerreform 2001</t>
+  </si>
+  <si>
+    <t>Einkommenssteuerreform 2004</t>
+  </si>
+  <si>
+    <t>Einkommenssteuerreform 2005</t>
+  </si>
+  <si>
+    <t>Elterngeld</t>
+  </si>
+  <si>
+    <t>Betreuungsgeld</t>
+  </si>
+  <si>
+    <t>Mutterschaftsurlaubsgeld (1979)</t>
+  </si>
+  <si>
+    <t>Erziehungsgeld (1986)</t>
+  </si>
+  <si>
+    <t>Kündigungsschutzausweitung für Mütter (1992)</t>
+  </si>
+  <si>
+    <t>EEG Windstrom</t>
+  </si>
+  <si>
+    <t>EEG Solarstrom</t>
+  </si>
+  <si>
+    <t>Informationsbroschüre über Chancen am Arbeitsmarkt</t>
+  </si>
+  <si>
+    <t>Renteninformationsschreiben</t>
+  </si>
+  <si>
+    <t>Umzugskostenübernahme</t>
+  </si>
+  <si>
+    <t>Dezentralisierung von Jobcentern</t>
+  </si>
+  <si>
+    <t>Inhouse Stellenvermittlung</t>
+  </si>
+  <si>
+    <t>Überbrückungsgeld</t>
+  </si>
+  <si>
+    <t>Gründungszuschuss</t>
+  </si>
+  <si>
+    <t>Existenzgründungszuschuss</t>
+  </si>
+  <si>
+    <t>Lohnzuschuss</t>
+  </si>
+  <si>
+    <t>Arbeitsgelegenheiten</t>
+  </si>
+  <si>
+    <t>Ein-Euro-Jobs</t>
+  </si>
+  <si>
+    <t>Arbeitsbeschaffungsmaßnahmen</t>
+  </si>
+  <si>
+    <t>Arbeislosenversicherung (42 Jahre)</t>
+  </si>
+  <si>
+    <t>Arbeislosenversicherung (44 Jahre)</t>
+  </si>
+  <si>
+    <t>Arbeislosenversicherung (45 Jahre)</t>
+  </si>
+  <si>
+    <t>Arbeislosenversicherung (49 Jahre)</t>
+  </si>
+  <si>
+    <t>Bafög Reform 1990</t>
+  </si>
+  <si>
+    <t>Arbeislosenversicherungsreform 2006</t>
+  </si>
+  <si>
+    <t>Realschulabschluss mit Beendigung 10. Klasse Gymnasium</t>
+  </si>
+  <si>
+    <t>Verlängerung Hauptschule/Mittelschule um 1 Jahr</t>
+  </si>
+  <si>
+    <t>Studiengebühren</t>
+  </si>
+  <si>
+    <t>Abschaffung Schulgebühren</t>
+  </si>
+  <si>
+    <t>Informations-Workshop zum Thema Studium</t>
+  </si>
+  <si>
+    <t>Mentoring Programm "Rock your Life"</t>
+  </si>
+  <si>
+    <t>Mentoring Programm "Balu und Du"</t>
+  </si>
+  <si>
+    <t>G8 Reform</t>
+  </si>
+  <si>
+    <t>Trainingsmaßnahmen</t>
+  </si>
+  <si>
+    <t>Berufliche Weiterbildung</t>
+  </si>
+  <si>
+    <t>Bildungsgutscheine</t>
+  </si>
+  <si>
+    <t>Kurze Trainingsprogramme</t>
+  </si>
+  <si>
+    <t>Lange Trainingsprogramme</t>
+  </si>
+  <si>
+    <t>Berufliche Neuausrichtung</t>
+  </si>
+  <si>
+    <t>Übungsfirma</t>
+  </si>
+  <si>
+    <t>Aufteilung Realschule/Hauptschule ab 4. Klasse</t>
+  </si>
+  <si>
+    <t>what_works_included</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -921,6 +1062,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF9876AA"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -943,7 +1091,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -957,6 +1105,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1239,28 +1390,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="54.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
-    <col min="5" max="5" width="66.85546875" customWidth="1"/>
-    <col min="6" max="6" width="46.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="45.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="2" max="3" width="47" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="66.85546875" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="45.140625" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1268,1661 +1419,1959 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>285</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="150">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>189</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2">
         <v>1990</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>199</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>48.480624773955284</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>8868.6350000000002</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="60">
       <c r="A3" t="s">
         <v>183</v>
       </c>
       <c r="B3" t="s">
         <v>184</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3">
         <v>2001</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>199</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>48.922446097261144</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>9056.3310000000001</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="60">
       <c r="A4" t="s">
         <v>185</v>
       </c>
       <c r="B4" t="s">
         <v>186</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4">
         <v>2004</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>199</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>50.583095918192996</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>8886.7603079578239</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="75">
       <c r="A5" t="s">
         <v>187</v>
       </c>
       <c r="B5" t="s">
         <v>188</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5">
         <v>2005</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>199</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>50.583095918192996</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>9022.8359999999993</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>252</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="75">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D6">
         <v>2013</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" t="s">
+      <c r="I6" s="1"/>
+      <c r="J6" t="s">
         <v>174</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="105">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D7">
         <v>2011</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>10</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="75">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8">
         <v>2011</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>18</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" t="s">
+      <c r="I8" s="1"/>
+      <c r="J8" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>317</v>
+      </c>
+      <c r="D9">
         <v>2008</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>21</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="H9" s="1"/>
-      <c r="I9" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" t="s">
         <v>50</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="30">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10">
         <v>1993</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>200</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>35.200000000000003</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>1672</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="I10" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" t="s">
         <v>176</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>326</v>
+      </c>
+      <c r="D11">
         <v>1993</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>200</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>34.799999999999997</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>1570</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" t="s">
+      <c r="I11" s="1"/>
+      <c r="J11" t="s">
         <v>176</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>329</v>
+      </c>
+      <c r="D12">
         <v>1993</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>200</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>36</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>240</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>1434</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" t="s">
         <v>176</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>328</v>
+      </c>
+      <c r="D13">
         <v>1993</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>200</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>31</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>1558</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" t="s">
         <v>176</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="30">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>253</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>324</v>
+      </c>
+      <c r="D14">
         <v>2000</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>200</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>37</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>1559.6189999999999</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" t="s">
+      <c r="I14" s="1"/>
+      <c r="J14" t="s">
         <v>177</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="60">
       <c r="A15" t="s">
         <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>323</v>
+      </c>
+      <c r="D15">
         <v>2000</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>200</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>37</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>1542.066</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" t="s">
+      <c r="I15" s="1"/>
+      <c r="J15" t="s">
         <v>177</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="60">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>224</v>
       </c>
-      <c r="C16">
+      <c r="C16" t="s">
+        <v>304</v>
+      </c>
+      <c r="D16">
         <v>2003</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>224</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>38.86</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>1459.3779999999999</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" t="s">
+      <c r="I16" s="1"/>
+      <c r="J16" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="90">
       <c r="A17" t="s">
         <v>28</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C17">
+      <c r="C17" t="s">
+        <v>302</v>
+      </c>
+      <c r="D17">
         <v>2003</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>224</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>40.17</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>2189.3620000000001</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" t="s">
+      <c r="I17" s="1"/>
+      <c r="J17" t="s">
         <v>53</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="105">
       <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" t="s">
         <v>225</v>
       </c>
-      <c r="C18">
+      <c r="C18" t="s">
+        <v>303</v>
+      </c>
+      <c r="D18">
         <v>2009</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>224</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>40.969000000000001</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>2047.962</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>178</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="60">
       <c r="A19" t="s">
         <v>32</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="C19">
+      <c r="C19" t="s">
+        <v>325</v>
+      </c>
+      <c r="D19">
         <v>2003</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>200</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>39.03</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>1901.21</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>284</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="180">
       <c r="A20" t="s">
         <v>34</v>
       </c>
       <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>2015</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>168</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>46.96</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>57</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="K20" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="180">
       <c r="A21" t="s">
         <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>2015</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>168</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>46.96</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>57</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="K21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="120">
       <c r="A22" t="s">
         <v>40</v>
       </c>
       <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C22">
+      <c r="C22" t="s">
+        <v>308</v>
+      </c>
+      <c r="D22">
         <v>2005</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>201</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>39.64795218424306</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>58</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="90">
       <c r="A23" t="s">
         <v>39</v>
       </c>
       <c r="B23" t="s">
         <v>41</v>
       </c>
-      <c r="C23">
+      <c r="C23" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23">
         <v>2005</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>201</v>
       </c>
-      <c r="E23" s="4">
+      <c r="F23" s="4">
         <v>38.264488399999998</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="105">
       <c r="A24" t="s">
         <v>42</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
-      <c r="C24">
+      <c r="C24" t="s">
+        <v>306</v>
+      </c>
+      <c r="D24">
         <v>2005</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>201</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>34.553800649999999</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="60">
       <c r="A25" t="s">
         <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>63</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>2012</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>182</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>46.96</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>198</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="120">
       <c r="A26" t="s">
         <v>64</v>
       </c>
       <c r="B26" t="s">
         <v>68</v>
       </c>
-      <c r="C26">
+      <c r="C26" t="s">
+        <v>292</v>
+      </c>
+      <c r="D26">
         <v>1979</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>204</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="G26" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>191</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="150">
       <c r="A27" t="s">
         <v>65</v>
       </c>
       <c r="B27" t="s">
         <v>69</v>
       </c>
-      <c r="C27">
+      <c r="C27" t="s">
+        <v>293</v>
+      </c>
+      <c r="D27">
         <v>1986</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>204</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="G27" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>191</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="135">
       <c r="A28" t="s">
         <v>66</v>
       </c>
       <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="C28">
+      <c r="C28" t="s">
+        <v>294</v>
+      </c>
+      <c r="D28">
         <v>1992</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>204</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>28.1</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>71</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="60">
       <c r="A29" t="s">
         <v>73</v>
       </c>
       <c r="B29" t="s">
         <v>74</v>
       </c>
-      <c r="C29">
+      <c r="C29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D29">
         <v>2013</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>204</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>31.36</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>75</v>
       </c>
-      <c r="J29" s="2" t="s">
+      <c r="K29" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="K29" t="s">
+      <c r="L29" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="120">
       <c r="A30" t="s">
         <v>77</v>
       </c>
       <c r="B30" t="s">
         <v>78</v>
       </c>
-      <c r="C30">
+      <c r="C30" t="s">
+        <v>290</v>
+      </c>
+      <c r="D30">
         <v>2007</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>204</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>29.768270000000001</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="G30" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>2235.6489999999999</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>79</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="K30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K30" t="s">
+      <c r="L30" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="120">
       <c r="A31" t="s">
         <v>206</v>
       </c>
       <c r="B31" t="s">
         <v>207</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>2020</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>67</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>81</v>
       </c>
-      <c r="J31" s="2" t="s">
+      <c r="K31" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K31" t="s">
+      <c r="L31" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="75">
       <c r="A32" t="s">
         <v>83</v>
       </c>
       <c r="B32" t="s">
         <v>156</v>
       </c>
-      <c r="C32">
+      <c r="C32" t="s">
+        <v>313</v>
+      </c>
+      <c r="D32">
         <v>1990</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>13</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>19.809999999999999</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>85</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="K32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="K32" t="s">
+      <c r="L32" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="75">
       <c r="A33" t="s">
         <v>86</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
       </c>
-      <c r="C33">
+      <c r="C33" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33">
         <v>2001</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>13</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>19.420999999999999</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>88</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="135">
       <c r="A34" t="s">
         <v>90</v>
       </c>
       <c r="B34" t="s">
         <v>91</v>
       </c>
-      <c r="C34">
+      <c r="C34" t="s">
+        <v>309</v>
+      </c>
+      <c r="D34">
         <v>1993</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>114</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>42</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="G34" s="1">
+      <c r="H34" s="1">
         <v>1934.5</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>92</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K34" t="s">
+      <c r="L34" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="135">
       <c r="A35" t="s">
         <v>95</v>
       </c>
       <c r="B35" t="s">
         <v>93</v>
       </c>
-      <c r="C35">
+      <c r="C35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D35">
         <v>1993</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>114</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>44</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="G35" s="1">
+      <c r="H35" s="1">
         <v>1928.4169999999999</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>92</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K35" t="s">
+      <c r="L35" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="135">
       <c r="A36" t="s">
         <v>96</v>
       </c>
       <c r="B36" t="s">
         <v>94</v>
       </c>
-      <c r="C36">
+      <c r="C36" t="s">
+        <v>312</v>
+      </c>
+      <c r="D36">
         <v>1993</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>114</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>42</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="G36" s="1">
+      <c r="H36" s="1">
         <v>1925.375</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>92</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="K36" t="s">
+      <c r="L36" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="120" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="120">
       <c r="A37" t="s">
         <v>97</v>
       </c>
       <c r="B37" t="s">
         <v>98</v>
       </c>
-      <c r="C37">
+      <c r="C37" t="s">
+        <v>311</v>
+      </c>
+      <c r="D37">
         <v>2002</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>114</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>45</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="G37" s="1">
+      <c r="H37" s="1">
         <v>1999.866</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>100</v>
       </c>
-      <c r="J37" s="2" t="s">
+      <c r="K37" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K37" t="s">
+      <c r="L37" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="135">
       <c r="A38" t="s">
         <v>116</v>
       </c>
       <c r="B38" t="s">
         <v>101</v>
       </c>
-      <c r="C38">
+      <c r="C38" t="s">
+        <v>314</v>
+      </c>
+      <c r="D38">
         <v>2006</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="1">
+      <c r="F38" s="1">
         <v>50.492400000000004</v>
       </c>
-      <c r="F38" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>102</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K38" t="s">
+      <c r="L38" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="60">
       <c r="A39" t="s">
         <v>106</v>
       </c>
       <c r="B39" t="s">
         <v>107</v>
       </c>
-      <c r="C39">
+      <c r="C39" t="s">
+        <v>297</v>
+      </c>
+      <c r="D39">
         <v>2011</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>202</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>36.92</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G39" s="1">
+      <c r="H39" s="1">
         <v>1593.2249999999999</v>
       </c>
-      <c r="I39" s="4" t="s">
+      <c r="J39" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K39" t="s">
+      <c r="L39" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="60">
       <c r="A40" t="s">
         <v>108</v>
       </c>
       <c r="B40" t="s">
         <v>109</v>
       </c>
-      <c r="C40">
+      <c r="C40" t="s">
+        <v>299</v>
+      </c>
+      <c r="D40">
         <v>2006</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>202</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>37.71</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="G40" s="1">
+      <c r="H40" s="1">
         <v>2624.9580000000001</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>283</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="K40" t="s">
+      <c r="L40" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="90">
       <c r="A41" t="s">
         <v>115</v>
       </c>
       <c r="B41" t="s">
         <v>113</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="8"/>
+      <c r="D41">
         <v>2004</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>67</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>37.630000000000003</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>2731</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="J41" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="K41" t="s">
+      <c r="L41" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="195" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="195">
       <c r="A42" t="s">
         <v>119</v>
       </c>
       <c r="B42" t="s">
         <v>120</v>
       </c>
-      <c r="C42">
+      <c r="C42" t="s">
+        <v>305</v>
+      </c>
+      <c r="D42">
         <v>2001</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>201</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>39.612000000000002</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="G42" s="1">
+      <c r="H42" s="1">
         <v>1278.2249999999999</v>
       </c>
-      <c r="I42" s="6" t="s">
+      <c r="J42" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="90">
       <c r="A43" t="s">
         <v>123</v>
       </c>
       <c r="B43" t="s">
         <v>122</v>
       </c>
-      <c r="C43">
+      <c r="C43" t="s">
+        <v>301</v>
+      </c>
+      <c r="D43">
         <v>2009</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>202</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>50.181100000000001</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="G43" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="G43" s="1">
+      <c r="H43" s="1">
         <v>1543.018</v>
       </c>
-      <c r="I43" s="4" t="s">
+      <c r="J43" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="150">
       <c r="A44" t="s">
         <v>157</v>
       </c>
       <c r="B44" t="s">
         <v>158</v>
       </c>
-      <c r="C44">
+      <c r="C44" t="s">
+        <v>298</v>
+      </c>
+      <c r="D44">
         <v>2005</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>202</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>27</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="G44" s="1">
+      <c r="H44" s="1">
         <v>2004.07</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>160</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="K44" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="105">
       <c r="A45" t="s">
         <v>164</v>
       </c>
       <c r="B45" t="s">
         <v>165</v>
       </c>
-      <c r="C45">
+      <c r="C45" t="s">
+        <v>300</v>
+      </c>
+      <c r="D45">
         <v>2012</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>202</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>44.531999999999996</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="G45" s="1">
+      <c r="H45" s="1">
         <v>994.59460000000001</v>
       </c>
-      <c r="I45" s="4" t="s">
+      <c r="J45" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="K45" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="135">
       <c r="A46" t="s">
         <v>166</v>
       </c>
       <c r="B46" t="s">
         <v>167</v>
       </c>
-      <c r="C46">
+      <c r="C46" t="s">
+        <v>295</v>
+      </c>
+      <c r="D46">
         <v>2012</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>168</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>50.49</v>
       </c>
-      <c r="F46" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="G46" s="1">
+      <c r="H46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>171</v>
       </c>
-      <c r="J46" s="2" t="s">
+      <c r="K46" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="K46" t="s">
+      <c r="L46" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="135">
       <c r="A47" t="s">
         <v>172</v>
       </c>
       <c r="B47" t="s">
         <v>173</v>
       </c>
-      <c r="C47">
+      <c r="C47" t="s">
+        <v>296</v>
+      </c>
+      <c r="D47">
         <v>2012</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>168</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>50.49</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G47" s="1">
+      <c r="H47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>171</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="K47" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="K47" t="s">
+      <c r="L47" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="105">
       <c r="A48" t="s">
         <v>259</v>
       </c>
       <c r="B48" t="s">
         <v>260</v>
       </c>
-      <c r="C48">
+      <c r="C48" t="s">
+        <v>316</v>
+      </c>
+      <c r="D48">
         <v>1967</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>13</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>16</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="H48" s="1"/>
-      <c r="I48" t="s">
+      <c r="I48" s="1"/>
+      <c r="J48" t="s">
         <v>257</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="K48" s="2" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="120">
       <c r="A49" t="s">
         <v>264</v>
       </c>
       <c r="B49" t="s">
         <v>263</v>
       </c>
-      <c r="C49">
+      <c r="C49" t="s">
+        <v>330</v>
+      </c>
+      <c r="D49">
         <v>2003</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>13</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>10</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>257</v>
       </c>
-      <c r="J49" s="2" t="s">
+      <c r="K49" s="2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="75">
       <c r="A50" t="s">
         <v>265</v>
       </c>
       <c r="B50" t="s">
         <v>266</v>
       </c>
-      <c r="C50">
+      <c r="C50" t="s">
+        <v>318</v>
+      </c>
+      <c r="D50">
         <v>1957</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>13</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>10</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="G50" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="J50" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="J50" s="2" t="s">
+      <c r="K50" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="105">
       <c r="A51" t="s">
         <v>272</v>
       </c>
       <c r="B51" t="s">
         <v>273</v>
       </c>
-      <c r="C51">
+      <c r="C51" t="s">
+        <v>320</v>
+      </c>
+      <c r="D51">
         <v>2017</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>13</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>14</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>271</v>
       </c>
-      <c r="J51" s="2" t="s">
+      <c r="K51" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="135">
       <c r="A52" t="s">
         <v>275</v>
       </c>
       <c r="B52" t="s">
         <v>276</v>
       </c>
-      <c r="C52">
+      <c r="C52" t="s">
+        <v>315</v>
+      </c>
+      <c r="D52">
         <v>1978</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>13</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>16</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="J52" s="2" t="s">
+      <c r="K52" s="2" t="s">
         <v>277</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J6" r:id="rId2"/>
-    <hyperlink ref="J7" r:id="rId3"/>
-    <hyperlink ref="J9" r:id="rId4"/>
-    <hyperlink ref="J8" r:id="rId5"/>
-    <hyperlink ref="J14" r:id="rId6"/>
-    <hyperlink ref="J15" r:id="rId7"/>
-    <hyperlink ref="J18" r:id="rId8"/>
-    <hyperlink ref="J19" r:id="rId9"/>
-    <hyperlink ref="J20" r:id="rId10"/>
-    <hyperlink ref="J21" r:id="rId11"/>
-    <hyperlink ref="J22" r:id="rId12"/>
-    <hyperlink ref="J23" r:id="rId13"/>
-    <hyperlink ref="J24" r:id="rId14"/>
-    <hyperlink ref="J25" r:id="rId15"/>
-    <hyperlink ref="J28" r:id="rId16"/>
-    <hyperlink ref="J27" r:id="rId17"/>
-    <hyperlink ref="J26" r:id="rId18"/>
-    <hyperlink ref="J29" r:id="rId19"/>
-    <hyperlink ref="J30" r:id="rId20"/>
-    <hyperlink ref="J5" r:id="rId21"/>
-    <hyperlink ref="J31" r:id="rId22" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="J32" r:id="rId23" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
-    <hyperlink ref="J33" r:id="rId24" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="J34" r:id="rId25"/>
-    <hyperlink ref="J37" r:id="rId26"/>
-    <hyperlink ref="J4" r:id="rId27"/>
-    <hyperlink ref="J3" r:id="rId28"/>
-    <hyperlink ref="J48" r:id="rId29"/>
-    <hyperlink ref="J49" r:id="rId30"/>
-    <hyperlink ref="J50" r:id="rId31"/>
-    <hyperlink ref="J51" r:id="rId32"/>
-    <hyperlink ref="J52" r:id="rId33"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K6" r:id="rId2"/>
+    <hyperlink ref="K7" r:id="rId3"/>
+    <hyperlink ref="K9" r:id="rId4"/>
+    <hyperlink ref="K8" r:id="rId5"/>
+    <hyperlink ref="K14" r:id="rId6"/>
+    <hyperlink ref="K15" r:id="rId7"/>
+    <hyperlink ref="K18" r:id="rId8"/>
+    <hyperlink ref="K19" r:id="rId9"/>
+    <hyperlink ref="K20" r:id="rId10"/>
+    <hyperlink ref="K21" r:id="rId11"/>
+    <hyperlink ref="K22" r:id="rId12"/>
+    <hyperlink ref="K23" r:id="rId13"/>
+    <hyperlink ref="K24" r:id="rId14"/>
+    <hyperlink ref="K25" r:id="rId15"/>
+    <hyperlink ref="K28" r:id="rId16"/>
+    <hyperlink ref="K27" r:id="rId17"/>
+    <hyperlink ref="K26" r:id="rId18"/>
+    <hyperlink ref="K29" r:id="rId19"/>
+    <hyperlink ref="K30" r:id="rId20"/>
+    <hyperlink ref="K5" r:id="rId21"/>
+    <hyperlink ref="K31" r:id="rId22" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="K32" r:id="rId23" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
+    <hyperlink ref="K33" r:id="rId24" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="K34" r:id="rId25"/>
+    <hyperlink ref="K37" r:id="rId26"/>
+    <hyperlink ref="K4" r:id="rId27"/>
+    <hyperlink ref="K3" r:id="rId28"/>
+    <hyperlink ref="K48" r:id="rId29"/>
+    <hyperlink ref="K49" r:id="rId30"/>
+    <hyperlink ref="K50" r:id="rId31"/>
+    <hyperlink ref="K51" r:id="rId32"/>
+    <hyperlink ref="K52" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>

</xml_diff>

<commit_message>
* added columns maryland scale, peer review and comment column to programs.xlsx * added option to reference bibtex entries in javascript by adding a script which convert bibTex to JSON
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="393">
   <si>
     <t>program_identifier</t>
   </si>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>Marcus &amp; Zambre (2019)</t>
-  </si>
-  <si>
-    <t>https://ideas.repec.org/p/arx/papers/1909.08299.html;https://ideas.repec.org/a/eee/ecoedu/v41y2014icp14-23.html</t>
-  </si>
-  <si>
-    <t>Gorgen &amp; Schienle (2019);Bruckmeier &amp; Wigger (2014)</t>
   </si>
   <si>
     <t>https://ideas.repec.org/a/bla/jeurec/v9y2011i4p742-784.html</t>
@@ -425,9 +419,6 @@
     <t>caliendo2016</t>
   </si>
   <si>
-    <t>gorgen2019;bruckmeier2014</t>
-  </si>
-  <si>
     <t>hohmeyer2010</t>
   </si>
   <si>
@@ -447,9 +438,6 @@
   </si>
   <si>
     <t>collischon2020</t>
-  </si>
-  <si>
-    <t>kluve2013;frodermann2020</t>
   </si>
   <si>
     <t>dorn2020</t>
@@ -739,9 +727,6 @@
     <t>Government sponsored short-term training programs "Trainingsmaßnahmen", which were introduced again in 1998 after being abolished in 1993.</t>
   </si>
   <si>
-    <t>Government sponsored training to obtain a new professional degree in a field other than the profession currently held.</t>
-  </si>
-  <si>
     <t>Elementary school students who come from families with low socio-economic status  were assigned a mentor. The mentors should encourage the acquisition of new ideas and skills. Falk et al. (2020) find positive effects on children's  long-term educational trajectories. A higher share of students attends the academic high school track.</t>
   </si>
   <si>
@@ -797,9 +782,6 @@
     <t>https://ideas.repec.org/a/bla/scandj/v116y2014i3p878-907.html</t>
   </si>
   <si>
-    <t>Piopiunik (2014)</t>
-  </si>
-  <si>
     <t>Between 1946 and 1969 all German federal states extended the length of the least academic school track "Hauptschule" in Germany by one year. Piopiunik (2014) finds that this reform improved educational outcomes of sons whose mothers were affected by the compulsary schooling reform.</t>
   </si>
   <si>
@@ -809,9 +791,6 @@
     <t>Compulsary Schooling</t>
   </si>
   <si>
-    <t>https://ideas.repec.org/p/ces/ifowps/_153.html</t>
-  </si>
-  <si>
     <t>In 2000, the Bavarian parliament passed a reform that started tracking (i.e. students attending different levels of secondary education) in 4th instead of 6th grade. The reform only affected the basic and middle track (Hauptschule and Realschule). Piopiunik (2014) finds that the earlier tracking reduces PISA test scores by 13 points on average.</t>
   </si>
   <si>
@@ -1020,6 +999,227 @@
   </si>
   <si>
     <t>what_works_included</t>
+  </si>
+  <si>
+    <t>identification</t>
+  </si>
+  <si>
+    <t>maryland_scale</t>
+  </si>
+  <si>
+    <t>indentification_comments</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>peer_reviewed</t>
+  </si>
+  <si>
+    <t>RCT</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>(1) Randomization probably succesful, the authors show that GPA is the same between Treatment and no Treatment
+(2) Attirition appears to be random, see Table A2
+(3) Contamination should not be an issue. The control group are other students who applied for the mentoring program.</t>
+  </si>
+  <si>
+    <t>DiD</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>(1) Pre-Trends look good, using other federal states as control group seems credible. There are some threats to identification, other policy changes that coincide, students trying to evade G8. Authors discuss these issues and provide robustness tests, which confirm the results of the baseline spec.
+(2) Time of Treatment is clear, we know when the G8 was introduced.</t>
+  </si>
+  <si>
+    <t>bruckmeier2014;gorgen2019</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/ecoedu/v41y2014icp14-23.html;https://ideas.repec.org/p/arx/papers/1909.08299.html</t>
+  </si>
+  <si>
+    <t>Bruckmeier &amp; Wigger (2014);Gorgen &amp; Schienle (2019)</t>
+  </si>
+  <si>
+    <t>PSM</t>
+  </si>
+  <si>
+    <t>The authors construct a control and treatment group by matching individuals with similar probabilites of taking part in a government sponsored training program. The authors argue that the assumptions required for propensity score matching to give valid results hold. This includes: 1) Good Matching (A problem that arises is that individual motiviation which is probalbly a key factor of finding employment is unobservable. The authors try to capture this effect by taking the previous employment history into account), see p. 758 2) Enough Overlap. At most 21% of Obs have to be deleted, see p.760
+3) If CIA holds, matched individuals should on average follow the same trend
+4) Program Participation duration is known and singluar.</t>
+  </si>
+  <si>
+    <t>See above</t>
+  </si>
+  <si>
+    <t>The authors make use of a dynamic matching estimator which allows for differential treatment starts.  The variables upon which the matching estimator is based should lead to good matching, see Section C starting on p. 856. Overlap is discussed on p. 877 Section C. Balacing test shows that there is no treatment effect 7 years before the start.</t>
+  </si>
+  <si>
+    <t>Section 4 discusses relevant indentification assumptions, matching and estimation procedure. This paper has access to personality traits which may be an important left out variable in other studies. However, the inclusion of these traits seems to have a rather small impact on the results. Therefore, concerns that matching procedures which cannot rely on persionality traits do not fulfill the CIA, may not be relevant.</t>
+  </si>
+  <si>
+    <t>The working paper version includes an IV estimation, which is imprecise but confirms the results of the selection on observables PSM approach. The employed instrument is the intensity with which training vouchers are awarded in a region. As the IV reaches the same conclusion, this paper could be a 4 on the maryland scale. Since the IV was excluded in the published version and the exogeneity of the instrument is somewhat debatable, it should probably still be a 3</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>Identification by comparing means between highway sections in Germany and in the Netherlands. No confidence intervals, no regression, no controls.</t>
+  </si>
+  <si>
+    <t>CSR</t>
+  </si>
+  <si>
+    <t>Methodological choices and assumptions are discussed in Section 6. The rich administrative dataset should allow for matching along a wide array of dimensions. In Section 6.3 the authors argue that the covariates are balanced between matchted participants and non-participants. Also, there is enough overlap to produce credible results.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>This Paper uses a difference in difference approach but unlike other DiD scenarios selection into treatment is as good as random. The applicability of maternal leave reforms was governed by the birthdate of the child. Whether a child is born before or after the reform can be regarded as random, unless it is possible to strategically delay births to benefit from the reform. The authors find no evidence of strategic birth timing. To account for seasonal effects children born one year prior are used as a control group. On the Maryland scale DiD would usually be 3. However, the selection into treatment is more similar to a RDD, thus adressing the biggest flaw of DiD. -&gt; Comparable to IV and RDD on Maryland scale.</t>
+  </si>
+  <si>
+    <t>The Eligibility for "Betreuungsgeld" was governed by the birthdate of the child. The  cutoff date was changed unexpectedly. No strategic timing of births possible. DiD is used to correct for seasonal differences. In particular, being born in Autumn may lead to earlier eligibility for daycare centers. Since treatment is governed by a random process this DiD is comparable to IV and RDD.</t>
+  </si>
+  <si>
+    <t>frodermann2020;kluve2013</t>
+  </si>
+  <si>
+    <t>The Eligibility for "Elterngeld" was governed by the birthdate of the child. The cutoff date for the new parental leave system was decided on after the birth. -&gt;  No strategic timing of births possible. DiD is used to correct for seasonal differences. Since treatment is governed by a random process this DiD is comparable to IV and RDD.</t>
+  </si>
+  <si>
+    <t>Simulation...</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>DiD using students not eligible for Bafög as control-group. No further controls. No pretrend, or leads and lags in the paper. Hard to tell if the common trends assumption would hold. There could very well be time-varying factors that affect students from low income households differently and thus bias the estimate.</t>
+  </si>
+  <si>
+    <t>DiD using students not affected by the expansion of Bafög as control. Pre-trend is shown,  and no sig effect is found. However, it looks like there generally a lot of  uncertainty in the data and the estimates are rather imprecisie. Also the pre-trend fluctuates quite a bit, and is sometimes almost significant. (And more sig than the reform effect). -&gt; Categorize as 3,2</t>
+  </si>
+  <si>
+    <t>RDD</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>(1) Discontinuity is sharp
+(2) Nothing else relevant to the outcome changes at the discontinuity
+(3) Behavior may be altered at the cut-off. However, the magnitude appears to be rather small, and the authors conduct various robustness checks to account for potential sorting around the cut-off.</t>
+  </si>
+  <si>
+    <t>(1) Discontinuity is sharp
+(2) Nothing else relevant to the outcome changes at the discontinuity
+(3) Behavior may be altered at the cut-off. The authors concut tests and provide graphical evidence that observable characteristics are smooth around the discontinuity in treatment</t>
+  </si>
+  <si>
+    <t>(1) Common Trends assumption motivated by non-sig leads
+(2) Timing of treatment is given by the Hartz reform</t>
+  </si>
+  <si>
+    <t>(1) Randomization successful, see Table 1
+(2) Attrition cannot be an issue because the study uses administrative data. The labor market outcome is always observed
+(3) Contamination could theoretically be an issue. However, in practice the spillover of receiving the brochure should be negligible.</t>
+  </si>
+  <si>
+    <t>(1) Rich set of matching variables, see Table A2 
+(2) Section 3.4 discusses  identification assumptions &amp; overlap. Various robustness checks are conducted.  Overlap assumption fulfilled. Tests for covariate balance show only sig. differences in two variables</t>
+  </si>
+  <si>
+    <t>Authors use a "preference for mobility programs" measure of the local employment agency as insturment. The authors show relevance (F &gt; 10) and argue for exogeneity and exclusion.</t>
+  </si>
+  <si>
+    <t>Some sort of matching estimator is used, selection on observables approach. Either 2 or 3 on the Maryland scale.</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t>The settings of this paper is non standard. The authors evaluated a field experiment where subsidies were payed to previously unemployed upon accepting a new job. There was a control and a treatment group. The control group was southern Mannheim. The treatment northern Mannheim. There was no real randomization. The authors argue that southern and northern Mannheim are similar in terms of labor market conditions. They control for various observable characterisics: age, gender, household composition. On the maryland scale this should either be a 2 or a 3.  This pseudo experiment with the treatment and control group in a local labor market with comparable conditions is probably a bit better than a pure cross-sectional regression. Individuals are unlikely to select in treatment. -&gt; 3 on Maryland scale.</t>
+  </si>
+  <si>
+    <t>Elements of RDD and Event Study. The randomness which determines the receiption of the letter makes this paper a 4 on the Maryland scale.</t>
+  </si>
+  <si>
+    <t>Authors provide evidence for SUTVA and common trends. Timing of treatment is unambiguous.</t>
+  </si>
+  <si>
+    <t>SEM</t>
+  </si>
+  <si>
+    <t>Pair-wise randomization and Matching. Little and symmetric attrition</t>
+  </si>
+  <si>
+    <t>Exploits staggered introduction across federal states. Discusses various potential sources of bias including self selection into treatment, political leadership</t>
+  </si>
+  <si>
+    <t>piopiunik2014a</t>
+  </si>
+  <si>
+    <t>Piopiunik (2014b)</t>
+  </si>
+  <si>
+    <t>Piopiunik (2014a)</t>
+  </si>
+  <si>
+    <t>piopiunik2014b</t>
+  </si>
+  <si>
+    <t>riphan2012</t>
+  </si>
+  <si>
+    <t>resnjanskij2021</t>
+  </si>
+  <si>
+    <t>obergruber2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) Randomization successful, see Table 1
+(2) Authors argue that attrition is not a problem. In general, attrition is low. Response rate &gt; 90% for follow up surveys. Attrition non random, but identical accross control and treatment. See p. 12.
+(3) Contamination should not be an issue as randomization took place across schools (not within). Unlikely that information treatment spreads to other schools.
+</t>
+  </si>
+  <si>
+    <t>(1) Parallel trends might be violated because of different trends between East and West, and a tendency to introduce tuition fees in the West. The Authors add state specific trends, and FE. The DiD now has elements of a Panel Regression.
+(2) Time of Treatment is given by the introduction of tuition fees.</t>
+  </si>
+  <si>
+    <t>DiD using staggered introduction. Pre-trends cannot be examined. However, there is a large set of robustness checks available.</t>
+  </si>
+  <si>
+    <t>Difference in Difference, and Triple Differences (Considering other federal states and also "Gymnasien" in Bavaria, which are unaffected by the reform). Thorough robustness checks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identification using difference in difference (exploits differences in timing of reform), contains various robustness checks. Specifications with and without state-specific trends </t>
+  </si>
+  <si>
+    <t>Individuals were randomly assigned to a internal or external placement service. However, there is potential to not show up at the external provider. This creates econometric problems (see p. 481), which require further assumptions to get vaild results. Still, the interal validity of this study seems very high. Marlyand scale 4 seems reasonable</t>
+  </si>
+  <si>
+    <t>More of a collection of results from different sources.</t>
+  </si>
+  <si>
+    <t>IV approach to measure the ETI. IV assumptions plausably argued for in Paper. Published in JPubEc.</t>
+  </si>
+  <si>
+    <t>This paper is different from the other papers in that it does not isolate a single effect of X on Y but rather estimates a structural equilibrium model (SEM). The stated assumptions are clear and seem reasonable. The Paper is published in JPubEc. -&gt; Assign a 3,3 on Maryland scale. Could also be higher, but since the metholdolgy allows for quite a bit of different choices which could drive results in one or the other direction 3,3 seems to be safer.</t>
+  </si>
+  <si>
+    <t>Government sponsored training to obtain a new professional degree in a field other than the currently profession.</t>
   </si>
 </sst>
 </file>
@@ -1390,10 +1590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1409,9 +1609,11 @@
     <col min="10" max="10" width="19.28515625" customWidth="1"/>
     <col min="11" max="11" width="45.140625" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="15" max="15" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45">
+    <row r="1" spans="1:17" ht="45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1419,7 +1621,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1440,183 +1642,243 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="150">
+        <v>324</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="150">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="D2">
         <v>1990</v>
       </c>
       <c r="E2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F2">
         <v>48.480624773955284</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>44</v>
       </c>
       <c r="K2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" t="s">
         <v>125</v>
       </c>
-      <c r="L2" t="s">
-        <v>127</v>
-      </c>
       <c r="M2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="60">
+      <c r="N2" t="s">
+        <v>328</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="P2" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="60">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F3">
         <v>48.922446097261144</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="60">
+      <c r="N3" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="P3" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="60">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="D4">
         <v>2004</v>
       </c>
       <c r="E4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F4">
         <v>50.583095918192996</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="75">
+      <c r="N4" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="P4" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="75">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D5">
         <v>2005</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F5">
         <v>50.583095918192996</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="M5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="75">
+      <c r="N5" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="P5" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="105">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1624,7 +1886,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="D6">
         <v>2013</v>
@@ -1636,23 +1898,35 @@
         <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="105">
+      <c r="N6" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="P6" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="105">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1660,7 +1934,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D7">
         <v>2011</v>
@@ -1672,23 +1946,35 @@
         <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>46</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="M7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="75">
+      <c r="N7" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="P7" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="75">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1696,7 +1982,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D8">
         <v>2011</v>
@@ -1708,7 +1994,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" t="s">
@@ -1718,13 +2004,25 @@
         <v>47</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="75">
+      <c r="N8" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="P8" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1732,7 +2030,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D9">
         <v>2008</v>
@@ -1744,23 +2042,35 @@
         <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>339</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>49</v>
+        <v>338</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>134</v>
+        <v>337</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="30">
+      <c r="N9" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="P9" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="150">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1768,38 +2078,50 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D10">
         <v>1993</v>
       </c>
       <c r="E10" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F10">
         <v>35.200000000000003</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H10" s="1">
         <v>1672</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="30">
+      <c r="N10" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1807,38 +2129,50 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D11">
         <v>1993</v>
       </c>
       <c r="E11" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F11">
         <v>34.799999999999997</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H11" s="1">
         <v>1570</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="N11" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1846,38 +2180,50 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D12">
         <v>1993</v>
       </c>
       <c r="E12" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F12">
         <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H12" s="1">
         <v>1434</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="45">
+      <c r="N12" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1885,77 +2231,101 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D13">
         <v>1993</v>
       </c>
       <c r="E13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F13">
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>238</v>
+        <v>392</v>
       </c>
       <c r="H13" s="1">
         <v>1558</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="K13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="30">
+      <c r="N13" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="75">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C14" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D14">
         <v>2000</v>
       </c>
       <c r="E14" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F14">
         <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H14" s="1">
         <v>1559.6189999999999</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="60">
+      <c r="N14" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="75">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1963,77 +2333,101 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D15">
         <v>2000</v>
       </c>
       <c r="E15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F15">
         <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H15" s="1">
         <v>1542.066</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="60">
+      <c r="N15" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="60">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C16" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="D16">
         <v>2003</v>
       </c>
       <c r="E16" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F16">
         <v>38.86</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H16" s="1">
         <v>1459.3779999999999</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="90">
+      <c r="N16" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="90">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2041,76 +2435,100 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D17">
         <v>2003</v>
       </c>
       <c r="E17" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F17">
         <v>40.17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H17" s="1">
         <v>2189.3620000000001</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="M17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="105">
+      <c r="N17" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="105">
       <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C18" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D18">
         <v>2009</v>
       </c>
       <c r="E18" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F18">
         <v>40.969000000000001</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H18" s="1">
         <v>2047.962</v>
       </c>
       <c r="J18" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="60">
+      <c r="N18" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="90">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2118,37 +2536,49 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D19">
         <v>2003</v>
       </c>
       <c r="E19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F19">
         <v>39.03</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H19" s="1">
         <v>1901.21</v>
       </c>
       <c r="J19" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="M19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="180">
+      <c r="N19" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="180">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2159,31 +2589,43 @@
         <v>2015</v>
       </c>
       <c r="E20" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F20">
         <v>46.96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="180">
+      <c r="N20" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="180">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2194,31 +2636,43 @@
         <v>2015</v>
       </c>
       <c r="E21" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F21">
         <v>46.96</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L21" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="120">
+      <c r="N21" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="120">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2226,34 +2680,46 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D22">
         <v>2005</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F22">
         <v>39.64795218424306</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" ht="90">
+      <c r="N22" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="90">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2261,34 +2727,46 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="D23">
         <v>2005</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="J23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" ht="105">
+      <c r="N23" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="105">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2296,290 +2774,383 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="J24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L24" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" ht="60">
+      <c r="N24" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="60">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D25">
         <v>2012</v>
       </c>
       <c r="E25" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F25">
         <v>46.96</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I25" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="120">
+      <c r="N25" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="135">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D26">
         <v>1979</v>
       </c>
       <c r="E26" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I26" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="150">
+      <c r="N26" t="s">
+        <v>334</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="150">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D27">
         <v>1986</v>
       </c>
       <c r="E27" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I27" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L27" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="135">
+      <c r="N27" t="s">
+        <v>334</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="135">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D28">
         <v>1992</v>
       </c>
       <c r="E28" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F28">
         <v>28.1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J28" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L28" t="s">
+        <v>137</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>334</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="75">
+      <c r="A29" t="s">
         <v>71</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="L28" t="s">
-        <v>140</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="60">
-      <c r="A29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B29" t="s">
-        <v>74</v>
-      </c>
       <c r="C29" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D29">
         <v>2013</v>
       </c>
       <c r="E29" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F29">
         <v>31.36</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="J29" t="s">
+        <v>73</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L29" t="s">
+        <v>138</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29" t="s">
+        <v>334</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="120">
+      <c r="A30" t="s">
         <v>75</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="B30" t="s">
         <v>76</v>
       </c>
-      <c r="L29" t="s">
-        <v>141</v>
-      </c>
-      <c r="M29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="120">
-      <c r="A30" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
       <c r="C30" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D30">
         <v>2007</v>
       </c>
       <c r="E30" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F30">
         <v>29.768270000000001</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H30" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L30" t="s">
-        <v>142</v>
+        <v>353</v>
       </c>
       <c r="M30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="120">
+      <c r="N30" t="s">
+        <v>334</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="120">
       <c r="A31" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B31" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D31">
         <v>2020</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L31" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="M31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="75">
+      <c r="N31" t="s">
+        <v>178</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="75">
       <c r="A32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C32" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D32">
         <v>1990</v>
@@ -2591,30 +3162,42 @@
         <v>19.809999999999999</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="J32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="K32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="L32" t="s">
+        <v>140</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32" t="s">
+        <v>334</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="75">
+      <c r="A33" t="s">
         <v>84</v>
       </c>
-      <c r="L32" t="s">
-        <v>144</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" ht="75">
-      <c r="A33" t="s">
-        <v>86</v>
-      </c>
       <c r="B33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D33">
         <v>2001</v>
@@ -2626,565 +3209,745 @@
         <v>19.420999999999999</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="J33" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L33" t="s">
+        <v>141</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33" t="s">
+        <v>334</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="135">
+      <c r="A34" t="s">
         <v>88</v>
       </c>
-      <c r="K33" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L33" t="s">
-        <v>145</v>
-      </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" ht="135">
-      <c r="A34" t="s">
-        <v>90</v>
-      </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D34">
         <v>1993</v>
       </c>
       <c r="E34" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F34">
         <v>42</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H34" s="1">
         <v>1934.5</v>
       </c>
       <c r="J34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L34" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" ht="135">
+      <c r="N34" t="s">
+        <v>359</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="135">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C35" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D35">
         <v>1993</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F35">
         <v>44</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H35" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="J35" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L35" t="s">
+        <v>142</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35" t="s">
+        <v>359</v>
+      </c>
+      <c r="O35" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="P35" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="135">
+      <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
         <v>92</v>
       </c>
-      <c r="K35" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="L35" t="s">
-        <v>146</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="135">
-      <c r="A36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" t="s">
-        <v>94</v>
-      </c>
       <c r="C36" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F36">
         <v>42</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="H36" s="1">
         <v>1925.375</v>
       </c>
       <c r="J36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L36" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="M36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="120">
+      <c r="N36" t="s">
+        <v>359</v>
+      </c>
+      <c r="O36" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="120">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D37">
         <v>2002</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F37">
         <v>45</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H37" s="1">
         <v>1999.866</v>
       </c>
       <c r="J37" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" t="s">
+        <v>143</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37" t="s">
+        <v>359</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="135">
+      <c r="A38" t="s">
+        <v>114</v>
+      </c>
+      <c r="B38" t="s">
         <v>99</v>
       </c>
-      <c r="L37" t="s">
-        <v>147</v>
-      </c>
-      <c r="M37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="135">
-      <c r="A38" t="s">
-        <v>116</v>
-      </c>
-      <c r="B38" t="s">
-        <v>101</v>
-      </c>
       <c r="C38" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D38">
         <v>2006</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J38" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L38" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="M38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" ht="60">
+      <c r="N38" t="s">
+        <v>334</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="75">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D39">
         <v>2011</v>
       </c>
       <c r="E39" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F39">
         <v>36.92</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L39" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="M39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="60">
+      <c r="N39" t="s">
+        <v>331</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="60">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C40" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D40">
         <v>2006</v>
       </c>
       <c r="E40" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F40">
         <v>37.71</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="J40" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="L40" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="M40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="90">
+      <c r="N40" t="s">
+        <v>328</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="90">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41">
         <v>2004</v>
       </c>
       <c r="E41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F41">
         <v>37.630000000000003</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H41">
         <v>2731</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L41" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="M41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" ht="195">
+      <c r="N41" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="195">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D42">
         <v>2001</v>
       </c>
       <c r="E42" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F42">
         <v>39.612000000000002</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="M42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" ht="90">
+      <c r="N42" t="s">
+        <v>331</v>
+      </c>
+      <c r="O42" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="P42" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="90">
       <c r="A43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D43">
         <v>2009</v>
       </c>
       <c r="E43" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F43">
         <v>50.181100000000001</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="H43" s="1">
         <v>1543.018</v>
       </c>
       <c r="J43" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="L43" t="s">
+        <v>151</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43" t="s">
+        <v>331</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="P43" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="150">
+      <c r="A44" t="s">
+        <v>153</v>
+      </c>
+      <c r="B44" t="s">
         <v>154</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="L43" t="s">
-        <v>155</v>
-      </c>
-      <c r="M43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="150">
-      <c r="A44" t="s">
-        <v>157</v>
-      </c>
-      <c r="B44" t="s">
-        <v>158</v>
-      </c>
       <c r="C44" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D44">
         <v>2005</v>
       </c>
       <c r="E44" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F44">
         <v>27</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H44" s="1">
         <v>2004.07</v>
       </c>
       <c r="J44" t="s">
+        <v>156</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="L44" t="s">
+        <v>155</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44" t="s">
+        <v>359</v>
+      </c>
+      <c r="O44" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="105">
+      <c r="A45" t="s">
         <v>160</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="B45" t="s">
         <v>161</v>
       </c>
-      <c r="L44" t="s">
-        <v>159</v>
-      </c>
-      <c r="M44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="105">
-      <c r="A45" t="s">
-        <v>164</v>
-      </c>
-      <c r="B45" t="s">
-        <v>165</v>
-      </c>
       <c r="C45" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D45">
         <v>2012</v>
       </c>
       <c r="E45" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F45">
         <v>44.531999999999996</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="K45" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L45" t="s">
+        <v>159</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45" t="s">
+        <v>334</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="135">
+      <c r="A46" t="s">
         <v>162</v>
       </c>
-      <c r="L45" t="s">
+      <c r="B46" t="s">
         <v>163</v>
       </c>
-      <c r="M45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="135">
-      <c r="A46" t="s">
-        <v>166</v>
-      </c>
-      <c r="B46" t="s">
-        <v>167</v>
-      </c>
       <c r="C46" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D46">
         <v>2012</v>
       </c>
       <c r="E46" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F46">
         <v>50.49</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J46" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L46" t="s">
+        <v>166</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46" t="s">
+        <v>373</v>
+      </c>
+      <c r="O46" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="P46" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="135">
+      <c r="A47" t="s">
+        <v>168</v>
+      </c>
+      <c r="B47" t="s">
         <v>169</v>
       </c>
-      <c r="L46" t="s">
-        <v>170</v>
-      </c>
-      <c r="M46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="135">
-      <c r="A47" t="s">
-        <v>172</v>
-      </c>
-      <c r="B47" t="s">
-        <v>173</v>
-      </c>
       <c r="C47" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D47">
         <v>2012</v>
       </c>
       <c r="E47" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F47">
         <v>50.49</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J47" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="L47" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="105">
+      <c r="N47" t="s">
+        <v>373</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="105">
       <c r="A48" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B48" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C48" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D48">
         <v>1967</v>
@@ -3196,28 +3959,43 @@
         <v>16</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" t="s">
+        <v>378</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="L48" t="s">
+        <v>376</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48" t="s">
+        <v>334</v>
+      </c>
+      <c r="O48" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" ht="120">
+      <c r="A49" t="s">
         <v>257</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="B49" t="s">
         <v>256</v>
       </c>
-      <c r="M48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="120">
-      <c r="A49" t="s">
-        <v>264</v>
-      </c>
-      <c r="B49" t="s">
-        <v>263</v>
-      </c>
       <c r="C49" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D49">
         <v>2003</v>
@@ -3229,27 +4007,42 @@
         <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="J49" t="s">
-        <v>257</v>
+        <v>377</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>261</v>
+        <v>251</v>
+      </c>
+      <c r="L49" t="s">
+        <v>379</v>
       </c>
       <c r="M49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" ht="75">
+      <c r="N49" t="s">
+        <v>334</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" ht="75">
       <c r="A50" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B50" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C50" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D50">
         <v>1957</v>
@@ -3261,27 +4054,42 @@
         <v>10</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
+      </c>
+      <c r="L50" s="7" t="s">
+        <v>380</v>
       </c>
       <c r="M50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" ht="105">
+      <c r="N50" t="s">
+        <v>334</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" ht="105">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B51" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C51" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D51">
         <v>2017</v>
@@ -3293,27 +4101,42 @@
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="J51" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
+      </c>
+      <c r="L51" t="s">
+        <v>381</v>
       </c>
       <c r="M51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" ht="135">
+      <c r="N51" t="s">
+        <v>331</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="P51" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" ht="135">
       <c r="A52" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B52" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C52" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D52">
         <v>1978</v>
@@ -3325,15 +4148,30 @@
         <v>16</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
+      </c>
+      <c r="L52" s="7" t="s">
+        <v>382</v>
       </c>
       <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52" t="s">
+        <v>334</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q52">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* updated literature.bib to json script to use the bibtex keys instead of the some meaningless index-number for the resulting json object * separated economic literature from data sources in programs.xlsx (This adds a new column: other_data_sources) * added missing data sources to literature.bib
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="405">
   <si>
     <t>program_identifier</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Subsidized Job Opportunities</t>
-  </si>
-  <si>
-    <t>Atkinson &amp; Piketty (2010);Gottfried &amp; Schellhorn (2004)</t>
   </si>
   <si>
     <t>https://ideas.repec.org/p/diw/diwwpp/dp1770.html</t>
@@ -391,16 +388,9 @@
     <t>Bafög Reform 2001</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ideas.repec.org/b/oxp/obooks/9780199286898.html;https://ideas.repec.org/p/iaw/iawdip/15.html
-</t>
-  </si>
-  <si>
     <t>bibtexkeys</t>
   </si>
   <si>
-    <t>atkinson2010;gottfried2004</t>
-  </si>
-  <si>
     <t>peter2018</t>
   </si>
   <si>
@@ -425,9 +415,6 @@
     <t>https://ideas.repec.org/a/sae/ilrrev/v70y2017i3p767-812.html;https://ideas.repec.org/p/iza/izadps/dp9138.html</t>
   </si>
   <si>
-    <t>doerr2014;huber2015</t>
-  </si>
-  <si>
     <t>thiedig2018</t>
   </si>
   <si>
@@ -453,9 +440,6 @@
   </si>
   <si>
     <t>caliendo2013;schmieder2016</t>
-  </si>
-  <si>
-    <t>petrunyk2018;schmieder2012;schmieder2016</t>
   </si>
   <si>
     <t>altmann2018</t>
@@ -760,16 +744,6 @@
     <t>Since 2005 the German pension administration sends out letters designed to inform about one's expected future pension payments. These letters also highlight the link between social security contributions and the resulting pension entitlement. To receive such a letter, the recipient had to be at least 27 years old. This age cutoff thus generated quasi-random variation which allows evaluating the resulting effects on earnings and retirement savings.</t>
   </si>
   <si>
-    <t>doerrenberg2015;wid2020</t>
-  </si>
-  <si>
-    <t>Doerrenberg et al. (2015);World Inequality Database (2020)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://ideas.repec.org/p/ces/ceswps/_5369.html;https://wid.world/
-</t>
-  </si>
-  <si>
     <t>Classroom Training</t>
   </si>
   <si>
@@ -1061,9 +1035,6 @@
   </si>
   <si>
     <t>The authors make use of a dynamic matching estimator which allows for differential treatment starts.  The variables upon which the matching estimator is based should lead to good matching, see Section C starting on p. 856. Overlap is discussed on p. 877 Section C. Balacing test shows that there is no treatment effect 7 years before the start.</t>
-  </si>
-  <si>
-    <t>Section 4 discusses relevant indentification assumptions, matching and estimation procedure. This paper has access to personality traits which may be an important left out variable in other studies. However, the inclusion of these traits seems to have a rather small impact on the results. Therefore, concerns that matching procedures which cannot rely on persionality traits do not fulfill the CIA, may not be relevant.</t>
   </si>
   <si>
     <t>The working paper version includes an IV estimation, which is imprecise but confirms the results of the selection on observables PSM approach. The employed instrument is the intensity with which training vouchers are awarded in a region. As the IV reaches the same conclusion, this paper could be a 4 on the maryland scale. Since the IV was excluded in the published version and the exogeneity of the instrument is somewhat debatable, it should probably still be a 3</t>
@@ -1207,9 +1178,6 @@
     <t xml:space="preserve">Identification using difference in difference (exploits differences in timing of reform), contains various robustness checks. Specifications with and without state-specific trends </t>
   </si>
   <si>
-    <t>Individuals were randomly assigned to a internal or external placement service. However, there is potential to not show up at the external provider. This creates econometric problems (see p. 481), which require further assumptions to get vaild results. Still, the interal validity of this study seems very high. Marlyand scale 4 seems reasonable</t>
-  </si>
-  <si>
     <t>More of a collection of results from different sources.</t>
   </si>
   <si>
@@ -1220,6 +1188,72 @@
   </si>
   <si>
     <t>Government sponsored training to obtain a new professional degree in a field other than the currently profession.</t>
+  </si>
+  <si>
+    <t>other_data_sources</t>
+  </si>
+  <si>
+    <t>wid2020;destatisTax1995</t>
+  </si>
+  <si>
+    <t>wid2020;destatisTax2001</t>
+  </si>
+  <si>
+    <t>wid2020;destatisTax2004</t>
+  </si>
+  <si>
+    <t>Doerrenberg et al. (2017)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html</t>
+  </si>
+  <si>
+    <t>doerrenberg2017</t>
+  </si>
+  <si>
+    <t>doerr2014</t>
+  </si>
+  <si>
+    <t>biewen2014;huber2015</t>
+  </si>
+  <si>
+    <t>destatisAgePopulation</t>
+  </si>
+  <si>
+    <t>Individuals were randomly assigned to an internal or external placement service. However, there is potential to not show up at the external provider. This creates econometric problems (see p. 481), which require further assumptions to get vaild results. Still, the interal validity of this study seems very high. Marlyand scale 4 seems reasonable</t>
+  </si>
+  <si>
+    <t>destatis2019a;schmillen2014</t>
+  </si>
+  <si>
+    <t>destatis2019b;schmillen2014</t>
+  </si>
+  <si>
+    <t>destatis2019a;destatis2019b;schmillen2014</t>
+  </si>
+  <si>
+    <t>schmillen2014</t>
+  </si>
+  <si>
+    <t>destatisMothersAge;destatis2019b;schmillen2014</t>
+  </si>
+  <si>
+    <t>destatis2019a;destatis1991;schmillen2014</t>
+  </si>
+  <si>
+    <t>destatis2019a;destatis2004;schmillen2014</t>
+  </si>
+  <si>
+    <t>petrunyk2018;schmieder2016</t>
+  </si>
+  <si>
+    <t>schmieder2012</t>
+  </si>
+  <si>
+    <t>Section 4 discusses relevant indentification assumptions, matching and estimation procedure. This paper has access to personality traits which may be an important left out variable in other studies. However, the inclusion of these traits seems to have a rather small impact on the results. Therefore, concerns that matching procedures which cannot rely on personality traits do not fulfill the CIA, may not be relevant.</t>
+  </si>
+  <si>
+    <t>destatis2019a;destatis2015;schmillen2014</t>
   </si>
 </sst>
 </file>
@@ -1590,10 +1624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1608,12 +1642,12 @@
     <col min="9" max="9" width="26.42578125" customWidth="1"/>
     <col min="10" max="10" width="19.28515625" customWidth="1"/>
     <col min="11" max="11" width="45.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" customWidth="1"/>
-    <col min="15" max="15" width="76.28515625" customWidth="1"/>
+    <col min="12" max="13" width="17.28515625" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" customWidth="1"/>
+    <col min="16" max="16" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45">
+    <row r="1" spans="1:18" ht="45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1621,7 +1655,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1642,243 +1676,258 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>324</v>
+        <v>383</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="150">
+        <v>318</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="150">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="D2">
         <v>1990</v>
       </c>
       <c r="E2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F2">
         <v>48.480624773955284</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>44</v>
+        <v>387</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>123</v>
+        <v>388</v>
       </c>
       <c r="L2" t="s">
-        <v>125</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
-        <v>328</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="P2" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="60">
+        <v>389</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>320</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>321</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="60">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C3" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F3">
         <v>48.922446097261144</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>246</v>
+        <v>387</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>328</v>
+        <v>388</v>
+      </c>
+      <c r="L3" t="s">
+        <v>389</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="P3" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="60">
+        <v>320</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>321</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="60">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C4" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D4">
         <v>2004</v>
       </c>
       <c r="E4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F4">
         <v>50.583095918192996</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>246</v>
+        <v>387</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>328</v>
+        <v>388</v>
+      </c>
+      <c r="L4" t="s">
+        <v>389</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="P4" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="75">
+        <v>320</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>321</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="75">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D5">
         <v>2005</v>
       </c>
       <c r="E5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F5">
         <v>50.583095918192996</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>246</v>
+        <v>387</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>328</v>
+        <v>388</v>
+      </c>
+      <c r="L5" t="s">
+        <v>389</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="P5" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="105">
+        <v>320</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>321</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="105">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1886,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="D6">
         <v>2013</v>
@@ -1898,35 +1947,38 @@
         <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>126</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>331</v>
+        <v>123</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="P6" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q6">
+        <v>323</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>324</v>
+      </c>
+      <c r="R6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="105">
+    <row r="7" spans="1:18" ht="105">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1934,7 +1986,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D7">
         <v>2011</v>
@@ -1946,35 +1998,38 @@
         <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>331</v>
+        <v>124</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="P7" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q7">
+        <v>323</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>324</v>
+      </c>
+      <c r="R7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="75">
+    <row r="8" spans="1:18" ht="75">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1982,7 +2037,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D8">
         <v>2011</v>
@@ -1994,35 +2049,38 @@
         <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>334</v>
+        <v>125</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="P8" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="75">
+        <v>326</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>327</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2030,7 +2088,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D9">
         <v>2008</v>
@@ -2042,35 +2100,38 @@
         <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>334</v>
+        <v>329</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="P9" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="150">
+        <v>326</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>327</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="150">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2078,50 +2139,51 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D10">
         <v>1993</v>
       </c>
       <c r="E10" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F10">
         <v>35.200000000000003</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H10" s="1">
         <v>1672</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M10">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>340</v>
+        <v>126</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10">
+        <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="30">
+        <v>333</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="30">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2129,50 +2191,51 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D11">
         <v>1993</v>
       </c>
       <c r="E11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F11">
         <v>34.799999999999997</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="H11" s="1">
         <v>1570</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>340</v>
+        <v>126</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11">
+        <v>1</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>334</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2180,50 +2243,51 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="D12">
         <v>1993</v>
       </c>
       <c r="E12" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F12">
         <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H12" s="1">
         <v>1434</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>340</v>
+        <v>126</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12">
+        <v>1</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="45">
+        <v>334</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2231,101 +2295,103 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D13">
         <v>1993</v>
       </c>
       <c r="E13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F13">
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="H13" s="1">
         <v>1558</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>340</v>
+        <v>126</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13">
+        <v>1</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="75">
+        <v>334</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="75">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C14" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D14">
         <v>2000</v>
       </c>
       <c r="E14" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F14">
         <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H14" s="1">
         <v>1559.6189999999999</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>340</v>
+        <v>127</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14">
+        <v>1</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="75">
+      <c r="Q14" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="75">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2333,101 +2399,102 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D15">
         <v>2000</v>
       </c>
       <c r="E15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F15">
         <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H15" s="1">
         <v>1542.066</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>340</v>
+        <v>127</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15">
+        <v>1</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="Q15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="60">
+      <c r="Q15" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="60">
       <c r="A16" t="s">
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C16" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="D16">
         <v>2003</v>
       </c>
       <c r="E16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F16">
         <v>38.86</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H16" s="1">
         <v>1459.3779999999999</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="L16" t="s">
-        <v>149</v>
-      </c>
-      <c r="M16">
-        <v>1</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>340</v>
+        <v>144</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>365</v>
+        <v>332</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="90">
+        <v>356</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="90">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2435,100 +2502,100 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="D17">
         <v>2003</v>
       </c>
       <c r="E17" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F17">
         <v>40.17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H17" s="1">
         <v>2189.3620000000001</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="L17" t="s">
-        <v>149</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>340</v>
+        <v>144</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>365</v>
+        <v>332</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="105">
+        <v>356</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="105">
       <c r="A18" t="s">
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C18" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="D18">
         <v>2009</v>
       </c>
       <c r="E18" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F18">
         <v>40.969000000000001</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="H18" s="1">
         <v>2047.962</v>
       </c>
       <c r="J18" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L18" t="s">
-        <v>131</v>
-      </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>340</v>
+        <v>128</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="90">
+        <v>403</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="90">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2536,49 +2603,52 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D19">
         <v>2003</v>
       </c>
       <c r="E19" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F19">
         <v>39.03</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H19" s="1">
         <v>1901.21</v>
       </c>
       <c r="J19" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="L19" t="s">
-        <v>134</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>340</v>
+        <v>390</v>
+      </c>
+      <c r="M19" t="s">
+        <v>391</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="180">
+        <v>336</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="180">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2589,43 +2659,46 @@
         <v>2015</v>
       </c>
       <c r="E20" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F20">
         <v>46.96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L20" t="s">
-        <v>135</v>
-      </c>
-      <c r="M20">
+        <v>131</v>
+      </c>
+      <c r="M20" t="s">
+        <v>392</v>
+      </c>
+      <c r="N20">
         <v>0</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>348</v>
-      </c>
       <c r="O20" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q20">
+        <v>338</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="R20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="180">
+    <row r="21" spans="1:18" ht="180">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2636,43 +2709,46 @@
         <v>2015</v>
       </c>
       <c r="E21" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F21">
         <v>46.96</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L21" t="s">
-        <v>135</v>
-      </c>
-      <c r="M21">
+        <v>131</v>
+      </c>
+      <c r="M21" t="s">
+        <v>392</v>
+      </c>
+      <c r="N21">
         <v>0</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>348</v>
-      </c>
       <c r="O21" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="Q21">
+        <v>338</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="R21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="120">
+    <row r="22" spans="1:18" ht="120">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2680,46 +2756,46 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D22">
         <v>2005</v>
       </c>
       <c r="E22" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F22">
         <v>39.64795218424306</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J22" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K22" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="L22" t="s">
-        <v>132</v>
-      </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-      <c r="N22" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="O22" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q22">
+      <c r="Q22" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="90">
+    <row r="23" spans="1:18" ht="90">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2727,46 +2803,46 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="D23">
         <v>2005</v>
       </c>
       <c r="E23" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J23" t="s">
+        <v>55</v>
+      </c>
+      <c r="K23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K23" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="L23" t="s">
-        <v>132</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
-      </c>
-      <c r="N23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="O23" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q23">
+      <c r="Q23" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="105">
+    <row r="24" spans="1:18" ht="105">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2774,383 +2850,395 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J24" t="s">
+        <v>55</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K24" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="L24" t="s">
-        <v>132</v>
-      </c>
-      <c r="M24">
-        <v>1</v>
-      </c>
-      <c r="N24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="P24" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q24">
+      <c r="Q24" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="60">
+    <row r="25" spans="1:18" ht="60">
       <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
         <v>60</v>
-      </c>
-      <c r="B25" t="s">
-        <v>61</v>
       </c>
       <c r="D25">
         <v>2012</v>
       </c>
       <c r="E25" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F25">
         <v>46.96</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I25" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="J25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="L25" t="s">
-        <v>136</v>
-      </c>
-      <c r="M25">
+        <v>132</v>
+      </c>
+      <c r="M25" t="s">
+        <v>392</v>
+      </c>
+      <c r="N25">
         <v>0</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="O25" s="1" t="s">
-        <v>389</v>
+        <v>173</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q25">
+        <v>379</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="R25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="135">
+    <row r="26" spans="1:18" ht="135">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D26">
         <v>1979</v>
       </c>
       <c r="E26" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I26" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="J26" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="L26" t="s">
-        <v>137</v>
-      </c>
-      <c r="M26">
-        <v>1</v>
-      </c>
-      <c r="N26" t="s">
-        <v>334</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>351</v>
+        <v>133</v>
+      </c>
+      <c r="M26" t="s">
+        <v>397</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>326</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="150">
+        <v>342</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="150">
       <c r="A27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D27">
         <v>1986</v>
       </c>
       <c r="E27" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I27" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="J27" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K27" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="L27" t="s">
-        <v>137</v>
-      </c>
-      <c r="M27">
-        <v>1</v>
-      </c>
-      <c r="N27" t="s">
-        <v>334</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>351</v>
+        <v>133</v>
+      </c>
+      <c r="M27" t="s">
+        <v>395</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>326</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="135">
+        <v>342</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="135">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D28">
         <v>1992</v>
       </c>
       <c r="E28" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F28">
         <v>28.1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="J28" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="L28" t="s">
+        <v>133</v>
+      </c>
+      <c r="M28" t="s">
+        <v>398</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
+        <v>326</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="75">
+      <c r="A29" t="s">
         <v>70</v>
       </c>
-      <c r="L28" t="s">
-        <v>137</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28" t="s">
-        <v>334</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="75">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>71</v>
       </c>
-      <c r="B29" t="s">
-        <v>72</v>
-      </c>
       <c r="C29" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D29">
         <v>2013</v>
       </c>
       <c r="E29" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F29">
         <v>31.36</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="J29" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" t="s">
+        <v>134</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
+        <v>326</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="120">
+      <c r="A30" t="s">
         <v>74</v>
       </c>
-      <c r="L29" t="s">
-        <v>138</v>
-      </c>
-      <c r="M29">
-        <v>1</v>
-      </c>
-      <c r="N29" t="s">
-        <v>334</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="120">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>75</v>
       </c>
-      <c r="B30" t="s">
-        <v>76</v>
-      </c>
       <c r="C30" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="D30">
         <v>2007</v>
       </c>
       <c r="E30" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F30">
         <v>29.768270000000001</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H30" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="J30" t="s">
+        <v>76</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K30" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="L30" t="s">
-        <v>353</v>
-      </c>
-      <c r="M30">
-        <v>1</v>
-      </c>
-      <c r="N30" t="s">
-        <v>334</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>354</v>
+        <v>344</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>326</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q30">
+        <v>345</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="120">
+    <row r="31" spans="1:18" ht="120">
       <c r="A31" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D31">
         <v>2020</v>
       </c>
       <c r="E31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="J31" t="s">
+        <v>78</v>
+      </c>
+      <c r="K31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" t="s">
+        <v>135</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31" t="s">
+        <v>173</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="75">
+      <c r="A32" t="s">
         <v>80</v>
       </c>
-      <c r="L31" t="s">
-        <v>139</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31" t="s">
-        <v>178</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="75">
-      <c r="A32" t="s">
-        <v>81</v>
-      </c>
       <c r="B32" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C32" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="D32">
         <v>1990</v>
@@ -3162,42 +3250,45 @@
         <v>19.809999999999999</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="J32" t="s">
+        <v>82</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" t="s">
+        <v>136</v>
+      </c>
+      <c r="M32" t="s">
+        <v>399</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32" t="s">
+        <v>326</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="75">
+      <c r="A33" t="s">
         <v>83</v>
       </c>
-      <c r="K32" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L32" t="s">
-        <v>140</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="N32" t="s">
-        <v>334</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="75">
-      <c r="A33" t="s">
-        <v>84</v>
-      </c>
       <c r="B33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D33">
         <v>2001</v>
@@ -3209,745 +3300,751 @@
         <v>19.420999999999999</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="J33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L33" t="s">
-        <v>141</v>
-      </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="N33" t="s">
-        <v>334</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>358</v>
+        <v>137</v>
+      </c>
+      <c r="M33" t="s">
+        <v>400</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33" t="s">
+        <v>326</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q33">
+        <v>349</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="R33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="135">
+    <row r="34" spans="1:18" ht="135">
       <c r="A34" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
         <v>88</v>
       </c>
-      <c r="B34" t="s">
-        <v>89</v>
-      </c>
       <c r="C34" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="D34">
         <v>1993</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F34">
         <v>42</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H34" s="1">
         <v>1934.5</v>
       </c>
       <c r="J34" t="s">
+        <v>89</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L34" t="s">
+        <v>138</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
+        <v>350</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="135">
+      <c r="A35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" t="s">
         <v>90</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L34" t="s">
-        <v>142</v>
-      </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="N34" t="s">
-        <v>359</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="135">
-      <c r="A35" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" t="s">
-        <v>91</v>
-      </c>
       <c r="C35" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="D35">
         <v>1993</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F35">
         <v>44</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H35" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="J35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L35" t="s">
-        <v>142</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="N35" t="s">
-        <v>359</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>361</v>
+        <v>138</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
+        <v>350</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="135">
+        <v>352</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="135">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F36">
         <v>42</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H36" s="1">
         <v>1925.375</v>
       </c>
       <c r="J36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L36" t="s">
-        <v>142</v>
-      </c>
-      <c r="M36">
-        <v>1</v>
-      </c>
-      <c r="N36" t="s">
-        <v>359</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>361</v>
+        <v>138</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
+        <v>350</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="120">
+        <v>352</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="120">
       <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" t="s">
         <v>95</v>
       </c>
-      <c r="B37" t="s">
-        <v>96</v>
-      </c>
       <c r="C37" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="D37">
         <v>2002</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F37">
         <v>45</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H37" s="1">
         <v>1999.866</v>
       </c>
       <c r="J37" t="s">
+        <v>97</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37" t="s">
+        <v>139</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37" t="s">
+        <v>350</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="135">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" t="s">
         <v>98</v>
       </c>
-      <c r="K37" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L37" t="s">
-        <v>143</v>
-      </c>
-      <c r="M37">
-        <v>1</v>
-      </c>
-      <c r="N37" t="s">
-        <v>359</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="135">
-      <c r="A38" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" t="s">
-        <v>99</v>
-      </c>
       <c r="C38" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="D38">
         <v>2006</v>
       </c>
       <c r="E38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="J38" t="s">
+        <v>99</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K38" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="L38" t="s">
-        <v>144</v>
-      </c>
-      <c r="M38">
-        <v>1</v>
-      </c>
-      <c r="N38" t="s">
-        <v>334</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>363</v>
+        <v>401</v>
+      </c>
+      <c r="M38" t="s">
+        <v>402</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38" t="s">
+        <v>326</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q38">
+        <v>354</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="75">
+    <row r="39" spans="1:18" ht="75">
       <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B39" t="s">
         <v>104</v>
       </c>
-      <c r="B39" t="s">
-        <v>105</v>
-      </c>
       <c r="C39" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="D39">
         <v>2011</v>
       </c>
       <c r="E39" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F39">
         <v>36.92</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="H39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L39" t="s">
-        <v>145</v>
-      </c>
-      <c r="M39">
-        <v>1</v>
-      </c>
-      <c r="N39" t="s">
-        <v>331</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>364</v>
+        <v>140</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39" t="s">
+        <v>323</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="60">
+        <v>355</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="R39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="60">
       <c r="A40" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" t="s">
         <v>106</v>
       </c>
-      <c r="B40" t="s">
-        <v>107</v>
-      </c>
       <c r="C40" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D40">
         <v>2006</v>
       </c>
       <c r="E40" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F40">
         <v>37.71</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="H40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="J40" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L40" t="s">
-        <v>148</v>
-      </c>
-      <c r="M40">
-        <v>1</v>
-      </c>
-      <c r="N40" t="s">
-        <v>328</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>366</v>
+        <v>143</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40" t="s">
+        <v>320</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="90">
+        <v>357</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="90">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41">
         <v>2004</v>
       </c>
       <c r="E41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41">
         <v>37.630000000000003</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H41">
         <v>2731</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L41" t="s">
-        <v>146</v>
-      </c>
-      <c r="M41">
+        <v>141</v>
+      </c>
+      <c r="N41">
         <v>0</v>
       </c>
-      <c r="N41" s="1" t="s">
-        <v>348</v>
-      </c>
       <c r="O41" s="1" t="s">
-        <v>367</v>
+        <v>339</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="Q41">
+        <v>358</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="R41">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="195">
+    <row r="42" spans="1:18" ht="195">
       <c r="A42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" t="s">
         <v>117</v>
       </c>
-      <c r="B42" t="s">
-        <v>118</v>
-      </c>
       <c r="C42" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D42">
         <v>2001</v>
       </c>
       <c r="E42" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F42">
         <v>39.612000000000002</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L42" t="s">
-        <v>147</v>
-      </c>
-      <c r="M42">
-        <v>1</v>
-      </c>
-      <c r="N42" t="s">
-        <v>331</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>370</v>
+        <v>142</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42" t="s">
+        <v>323</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="Q42">
+        <v>361</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="R42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="90">
+    <row r="43" spans="1:18" ht="90">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D43">
         <v>2009</v>
       </c>
       <c r="E43" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F43">
         <v>50.181100000000001</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H43" s="1">
         <v>1543.018</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L43" t="s">
-        <v>151</v>
-      </c>
-      <c r="M43">
-        <v>1</v>
-      </c>
-      <c r="N43" t="s">
-        <v>331</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>388</v>
+        <v>146</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43" t="s">
+        <v>323</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="Q43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" ht="150">
+        <v>393</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="R43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="150">
       <c r="A44" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B44" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C44" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="D44">
         <v>2005</v>
       </c>
       <c r="E44" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F44">
         <v>27</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H44" s="1">
         <v>2004.07</v>
       </c>
       <c r="J44" t="s">
+        <v>151</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="L44" t="s">
+        <v>150</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44" t="s">
+        <v>350</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="105">
+      <c r="A45" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" t="s">
         <v>156</v>
       </c>
-      <c r="K44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="L44" t="s">
-        <v>155</v>
-      </c>
-      <c r="M44">
-        <v>1</v>
-      </c>
-      <c r="N44" t="s">
-        <v>359</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="105">
-      <c r="A45" t="s">
-        <v>160</v>
-      </c>
-      <c r="B45" t="s">
-        <v>161</v>
-      </c>
       <c r="C45" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D45">
         <v>2012</v>
       </c>
       <c r="E45" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F45">
         <v>44.531999999999996</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="K45" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="L45" t="s">
+        <v>154</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45" t="s">
+        <v>326</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="135">
+      <c r="A46" t="s">
+        <v>157</v>
+      </c>
+      <c r="B46" t="s">
         <v>158</v>
       </c>
-      <c r="L45" t="s">
-        <v>159</v>
-      </c>
-      <c r="M45">
-        <v>1</v>
-      </c>
-      <c r="N45" t="s">
-        <v>334</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="135">
-      <c r="A46" t="s">
-        <v>162</v>
-      </c>
-      <c r="B46" t="s">
-        <v>163</v>
-      </c>
       <c r="C46" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D46">
         <v>2012</v>
       </c>
       <c r="E46" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F46">
         <v>50.49</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="J46" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="L46" t="s">
-        <v>166</v>
-      </c>
-      <c r="M46">
-        <v>1</v>
-      </c>
-      <c r="N46" t="s">
-        <v>373</v>
-      </c>
-      <c r="O46" s="1" t="s">
-        <v>391</v>
+        <v>161</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46" t="s">
+        <v>364</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="135">
+        <v>381</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="135">
       <c r="A47" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C47" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D47">
         <v>2012</v>
       </c>
       <c r="E47" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="F47">
         <v>50.49</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="J47" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="L47" t="s">
-        <v>166</v>
-      </c>
-      <c r="M47">
-        <v>1</v>
-      </c>
-      <c r="N47" t="s">
-        <v>373</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>391</v>
+        <v>161</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47" t="s">
+        <v>364</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="105">
+        <v>381</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="105">
       <c r="A48" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B48" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C48" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D48">
         <v>1967</v>
@@ -3959,43 +4056,46 @@
         <v>16</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" t="s">
+        <v>369</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="L48" t="s">
+        <v>367</v>
+      </c>
+      <c r="M48" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="N48">
+        <v>1</v>
+      </c>
+      <c r="O48" t="s">
+        <v>326</v>
+      </c>
+      <c r="P48" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="K48" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="L48" t="s">
-        <v>376</v>
-      </c>
-      <c r="M48">
-        <v>1</v>
-      </c>
-      <c r="N48" t="s">
-        <v>334</v>
-      </c>
-      <c r="O48" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" ht="120">
+      <c r="Q48" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="120">
       <c r="A49" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B49" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C49" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D49">
         <v>2003</v>
@@ -4007,42 +4107,45 @@
         <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J49" t="s">
+        <v>368</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="L49" t="s">
+        <v>370</v>
+      </c>
+      <c r="M49" t="s">
+        <v>397</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49" t="s">
+        <v>326</v>
+      </c>
+      <c r="P49" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="Q49" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" ht="75">
+      <c r="A50" t="s">
+        <v>250</v>
+      </c>
+      <c r="B50" t="s">
         <v>251</v>
       </c>
-      <c r="L49" t="s">
-        <v>379</v>
-      </c>
-      <c r="M49">
-        <v>1</v>
-      </c>
-      <c r="N49" t="s">
-        <v>334</v>
-      </c>
-      <c r="O49" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" ht="75">
-      <c r="A50" t="s">
-        <v>258</v>
-      </c>
-      <c r="B50" t="s">
-        <v>259</v>
-      </c>
       <c r="C50" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="D50">
         <v>1957</v>
@@ -4054,42 +4157,45 @@
         <v>10</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="M50">
-        <v>1</v>
-      </c>
-      <c r="N50" t="s">
-        <v>334</v>
-      </c>
-      <c r="O50" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="N50">
+        <v>1</v>
+      </c>
+      <c r="O50" t="s">
+        <v>326</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" ht="105">
+        <v>366</v>
+      </c>
+      <c r="Q50" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" ht="105">
       <c r="A51" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B51" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="C51" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="D51">
         <v>2017</v>
@@ -4101,42 +4207,45 @@
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="J51" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="L51" t="s">
-        <v>381</v>
-      </c>
-      <c r="M51">
-        <v>1</v>
-      </c>
-      <c r="N51" t="s">
-        <v>331</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="P51" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q51">
+        <v>372</v>
+      </c>
+      <c r="M51" t="s">
+        <v>397</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
+      <c r="O51" t="s">
+        <v>323</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>324</v>
+      </c>
+      <c r="R51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="135">
+    <row r="52" spans="1:18" ht="135">
       <c r="A52" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B52" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="C52" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="D52">
         <v>1978</v>
@@ -4148,70 +4257,69 @@
         <v>16</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="M52">
-        <v>1</v>
-      </c>
-      <c r="N52" t="s">
-        <v>334</v>
-      </c>
-      <c r="O52" s="1" t="s">
-        <v>385</v>
+        <v>373</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52" t="s">
+        <v>326</v>
       </c>
       <c r="P52" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q52">
+        <v>376</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="R52">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
-    <hyperlink ref="K6" r:id="rId2"/>
-    <hyperlink ref="K7" r:id="rId3"/>
-    <hyperlink ref="K9" r:id="rId4"/>
-    <hyperlink ref="K8" r:id="rId5"/>
-    <hyperlink ref="K14" r:id="rId6"/>
-    <hyperlink ref="K15" r:id="rId7"/>
-    <hyperlink ref="K18" r:id="rId8"/>
-    <hyperlink ref="K19" r:id="rId9"/>
-    <hyperlink ref="K20" r:id="rId10"/>
-    <hyperlink ref="K21" r:id="rId11"/>
-    <hyperlink ref="K22" r:id="rId12"/>
-    <hyperlink ref="K23" r:id="rId13"/>
-    <hyperlink ref="K24" r:id="rId14"/>
-    <hyperlink ref="K25" r:id="rId15"/>
-    <hyperlink ref="K28" r:id="rId16"/>
-    <hyperlink ref="K27" r:id="rId17"/>
-    <hyperlink ref="K26" r:id="rId18"/>
-    <hyperlink ref="K29" r:id="rId19"/>
-    <hyperlink ref="K30" r:id="rId20"/>
-    <hyperlink ref="K5" r:id="rId21"/>
-    <hyperlink ref="K31" r:id="rId22" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="K32" r:id="rId23" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
-    <hyperlink ref="K33" r:id="rId24" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="K34" r:id="rId25"/>
-    <hyperlink ref="K37" r:id="rId26"/>
-    <hyperlink ref="K4" r:id="rId27"/>
-    <hyperlink ref="K3" r:id="rId28"/>
-    <hyperlink ref="K48" r:id="rId29"/>
-    <hyperlink ref="K49" r:id="rId30"/>
-    <hyperlink ref="K50" r:id="rId31"/>
-    <hyperlink ref="K51" r:id="rId32"/>
-    <hyperlink ref="K52" r:id="rId33"/>
+    <hyperlink ref="K6" r:id="rId1"/>
+    <hyperlink ref="K7" r:id="rId2"/>
+    <hyperlink ref="K9" r:id="rId3"/>
+    <hyperlink ref="K8" r:id="rId4"/>
+    <hyperlink ref="K14" r:id="rId5"/>
+    <hyperlink ref="K15" r:id="rId6"/>
+    <hyperlink ref="K18" r:id="rId7"/>
+    <hyperlink ref="K19" r:id="rId8"/>
+    <hyperlink ref="K20" r:id="rId9"/>
+    <hyperlink ref="K21" r:id="rId10"/>
+    <hyperlink ref="K22" r:id="rId11"/>
+    <hyperlink ref="K23" r:id="rId12"/>
+    <hyperlink ref="K24" r:id="rId13"/>
+    <hyperlink ref="K25" r:id="rId14"/>
+    <hyperlink ref="K28" r:id="rId15"/>
+    <hyperlink ref="K27" r:id="rId16"/>
+    <hyperlink ref="K26" r:id="rId17"/>
+    <hyperlink ref="K29" r:id="rId18"/>
+    <hyperlink ref="K30" r:id="rId19"/>
+    <hyperlink ref="K31" r:id="rId20" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="K32" r:id="rId21" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
+    <hyperlink ref="K33" r:id="rId22" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="K34" r:id="rId23"/>
+    <hyperlink ref="K37" r:id="rId24"/>
+    <hyperlink ref="K48" r:id="rId25"/>
+    <hyperlink ref="K49" r:id="rId26"/>
+    <hyperlink ref="K50" r:id="rId27"/>
+    <hyperlink ref="K51" r:id="rId28"/>
+    <hyperlink ref="K52" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* updated convert BibTexToJSON script to include all fields * fixed formatting errors in literature.bib * updated plot.js to now display additional data sources
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -319,9 +319,6 @@
     <t>Unemployment Benefits Hartz Reform</t>
   </si>
   <si>
-    <t>Petrunyk &amp; Pfeifer (2018);Schmieder et al. (2012);Schmieder &amp; von Wachter (2016)</t>
-  </si>
-  <si>
     <t>https://ideas.repec.org/p/iza/izadps/dp11300.html;https://ideas.repec.org/a/oup/qjecon/v127y2012i2p701-752.html;https://ideas.repec.org/a/anr/reveco/v8y2016p547-581.html</t>
   </si>
   <si>
@@ -1254,6 +1251,9 @@
   </si>
   <si>
     <t>destatis2019a;destatis2015;schmillen2014</t>
+  </si>
+  <si>
+    <t>Petrunyk &amp; Pfeifer (2018);Schmieder &amp; von Wachter (2016)</t>
   </si>
 </sst>
 </file>
@@ -1626,8 +1626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="G35" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1655,7 +1655,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1676,31 +1676,31 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="150">
@@ -1708,52 +1708,52 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D2">
         <v>1990</v>
       </c>
       <c r="E2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F2">
         <v>48.480624773955284</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" t="s">
         <v>388</v>
       </c>
-      <c r="L2" t="s">
-        <v>389</v>
-      </c>
       <c r="M2" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
+        <v>319</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q2" t="s">
         <v>320</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>321</v>
       </c>
       <c r="R2">
         <v>1</v>
@@ -1761,55 +1761,55 @@
     </row>
     <row r="3" spans="1:18" ht="60">
       <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
         <v>174</v>
       </c>
-      <c r="B3" t="s">
-        <v>175</v>
-      </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F3">
         <v>48.922446097261144</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" t="s">
         <v>388</v>
       </c>
-      <c r="L3" t="s">
-        <v>389</v>
-      </c>
       <c r="M3" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q3" t="s">
         <v>320</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>321</v>
       </c>
       <c r="R3">
         <v>1</v>
@@ -1817,55 +1817,55 @@
     </row>
     <row r="4" spans="1:18" ht="60">
       <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
         <v>176</v>
       </c>
-      <c r="B4" t="s">
-        <v>177</v>
-      </c>
       <c r="C4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4">
         <v>2004</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F4">
         <v>50.583095918192996</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L4" t="s">
         <v>388</v>
       </c>
-      <c r="L4" t="s">
-        <v>389</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q4" t="s">
         <v>320</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>321</v>
       </c>
       <c r="R4">
         <v>1</v>
@@ -1873,55 +1873,55 @@
     </row>
     <row r="5" spans="1:18" ht="75">
       <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="s">
         <v>178</v>
       </c>
-      <c r="B5" t="s">
-        <v>179</v>
-      </c>
       <c r="C5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D5">
         <v>2005</v>
       </c>
       <c r="E5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F5">
         <v>50.583095918192996</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="L5" t="s">
         <v>388</v>
       </c>
-      <c r="L5" t="s">
-        <v>389</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q5" t="s">
         <v>320</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>321</v>
       </c>
       <c r="R5">
         <v>1</v>
@@ -1935,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D6">
         <v>2013</v>
@@ -1947,32 +1947,32 @@
         <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q6" t="s">
         <v>323</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>324</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1986,7 +1986,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D7">
         <v>2011</v>
@@ -1998,32 +1998,32 @@
         <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
       <c r="O7" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q7" t="s">
         <v>323</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>324</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -2037,7 +2037,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D8">
         <v>2011</v>
@@ -2049,7 +2049,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" t="s">
@@ -2059,22 +2059,22 @@
         <v>46</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="O8" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q8" t="s">
         <v>326</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>327</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -2088,7 +2088,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D9">
         <v>2008</v>
@@ -2100,32 +2100,32 @@
         <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q9" t="s">
         <v>326</v>
-      </c>
-      <c r="P9" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>327</v>
       </c>
       <c r="R9">
         <v>1</v>
@@ -2139,45 +2139,45 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D10">
         <v>1993</v>
       </c>
       <c r="E10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F10">
         <v>35.200000000000003</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H10" s="1">
         <v>1672</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K10" t="s">
         <v>48</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10">
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="P10" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>333</v>
-      </c>
       <c r="Q10" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -2191,45 +2191,45 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D11">
         <v>1993</v>
       </c>
       <c r="E11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F11">
         <v>34.799999999999997</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H11" s="1">
         <v>1570</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K11" t="s">
         <v>48</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -2243,45 +2243,45 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D12">
         <v>1993</v>
       </c>
       <c r="E12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F12">
         <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H12" s="1">
         <v>1434</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K12" t="s">
         <v>48</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12">
         <v>1</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R12">
         <v>1</v>
@@ -2295,45 +2295,45 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D13">
         <v>1993</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F13">
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H13" s="1">
         <v>1558</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K13" t="s">
         <v>48</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13">
         <v>1</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -2344,48 +2344,48 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D14">
         <v>2000</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F14">
         <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H14" s="1">
         <v>1559.6189999999999</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>49</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -2399,45 +2399,45 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D15">
         <v>2000</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F15">
         <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H15" s="1">
         <v>1542.066</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>49</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15">
         <v>1</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -2448,22 +2448,22 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D16">
         <v>2003</v>
       </c>
       <c r="E16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F16">
         <v>38.86</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H16" s="1">
         <v>1459.3779999999999</v>
@@ -2476,19 +2476,19 @@
         <v>51</v>
       </c>
       <c r="L16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N16">
         <v>1</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -2502,19 +2502,19 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D17">
         <v>2003</v>
       </c>
       <c r="E17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F17">
         <v>40.17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H17" s="1">
         <v>2189.3620000000001</v>
@@ -2527,19 +2527,19 @@
         <v>51</v>
       </c>
       <c r="L17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N17">
         <v>1</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R17">
         <v>1</v>
@@ -2550,46 +2550,46 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D18">
         <v>2009</v>
       </c>
       <c r="E18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F18">
         <v>40.969000000000001</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H18" s="1">
         <v>2047.962</v>
       </c>
       <c r="J18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>52</v>
       </c>
       <c r="L18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R18">
         <v>1</v>
@@ -2603,46 +2603,46 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D19">
         <v>2003</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F19">
         <v>39.03</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H19" s="1">
         <v>1901.21</v>
       </c>
       <c r="J19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L19" t="s">
+        <v>389</v>
+      </c>
+      <c r="M19" t="s">
         <v>390</v>
       </c>
-      <c r="M19" t="s">
-        <v>391</v>
-      </c>
       <c r="N19">
         <v>1</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R19">
         <v>1</v>
@@ -2659,16 +2659,16 @@
         <v>2015</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F20">
         <v>46.96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J20" t="s">
         <v>54</v>
@@ -2677,22 +2677,22 @@
         <v>53</v>
       </c>
       <c r="L20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M20" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -2709,16 +2709,16 @@
         <v>2015</v>
       </c>
       <c r="E21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F21">
         <v>46.96</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J21" t="s">
         <v>54</v>
@@ -2727,22 +2727,22 @@
         <v>53</v>
       </c>
       <c r="L21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -2756,19 +2756,19 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D22">
         <v>2005</v>
       </c>
       <c r="E22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F22">
         <v>39.64795218424306</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J22" t="s">
         <v>55</v>
@@ -2777,19 +2777,19 @@
         <v>56</v>
       </c>
       <c r="L22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -2803,19 +2803,19 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D23">
         <v>2005</v>
       </c>
       <c r="E23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J23" t="s">
         <v>55</v>
@@ -2824,19 +2824,19 @@
         <v>56</v>
       </c>
       <c r="L23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N23">
         <v>1</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R23">
         <v>0</v>
@@ -2850,19 +2850,19 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J24" t="s">
         <v>55</v>
@@ -2871,19 +2871,19 @@
         <v>56</v>
       </c>
       <c r="L24" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N24">
         <v>1</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R24">
         <v>0</v>
@@ -2900,16 +2900,16 @@
         <v>2012</v>
       </c>
       <c r="E25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F25">
         <v>46.96</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I25" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J25" t="s">
         <v>57</v>
@@ -2918,22 +2918,22 @@
         <v>58</v>
       </c>
       <c r="L25" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -2947,19 +2947,19 @@
         <v>65</v>
       </c>
       <c r="C26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D26">
         <v>1979</v>
       </c>
       <c r="E26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J26" t="s">
         <v>68</v>
@@ -2968,22 +2968,22 @@
         <v>69</v>
       </c>
       <c r="L26" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N26">
         <v>1</v>
       </c>
       <c r="O26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R26">
         <v>1</v>
@@ -2997,19 +2997,19 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D27">
         <v>1986</v>
       </c>
       <c r="E27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I27" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J27" t="s">
         <v>68</v>
@@ -3018,22 +3018,22 @@
         <v>69</v>
       </c>
       <c r="L27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N27">
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R27">
         <v>1</v>
@@ -3047,22 +3047,22 @@
         <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D28">
         <v>1992</v>
       </c>
       <c r="E28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F28">
         <v>28.1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J28" t="s">
         <v>68</v>
@@ -3071,22 +3071,22 @@
         <v>69</v>
       </c>
       <c r="L28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M28" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="N28">
         <v>1</v>
       </c>
       <c r="O28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R28">
         <v>1</v>
@@ -3100,19 +3100,19 @@
         <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D29">
         <v>2013</v>
       </c>
       <c r="E29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F29">
         <v>31.36</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="J29" t="s">
         <v>72</v>
@@ -3121,19 +3121,19 @@
         <v>73</v>
       </c>
       <c r="L29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N29">
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -3147,19 +3147,19 @@
         <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D30">
         <v>2007</v>
       </c>
       <c r="E30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F30">
         <v>29.768270000000001</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H30" s="1">
         <v>2235.6489999999999</v>
@@ -3171,19 +3171,19 @@
         <v>77</v>
       </c>
       <c r="L30" t="s">
+        <v>343</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>325</v>
+      </c>
+      <c r="P30" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="N30">
-        <v>1</v>
-      </c>
-      <c r="O30" t="s">
-        <v>326</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="Q30" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R30">
         <v>0</v>
@@ -3191,10 +3191,10 @@
     </row>
     <row r="31" spans="1:18" ht="120">
       <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
         <v>197</v>
-      </c>
-      <c r="B31" t="s">
-        <v>198</v>
       </c>
       <c r="D31">
         <v>2020</v>
@@ -3203,10 +3203,10 @@
         <v>64</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J31" t="s">
         <v>78</v>
@@ -3215,16 +3215,16 @@
         <v>79</v>
       </c>
       <c r="L31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N31">
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="R31">
         <v>0</v>
@@ -3235,10 +3235,10 @@
         <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D32">
         <v>1990</v>
@@ -3250,7 +3250,7 @@
         <v>19.809999999999999</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J32" t="s">
         <v>82</v>
@@ -3259,22 +3259,22 @@
         <v>81</v>
       </c>
       <c r="L32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M32" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="N32">
         <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -3285,10 +3285,10 @@
         <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D33">
         <v>2001</v>
@@ -3300,7 +3300,7 @@
         <v>19.420999999999999</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J33" t="s">
         <v>85</v>
@@ -3309,22 +3309,22 @@
         <v>84</v>
       </c>
       <c r="L33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M33" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="N33">
         <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="R33">
         <v>0</v>
@@ -3338,19 +3338,19 @@
         <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D34">
         <v>1993</v>
       </c>
       <c r="E34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F34">
         <v>42</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H34" s="1">
         <v>1934.5</v>
@@ -3362,19 +3362,19 @@
         <v>86</v>
       </c>
       <c r="L34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N34">
         <v>1</v>
       </c>
       <c r="O34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R34">
         <v>1</v>
@@ -3388,19 +3388,19 @@
         <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D35">
         <v>1993</v>
       </c>
       <c r="E35" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F35">
         <v>44</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H35" s="1">
         <v>1928.4169999999999</v>
@@ -3412,19 +3412,19 @@
         <v>86</v>
       </c>
       <c r="L35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N35">
         <v>1</v>
       </c>
       <c r="O35" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R35">
         <v>1</v>
@@ -3438,19 +3438,19 @@
         <v>91</v>
       </c>
       <c r="C36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F36">
         <v>42</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H36" s="1">
         <v>1925.375</v>
@@ -3462,19 +3462,19 @@
         <v>86</v>
       </c>
       <c r="L36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N36">
         <v>1</v>
       </c>
       <c r="O36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R36">
         <v>1</v>
@@ -3488,19 +3488,19 @@
         <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D37">
         <v>2002</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F37">
         <v>45</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H37" s="1">
         <v>1999.866</v>
@@ -3512,19 +3512,19 @@
         <v>96</v>
       </c>
       <c r="L37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N37">
         <v>1</v>
       </c>
       <c r="O37" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R37">
         <v>1</v>
@@ -3532,49 +3532,49 @@
     </row>
     <row r="38" spans="1:18" ht="135">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
         <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D38">
         <v>2006</v>
       </c>
       <c r="E38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J38" t="s">
+        <v>404</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="K38" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="L38" t="s">
+        <v>400</v>
+      </c>
+      <c r="M38" t="s">
         <v>401</v>
       </c>
-      <c r="M38" t="s">
-        <v>402</v>
-      </c>
       <c r="N38">
         <v>1</v>
       </c>
       <c r="O38" t="s">
+        <v>325</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="Q38" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="R38">
         <v>0</v>
@@ -3582,49 +3582,49 @@
     </row>
     <row r="39" spans="1:18" ht="75">
       <c r="A39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
         <v>103</v>
       </c>
-      <c r="B39" t="s">
-        <v>104</v>
-      </c>
       <c r="C39" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D39">
         <v>2011</v>
       </c>
       <c r="E39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F39">
         <v>36.92</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N39">
         <v>1</v>
       </c>
       <c r="O39" t="s">
+        <v>322</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q39" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>324</v>
       </c>
       <c r="R39">
         <v>1</v>
@@ -3632,49 +3632,49 @@
     </row>
     <row r="40" spans="1:18" ht="60">
       <c r="A40" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" t="s">
         <v>105</v>
       </c>
-      <c r="B40" t="s">
-        <v>106</v>
-      </c>
       <c r="C40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D40">
         <v>2006</v>
       </c>
       <c r="E40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F40">
         <v>37.71</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="J40" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N40">
         <v>1</v>
       </c>
       <c r="O40" t="s">
+        <v>319</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Q40" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="R40">
         <v>1</v>
@@ -3682,10 +3682,10 @@
     </row>
     <row r="41" spans="1:18" ht="90">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41">
@@ -3698,31 +3698,31 @@
         <v>37.630000000000003</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H41">
         <v>2731</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N41">
         <v>0</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="R41">
         <v>0</v>
@@ -3730,49 +3730,49 @@
     </row>
     <row r="42" spans="1:18" ht="195">
       <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" t="s">
         <v>116</v>
       </c>
-      <c r="B42" t="s">
-        <v>117</v>
-      </c>
       <c r="C42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D42">
         <v>2001</v>
       </c>
       <c r="E42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F42">
         <v>39.612000000000002</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N42">
         <v>1</v>
       </c>
       <c r="O42" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -3780,49 +3780,49 @@
     </row>
     <row r="43" spans="1:18" ht="90">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D43">
         <v>2009</v>
       </c>
       <c r="E43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F43">
         <v>50.181100000000001</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H43" s="1">
         <v>1543.018</v>
       </c>
       <c r="J43" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L43" t="s">
         <v>145</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="L43" t="s">
-        <v>146</v>
-      </c>
       <c r="N43">
         <v>1</v>
       </c>
       <c r="O43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="R43">
         <v>1</v>
@@ -3830,49 +3830,49 @@
     </row>
     <row r="44" spans="1:18" ht="150">
       <c r="A44" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" t="s">
         <v>148</v>
       </c>
-      <c r="B44" t="s">
-        <v>149</v>
-      </c>
       <c r="C44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D44">
         <v>2005</v>
       </c>
       <c r="E44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F44">
         <v>27</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H44" s="1">
         <v>2004.07</v>
       </c>
       <c r="J44" t="s">
+        <v>150</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="K44" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="L44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N44">
         <v>1</v>
       </c>
       <c r="O44" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="R44">
         <v>1</v>
@@ -3880,49 +3880,49 @@
     </row>
     <row r="45" spans="1:18" ht="105">
       <c r="A45" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" t="s">
         <v>155</v>
       </c>
-      <c r="B45" t="s">
-        <v>156</v>
-      </c>
       <c r="C45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D45">
         <v>2012</v>
       </c>
       <c r="E45" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F45">
         <v>44.531999999999996</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K45" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="L45" t="s">
         <v>153</v>
       </c>
-      <c r="L45" t="s">
-        <v>154</v>
-      </c>
       <c r="N45">
         <v>1</v>
       </c>
       <c r="O45" t="s">
+        <v>325</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="Q45" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="R45">
         <v>1</v>
@@ -3930,53 +3930,53 @@
     </row>
     <row r="46" spans="1:18" ht="135">
       <c r="A46" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" t="s">
         <v>157</v>
       </c>
-      <c r="B46" t="s">
-        <v>158</v>
-      </c>
       <c r="C46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D46">
         <v>2012</v>
       </c>
       <c r="E46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F46">
         <v>50.49</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L46" t="s">
         <v>160</v>
       </c>
-      <c r="L46" t="s">
-        <v>161</v>
-      </c>
       <c r="N46">
         <v>1</v>
       </c>
       <c r="O46" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R46">
         <v>1</v>
@@ -3984,53 +3984,53 @@
     </row>
     <row r="47" spans="1:18" ht="135">
       <c r="A47" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" t="s">
         <v>163</v>
       </c>
-      <c r="B47" t="s">
-        <v>164</v>
-      </c>
       <c r="C47" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D47">
         <v>2012</v>
       </c>
       <c r="E47" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F47">
         <v>50.49</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J47" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="L47" t="s">
         <v>160</v>
       </c>
-      <c r="L47" t="s">
-        <v>161</v>
-      </c>
       <c r="N47">
         <v>1</v>
       </c>
       <c r="O47" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R47">
         <v>1</v>
@@ -4038,13 +4038,13 @@
     </row>
     <row r="48" spans="1:18" ht="105">
       <c r="A48" t="s">
+        <v>244</v>
+      </c>
+      <c r="B48" t="s">
         <v>245</v>
       </c>
-      <c r="B48" t="s">
-        <v>246</v>
-      </c>
       <c r="C48" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D48">
         <v>1967</v>
@@ -4056,32 +4056,32 @@
         <v>16</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L48" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N48">
         <v>1</v>
       </c>
       <c r="O48" t="s">
+        <v>325</v>
+      </c>
+      <c r="P48" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q48" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="P48" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="R48">
         <v>1</v>
@@ -4089,13 +4089,13 @@
     </row>
     <row r="49" spans="1:18" ht="120">
       <c r="A49" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B49" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D49">
         <v>2003</v>
@@ -4107,31 +4107,31 @@
         <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J49" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M49" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N49">
         <v>1</v>
       </c>
       <c r="O49" t="s">
+        <v>325</v>
+      </c>
+      <c r="P49" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q49" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="P49" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="Q49" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="R49">
         <v>1</v>
@@ -4139,13 +4139,13 @@
     </row>
     <row r="50" spans="1:18" ht="75">
       <c r="A50" t="s">
+        <v>249</v>
+      </c>
+      <c r="B50" t="s">
         <v>250</v>
       </c>
-      <c r="B50" t="s">
-        <v>251</v>
-      </c>
       <c r="C50" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D50">
         <v>1957</v>
@@ -4157,31 +4157,31 @@
         <v>10</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N50">
         <v>1</v>
       </c>
       <c r="O50" t="s">
+        <v>325</v>
+      </c>
+      <c r="P50" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q50" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q50" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="R50">
         <v>1</v>
@@ -4189,13 +4189,13 @@
     </row>
     <row r="51" spans="1:18" ht="105">
       <c r="A51" t="s">
+        <v>256</v>
+      </c>
+      <c r="B51" t="s">
         <v>257</v>
       </c>
-      <c r="B51" t="s">
-        <v>258</v>
-      </c>
       <c r="C51" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D51">
         <v>2017</v>
@@ -4207,31 +4207,31 @@
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J51" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="L51" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M51" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N51">
         <v>1</v>
       </c>
       <c r="O51" t="s">
+        <v>322</v>
+      </c>
+      <c r="P51" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q51" t="s">
         <v>323</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>324</v>
       </c>
       <c r="R51">
         <v>0</v>
@@ -4239,13 +4239,13 @@
     </row>
     <row r="52" spans="1:18" ht="135">
       <c r="A52" t="s">
+        <v>259</v>
+      </c>
+      <c r="B52" t="s">
         <v>260</v>
       </c>
-      <c r="B52" t="s">
-        <v>261</v>
-      </c>
       <c r="C52" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D52">
         <v>1978</v>
@@ -4257,31 +4257,31 @@
         <v>16</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L52" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M52" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N52">
         <v>1</v>
       </c>
       <c r="O52" t="s">
+        <v>325</v>
+      </c>
+      <c r="P52" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q52" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>327</v>
       </c>
       <c r="R52">
         <v>1</v>

</xml_diff>

<commit_message>
* checked for updated publications. There seem to be no published versions of working papers referenced in the literature list. (7/2/22) * fixed wrong year in citation of Dustmann & Schönberg (2012) * replaced remaining links to MS Academic with IDEAS
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -195,10 +195,6 @@
     <t>Sieg (2014);Elvik (2013)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ideas.repec.org/p/mut/wpaper/21.html;https://academic.microsoft.com/paper/2110952839
-</t>
-  </si>
-  <si>
     <t>bicycleHelmet</t>
   </si>
   <si>
@@ -224,12 +220,6 @@
   </si>
   <si>
     <t>Maternity Leave Reform 1992</t>
-  </si>
-  <si>
-    <t>Dustmann &amp; Schönberg (2011)</t>
-  </si>
-  <si>
-    <t>https://academic.microsoft.com/paper/2075105139/</t>
   </si>
   <si>
     <t>homeCareSubsidy</t>
@@ -1254,6 +1244,15 @@
   </si>
   <si>
     <t>Informationsschreiben über zu erwartende Rentenansprüche</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/p/mut/wpaper/21.html;https://pubmed.ncbi.nlm.nih.gov/21376924/</t>
+  </si>
+  <si>
+    <t>Dustmann &amp; Schönberg (2012)</t>
+  </si>
+  <si>
+    <t>https://ideas.repec.org/a/aea/aejapp/v4y2012i3p190-224.html</t>
   </si>
 </sst>
 </file>
@@ -1626,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1655,7 +1654,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1676,31 +1675,31 @@
         <v>4</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>314</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="150">
@@ -1708,52 +1707,52 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D2">
         <v>1990</v>
       </c>
       <c r="E2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F2">
         <v>48.480624773955284</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H2" s="1">
         <v>8868.6350000000002</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="N2">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Q2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R2">
         <v>1</v>
@@ -1761,55 +1760,55 @@
     </row>
     <row r="3" spans="1:18" ht="60">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D3">
         <v>2001</v>
       </c>
       <c r="E3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F3">
         <v>48.922446097261144</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H3" s="1">
         <v>9056.3310000000001</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Q3" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R3">
         <v>1</v>
@@ -1817,55 +1816,55 @@
     </row>
     <row r="4" spans="1:18" ht="60">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D4">
         <v>2004</v>
       </c>
       <c r="E4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F4">
         <v>50.583095918192996</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H4" s="1">
         <v>8886.7603079578239</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L4" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="N4">
         <v>1</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Q4" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R4">
         <v>1</v>
@@ -1873,55 +1872,55 @@
     </row>
     <row r="5" spans="1:18" ht="75">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D5">
         <v>2005</v>
       </c>
       <c r="E5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F5">
         <v>50.583095918192996</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H5" s="1">
         <v>9022.8359999999993</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L5" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="Q5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R5">
         <v>1</v>
@@ -1935,7 +1934,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D6">
         <v>2013</v>
@@ -1947,32 +1946,32 @@
         <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="Q6" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="R6">
         <v>0</v>
@@ -1986,7 +1985,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D7">
         <v>2011</v>
@@ -1998,32 +1997,32 @@
         <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>45</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="Q7" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -2037,7 +2036,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D8">
         <v>2011</v>
@@ -2049,7 +2048,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" t="s">
@@ -2059,22 +2058,22 @@
         <v>46</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="Q8" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R8">
         <v>1</v>
@@ -2088,7 +2087,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D9">
         <v>2008</v>
@@ -2100,32 +2099,32 @@
         <v>21</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="Q9" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R9">
         <v>1</v>
@@ -2139,45 +2138,45 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D10">
         <v>1993</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F10">
         <v>35.200000000000003</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H10" s="1">
         <v>1672</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K10" t="s">
         <v>48</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10">
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R10">
         <v>1</v>
@@ -2191,45 +2190,45 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="D11">
         <v>1993</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F11">
         <v>34.799999999999997</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H11" s="1">
         <v>1570</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K11" t="s">
         <v>48</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11">
         <v>1</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -2243,45 +2242,45 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D12">
         <v>1993</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F12">
         <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H12" s="1">
         <v>1434</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K12" t="s">
         <v>48</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12">
         <v>1</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R12">
         <v>1</v>
@@ -2295,45 +2294,45 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="D13">
         <v>1993</v>
       </c>
       <c r="E13" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F13">
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="H13" s="1">
         <v>1558</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K13" t="s">
         <v>48</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13">
         <v>1</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -2344,48 +2343,48 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D14">
         <v>2000</v>
       </c>
       <c r="E14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F14">
         <v>37</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="H14" s="1">
         <v>1559.6189999999999</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>49</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="P14" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>330</v>
-      </c>
       <c r="Q14" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R14">
         <v>1</v>
@@ -2399,45 +2398,45 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D15">
         <v>2000</v>
       </c>
       <c r="E15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F15">
         <v>37</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H15" s="1">
         <v>1542.066</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>49</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15">
         <v>1</v>
       </c>
       <c r="O15" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="P15" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>330</v>
-      </c>
       <c r="Q15" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R15">
         <v>1</v>
@@ -2448,22 +2447,22 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C16" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D16">
         <v>2003</v>
       </c>
       <c r="E16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F16">
         <v>38.86</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H16" s="1">
         <v>1459.3779999999999</v>
@@ -2476,19 +2475,19 @@
         <v>51</v>
       </c>
       <c r="L16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N16">
         <v>1</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R16">
         <v>1</v>
@@ -2502,19 +2501,19 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="D17">
         <v>2003</v>
       </c>
       <c r="E17" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F17">
         <v>40.17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="H17" s="1">
         <v>2189.3620000000001</v>
@@ -2527,19 +2526,19 @@
         <v>51</v>
       </c>
       <c r="L17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N17">
         <v>1</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R17">
         <v>1</v>
@@ -2550,46 +2549,46 @@
         <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C18" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D18">
         <v>2009</v>
       </c>
       <c r="E18" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F18">
         <v>40.969000000000001</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H18" s="1">
         <v>2047.962</v>
       </c>
       <c r="J18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>52</v>
       </c>
       <c r="L18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R18">
         <v>1</v>
@@ -2603,46 +2602,46 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D19">
         <v>2003</v>
       </c>
       <c r="E19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F19">
         <v>39.03</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H19" s="1">
         <v>1901.21</v>
       </c>
       <c r="J19" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L19" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="M19" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="N19">
         <v>1</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R19">
         <v>1</v>
@@ -2659,16 +2658,16 @@
         <v>2015</v>
       </c>
       <c r="E20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F20">
         <v>46.96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J20" t="s">
         <v>54</v>
@@ -2677,22 +2676,22 @@
         <v>53</v>
       </c>
       <c r="L20" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M20" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="N20">
         <v>0</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="R20">
         <v>0</v>
@@ -2709,16 +2708,16 @@
         <v>2015</v>
       </c>
       <c r="E21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F21">
         <v>46.96</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="J21" t="s">
         <v>54</v>
@@ -2727,22 +2726,22 @@
         <v>53</v>
       </c>
       <c r="L21" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M21" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="N21">
         <v>0</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="R21">
         <v>0</v>
@@ -2756,19 +2755,19 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D22">
         <v>2005</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F22">
         <v>39.64795218424306</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="J22" t="s">
         <v>55</v>
@@ -2777,19 +2776,19 @@
         <v>56</v>
       </c>
       <c r="L22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N22">
         <v>1</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R22">
         <v>0</v>
@@ -2803,19 +2802,19 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D23">
         <v>2005</v>
       </c>
       <c r="E23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F23" s="4">
         <v>38.264488399999998</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J23" t="s">
         <v>55</v>
@@ -2824,19 +2823,19 @@
         <v>56</v>
       </c>
       <c r="L23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N23">
         <v>1</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R23">
         <v>0</v>
@@ -2850,19 +2849,19 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F24" s="1">
         <v>34.553800649999999</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J24" t="s">
         <v>55</v>
@@ -2871,69 +2870,69 @@
         <v>56</v>
       </c>
       <c r="L24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="N24">
         <v>1</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="60">
+    <row r="25" spans="1:18" ht="45">
       <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" t="s">
         <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
       </c>
       <c r="D25">
         <v>2012</v>
       </c>
       <c r="E25" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F25">
         <v>46.96</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="I25" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J25" t="s">
         <v>57</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>58</v>
+        <v>402</v>
       </c>
       <c r="L25" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="M25" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="R25">
         <v>0</v>
@@ -2941,49 +2940,49 @@
     </row>
     <row r="26" spans="1:18" ht="135">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D26">
         <v>1979</v>
       </c>
       <c r="E26" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I26" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J26" t="s">
-        <v>68</v>
+        <v>403</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>69</v>
+        <v>404</v>
       </c>
       <c r="L26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="M26" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="N26">
         <v>1</v>
       </c>
       <c r="O26" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R26">
         <v>1</v>
@@ -2991,49 +2990,49 @@
     </row>
     <row r="27" spans="1:18" ht="150">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D27">
         <v>1986</v>
       </c>
       <c r="E27" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I27" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="J27" t="s">
-        <v>68</v>
+        <v>403</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>69</v>
+        <v>404</v>
       </c>
       <c r="L27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="M27" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="N27">
         <v>1</v>
       </c>
       <c r="O27" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R27">
         <v>1</v>
@@ -3041,52 +3040,52 @@
     </row>
     <row r="28" spans="1:18" ht="135">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D28">
         <v>1992</v>
       </c>
       <c r="E28" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F28">
         <v>28.1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J28" t="s">
-        <v>68</v>
+        <v>403</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>69</v>
+        <v>404</v>
       </c>
       <c r="L28" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="M28" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="N28">
         <v>1</v>
       </c>
       <c r="O28" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R28">
         <v>1</v>
@@ -3094,46 +3093,46 @@
     </row>
     <row r="29" spans="1:18" ht="75">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D29">
         <v>2013</v>
       </c>
       <c r="E29" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F29">
         <v>31.36</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="J29" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="N29">
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -3141,49 +3140,49 @@
     </row>
     <row r="30" spans="1:18" ht="120">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D30">
         <v>2007</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F30">
         <v>29.768270000000001</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H30" s="1">
         <v>2235.6489999999999</v>
       </c>
       <c r="J30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L30" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="N30">
         <v>1</v>
       </c>
       <c r="O30" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R30">
         <v>0</v>
@@ -3191,40 +3190,40 @@
     </row>
     <row r="31" spans="1:18" ht="120">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D31">
         <v>2020</v>
       </c>
       <c r="E31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="J31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N31">
         <v>0</v>
       </c>
       <c r="O31" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="R31">
         <v>0</v>
@@ -3232,13 +3231,13 @@
     </row>
     <row r="32" spans="1:18" ht="75">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C32" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D32">
         <v>1990</v>
@@ -3250,31 +3249,31 @@
         <v>19.809999999999999</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="M32" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="N32">
         <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="R32">
         <v>0</v>
@@ -3282,13 +3281,13 @@
     </row>
     <row r="33" spans="1:18" ht="75">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D33">
         <v>2001</v>
@@ -3300,31 +3299,31 @@
         <v>19.420999999999999</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J33" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="M33" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="N33">
         <v>1</v>
       </c>
       <c r="O33" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="R33">
         <v>0</v>
@@ -3332,49 +3331,49 @@
     </row>
     <row r="34" spans="1:18" ht="135">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D34">
         <v>1993</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F34">
         <v>42</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H34" s="1">
         <v>1934.5</v>
       </c>
       <c r="J34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L34" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N34">
         <v>1</v>
       </c>
       <c r="O34" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R34">
         <v>1</v>
@@ -3382,49 +3381,49 @@
     </row>
     <row r="35" spans="1:18" ht="135">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C35" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D35">
         <v>1993</v>
       </c>
       <c r="E35" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F35">
         <v>44</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="H35" s="1">
         <v>1928.4169999999999</v>
       </c>
       <c r="J35" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L35" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N35">
         <v>1</v>
       </c>
       <c r="O35" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R35">
         <v>1</v>
@@ -3432,49 +3431,49 @@
     </row>
     <row r="36" spans="1:18" ht="135">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F36">
         <v>42</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H36" s="1">
         <v>1925.375</v>
       </c>
       <c r="J36" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L36" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="N36">
         <v>1</v>
       </c>
       <c r="O36" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R36">
         <v>1</v>
@@ -3482,49 +3481,49 @@
     </row>
     <row r="37" spans="1:18" ht="120">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C37" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D37">
         <v>2002</v>
       </c>
       <c r="E37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F37">
         <v>45</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H37" s="1">
         <v>1999.866</v>
       </c>
       <c r="J37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L37" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N37">
         <v>1</v>
       </c>
       <c r="O37" t="s">
+        <v>342</v>
+      </c>
+      <c r="P37" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="P37" s="1" t="s">
-        <v>348</v>
-      </c>
       <c r="Q37" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R37">
         <v>1</v>
@@ -3532,49 +3531,49 @@
     </row>
     <row r="38" spans="1:18" ht="135">
       <c r="A38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D38">
         <v>2006</v>
       </c>
       <c r="E38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F38" s="1">
         <v>50.492400000000004</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="J38" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L38" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="M38" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="N38">
         <v>1</v>
       </c>
       <c r="O38" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R38">
         <v>0</v>
@@ -3582,49 +3581,49 @@
     </row>
     <row r="39" spans="1:18" ht="75">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D39">
         <v>2011</v>
       </c>
       <c r="E39" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F39">
         <v>36.92</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H39" s="1">
         <v>1593.2249999999999</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L39" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N39">
         <v>1</v>
       </c>
       <c r="O39" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="R39">
         <v>1</v>
@@ -3632,49 +3631,49 @@
     </row>
     <row r="40" spans="1:18" ht="60">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D40">
         <v>2006</v>
       </c>
       <c r="E40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F40">
         <v>37.71</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H40" s="1">
         <v>2624.9580000000001</v>
       </c>
       <c r="J40" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L40" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="N40">
         <v>1</v>
       </c>
       <c r="O40" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R40">
         <v>1</v>
@@ -3682,47 +3681,47 @@
     </row>
     <row r="41" spans="1:18" ht="90">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41">
         <v>2004</v>
       </c>
       <c r="E41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F41">
         <v>37.630000000000003</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H41">
         <v>2731</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L41" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N41">
         <v>0</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="P41" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="R41">
         <v>0</v>
@@ -3730,49 +3729,49 @@
     </row>
     <row r="42" spans="1:18" ht="195">
       <c r="A42" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C42" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D42">
         <v>2001</v>
       </c>
       <c r="E42" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F42">
         <v>39.612000000000002</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H42" s="1">
         <v>1278.2249999999999</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L42" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="N42">
         <v>1</v>
       </c>
       <c r="O42" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -3780,49 +3779,49 @@
     </row>
     <row r="43" spans="1:18" ht="90">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D43">
         <v>2009</v>
       </c>
       <c r="E43" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F43">
         <v>50.181100000000001</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H43" s="1">
         <v>1543.018</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N43">
         <v>1</v>
       </c>
       <c r="O43" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="R43">
         <v>1</v>
@@ -3830,49 +3829,49 @@
     </row>
     <row r="44" spans="1:18" ht="150">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D44">
         <v>2005</v>
       </c>
       <c r="E44" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F44">
         <v>27</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H44" s="1">
         <v>2004.07</v>
       </c>
       <c r="J44" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L44" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="N44">
         <v>1</v>
       </c>
       <c r="O44" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="R44">
         <v>1</v>
@@ -3880,49 +3879,49 @@
     </row>
     <row r="45" spans="1:18" ht="105">
       <c r="A45" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C45" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D45">
         <v>2012</v>
       </c>
       <c r="E45" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F45">
         <v>44.531999999999996</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="H45" s="1">
         <v>994.59460000000001</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="L45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="N45">
         <v>1</v>
       </c>
       <c r="O45" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P45" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R45">
         <v>1</v>
@@ -3930,53 +3929,53 @@
     </row>
     <row r="46" spans="1:18" ht="135">
       <c r="A46" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B46" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D46">
         <v>2012</v>
       </c>
       <c r="E46" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F46">
         <v>50.49</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L46" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N46">
         <v>1</v>
       </c>
       <c r="O46" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R46">
         <v>1</v>
@@ -3984,53 +3983,53 @@
     </row>
     <row r="47" spans="1:18" ht="135">
       <c r="A47" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C47" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D47">
         <v>2012</v>
       </c>
       <c r="E47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F47">
         <v>50.49</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="J47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="L47" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="N47">
         <v>1</v>
       </c>
       <c r="O47" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R47">
         <v>1</v>
@@ -4038,13 +4037,13 @@
     </row>
     <row r="48" spans="1:18" ht="105">
       <c r="A48" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B48" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C48" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D48">
         <v>1967</v>
@@ -4056,32 +4055,32 @@
         <v>16</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="I48" s="1"/>
       <c r="J48" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L48" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="N48">
         <v>1</v>
       </c>
       <c r="O48" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P48" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R48">
         <v>1</v>
@@ -4089,13 +4088,13 @@
     </row>
     <row r="49" spans="1:18" ht="120">
       <c r="A49" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B49" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C49" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D49">
         <v>2003</v>
@@ -4107,31 +4106,31 @@
         <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J49" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="L49" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="M49" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="N49">
         <v>1</v>
       </c>
       <c r="O49" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P49" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R49">
         <v>1</v>
@@ -4139,13 +4138,13 @@
     </row>
     <row r="50" spans="1:18" ht="75">
       <c r="A50" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B50" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C50" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D50">
         <v>1957</v>
@@ -4157,31 +4156,31 @@
         <v>10</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="L50" s="7" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="M50" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="N50">
         <v>1</v>
       </c>
       <c r="O50" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="P50" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R50">
         <v>1</v>
@@ -4189,13 +4188,13 @@
     </row>
     <row r="51" spans="1:18" ht="105">
       <c r="A51" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B51" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C51" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D51">
         <v>2017</v>
@@ -4207,31 +4206,31 @@
         <v>14</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J51" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="L51" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="M51" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="N51">
         <v>1</v>
       </c>
       <c r="O51" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="P51" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="Q51" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="R51">
         <v>0</v>
@@ -4239,13 +4238,13 @@
     </row>
     <row r="52" spans="1:18" ht="135">
       <c r="A52" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B52" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C52" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D52">
         <v>1978</v>
@@ -4257,31 +4256,31 @@
         <v>16</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="L52" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="M52" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52" t="s">
+        <v>318</v>
+      </c>
+      <c r="P52" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="M52" s="7" t="s">
-        <v>390</v>
-      </c>
-      <c r="N52">
-        <v>1</v>
-      </c>
-      <c r="O52" t="s">
-        <v>321</v>
-      </c>
-      <c r="P52" s="1" t="s">
-        <v>371</v>
-      </c>
       <c r="Q52" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="R52">
         <v>1</v>
@@ -4303,21 +4302,21 @@
     <hyperlink ref="K23" r:id="rId12"/>
     <hyperlink ref="K24" r:id="rId13"/>
     <hyperlink ref="K25" r:id="rId14"/>
-    <hyperlink ref="K28" r:id="rId15"/>
-    <hyperlink ref="K27" r:id="rId16"/>
-    <hyperlink ref="K26" r:id="rId17"/>
-    <hyperlink ref="K29" r:id="rId18"/>
-    <hyperlink ref="K30" r:id="rId19"/>
-    <hyperlink ref="K31" r:id="rId20" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="K32" r:id="rId21" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
-    <hyperlink ref="K33" r:id="rId22" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="K34" r:id="rId23"/>
-    <hyperlink ref="K37" r:id="rId24"/>
-    <hyperlink ref="K48" r:id="rId25"/>
-    <hyperlink ref="K49" r:id="rId26"/>
-    <hyperlink ref="K50" r:id="rId27"/>
-    <hyperlink ref="K51" r:id="rId28"/>
-    <hyperlink ref="K52" r:id="rId29"/>
+    <hyperlink ref="K26" r:id="rId15"/>
+    <hyperlink ref="K29" r:id="rId16"/>
+    <hyperlink ref="K30" r:id="rId17"/>
+    <hyperlink ref="K31" r:id="rId18" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="K32" r:id="rId19" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
+    <hyperlink ref="K33" r:id="rId20" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="K34" r:id="rId21"/>
+    <hyperlink ref="K37" r:id="rId22"/>
+    <hyperlink ref="K48" r:id="rId23"/>
+    <hyperlink ref="K49" r:id="rId24"/>
+    <hyperlink ref="K50" r:id="rId25"/>
+    <hyperlink ref="K51" r:id="rId26"/>
+    <hyperlink ref="K52" r:id="rId27"/>
+    <hyperlink ref="K27" r:id="rId28"/>
+    <hyperlink ref="K28" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>

</xml_diff>

<commit_message>
* added (dummy) German description to programs.xlsx * added german program_name and description to json export
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="405">
   <si>
     <t>program_identifier</t>
   </si>
@@ -786,9 +786,6 @@
   </si>
   <si>
     <t>Caliendo et al. (2017)</t>
-  </si>
-  <si>
-    <t>Doerr et al. (2017);Huber et al. (2015)</t>
   </si>
   <si>
     <t>program_name_de</t>
@@ -1250,6 +1247,12 @@
   </si>
   <si>
     <t>Exploits staggered introduction across federal states. Discusses various potential sources of bias including self selection into treatment, political leadership. 3,2 because FE are not on unit of analysis level.</t>
+  </si>
+  <si>
+    <t>Doerr et al. (2017)</t>
+  </si>
+  <si>
+    <t>short_description_de</t>
   </si>
 </sst>
 </file>
@@ -1620,10 +1623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R52"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1633,17 +1636,17 @@
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
     <col min="6" max="6" width="66.85546875" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="45.140625" customWidth="1"/>
-    <col min="12" max="13" width="17.28515625" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" customWidth="1"/>
-    <col min="16" max="16" width="76.28515625" customWidth="1"/>
+    <col min="7" max="8" width="46.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="31.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="45.140625" customWidth="1"/>
+    <col min="13" max="14" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" customWidth="1"/>
+    <col min="17" max="17" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="45">
+    <row r="1" spans="1:20" ht="45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1654,7 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1666,40 +1669,44 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>359</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>301</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>300</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="150">
+        <v>299</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" ht="150">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1707,7 +1714,7 @@
         <v>167</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D2">
         <v>1990</v>
@@ -1721,41 +1728,44 @@
       <c r="G2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="1">
         <v>8868.6350000000002</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" t="s">
         <v>364</v>
       </c>
-      <c r="L2" t="s">
-        <v>365</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="N2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="R2" t="s">
         <v>302</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>303</v>
-      </c>
-      <c r="R2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="60">
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="60">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -1763,7 +1773,7 @@
         <v>162</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D3">
         <v>2001</v>
@@ -1777,41 +1787,44 @@
       <c r="G3" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="I3" s="1">
         <v>9056.3310000000001</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" t="s">
         <v>364</v>
       </c>
-      <c r="L3" t="s">
-        <v>365</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="R3" t="s">
         <v>302</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>303</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="60">
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="60">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1819,7 +1832,7 @@
         <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4">
         <v>2004</v>
@@ -1833,41 +1846,44 @@
       <c r="G4" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" s="1">
         <v>8886.7603079578239</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" t="s">
         <v>364</v>
       </c>
-      <c r="L4" t="s">
-        <v>365</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="N4" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="R4" t="s">
         <v>302</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>303</v>
-      </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="75">
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="75">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -1875,7 +1891,7 @@
         <v>166</v>
       </c>
       <c r="C5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D5">
         <v>2005</v>
@@ -1889,41 +1905,44 @@
       <c r="G5" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I5" s="1">
         <v>9022.8359999999993</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" t="s">
         <v>364</v>
       </c>
-      <c r="L5" t="s">
-        <v>365</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="N5" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="R5" t="s">
         <v>302</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>303</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="105">
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="105">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1931,7 +1950,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D6">
         <v>2013</v>
@@ -1945,36 +1964,39 @@
       <c r="G6" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" t="s">
+      <c r="H6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>388</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="M6" t="s">
         <v>389</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="L6" t="s">
-        <v>390</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="R6" t="s">
         <v>305</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>306</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="105">
+      <c r="S6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="105">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1982,7 +2004,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D7">
         <v>2011</v>
@@ -1996,36 +2018,39 @@
       <c r="G7" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
+      <c r="H7" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="N7" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="R7" t="s">
         <v>305</v>
       </c>
-      <c r="P7" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>306</v>
-      </c>
-      <c r="R7">
+      <c r="S7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="75">
+    <row r="8" spans="1:20" ht="75">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2033,7 +2058,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D8">
         <v>2011</v>
@@ -2047,36 +2072,39 @@
       <c r="G8" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="I8" s="1"/>
-      <c r="J8" t="s">
+      <c r="H8" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="M8" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="N8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="R8" t="s">
         <v>308</v>
       </c>
-      <c r="P8" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>309</v>
-      </c>
-      <c r="R8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="75">
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="75">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2084,7 +2112,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D9">
         <v>2008</v>
@@ -2098,36 +2126,39 @@
       <c r="G9" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I9" s="1"/>
-      <c r="J9" t="s">
-        <v>313</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="H9" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" t="s">
         <v>312</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="2" t="s">
         <v>311</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="R9" t="s">
         <v>308</v>
       </c>
-      <c r="P9" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>309</v>
-      </c>
-      <c r="R9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="150">
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="150">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2135,7 +2166,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D10">
         <v>1993</v>
@@ -2149,37 +2180,40 @@
       <c r="G10" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="I10" s="1">
         <v>1672</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" t="s">
+      <c r="J10" s="1"/>
+      <c r="K10" t="s">
         <v>154</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M10" s="1"/>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10" s="1" t="s">
+      <c r="N10" s="1"/>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="P10" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="30">
+      <c r="R10" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="30">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2187,7 +2221,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D11">
         <v>1993</v>
@@ -2201,37 +2235,40 @@
       <c r="G11" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I11" s="1">
         <v>1570</v>
       </c>
-      <c r="I11" s="1"/>
-      <c r="J11" t="s">
+      <c r="J11" s="1"/>
+      <c r="K11" t="s">
         <v>154</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M11" s="1"/>
-      <c r="N11">
-        <v>1</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>314</v>
+      <c r="N11" s="1"/>
+      <c r="O11">
+        <v>1</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18">
+        <v>315</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2239,7 +2276,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D12">
         <v>1993</v>
@@ -2253,37 +2290,40 @@
       <c r="G12" t="s">
         <v>216</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" t="s">
+        <v>216</v>
+      </c>
+      <c r="I12" s="1">
         <v>1434</v>
       </c>
-      <c r="I12" s="1"/>
-      <c r="J12" t="s">
+      <c r="J12" s="1"/>
+      <c r="K12" t="s">
         <v>154</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M12" s="1"/>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>314</v>
+      <c r="N12" s="1"/>
+      <c r="O12">
+        <v>1</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="45">
+        <v>315</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2291,7 +2331,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D13">
         <v>1993</v>
@@ -2303,39 +2343,42 @@
         <v>31</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="H13" s="1">
+        <v>357</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I13" s="1">
         <v>1558</v>
       </c>
-      <c r="I13" s="1"/>
-      <c r="J13" t="s">
+      <c r="J13" s="1"/>
+      <c r="K13" t="s">
         <v>154</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M13" s="1"/>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>314</v>
+      <c r="N13" s="1"/>
+      <c r="O13">
+        <v>1</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="75">
+        <v>315</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="75">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2343,7 +2386,7 @@
         <v>226</v>
       </c>
       <c r="C14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D14">
         <v>2000</v>
@@ -2357,37 +2400,40 @@
       <c r="G14" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I14" s="1">
         <v>1559.6189999999999</v>
       </c>
-      <c r="I14" s="1"/>
-      <c r="J14" t="s">
+      <c r="J14" s="1"/>
+      <c r="K14" t="s">
         <v>155</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="M14" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="M14" s="1"/>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>314</v>
+      <c r="N14" s="1"/>
+      <c r="O14">
+        <v>1</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="75">
+        <v>316</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="75">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2395,7 +2441,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D15">
         <v>2000</v>
@@ -2409,37 +2455,40 @@
       <c r="G15" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="I15" s="1">
         <v>1542.066</v>
       </c>
-      <c r="I15" s="1"/>
-      <c r="J15" t="s">
+      <c r="J15" s="1"/>
+      <c r="K15" t="s">
         <v>155</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="M15" s="1"/>
-      <c r="N15">
-        <v>1</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>314</v>
+      <c r="N15" s="1"/>
+      <c r="O15">
+        <v>1</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="60">
+        <v>316</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="60">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2447,7 +2496,7 @@
         <v>201</v>
       </c>
       <c r="C16" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D16">
         <v>2003</v>
@@ -2461,36 +2510,39 @@
       <c r="G16" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I16" s="1">
         <v>1459.3779999999999</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" t="s">
+      <c r="J16" s="1"/>
+      <c r="K16" t="s">
         <v>49</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>134</v>
       </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>314</v>
+      <c r="O16">
+        <v>1</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="90">
+        <v>333</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="90">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -2498,7 +2550,7 @@
         <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D17">
         <v>2003</v>
@@ -2512,36 +2564,39 @@
       <c r="G17" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I17" s="1">
         <v>2189.3620000000001</v>
       </c>
-      <c r="I17" s="1"/>
-      <c r="J17" t="s">
+      <c r="J17" s="1"/>
+      <c r="K17" t="s">
         <v>49</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="L17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>134</v>
       </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>314</v>
+      <c r="O17">
+        <v>1</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="105">
+        <v>333</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="105">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2549,7 +2604,7 @@
         <v>202</v>
       </c>
       <c r="C18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D18">
         <v>2009</v>
@@ -2563,35 +2618,38 @@
       <c r="G18" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="I18" s="1">
         <v>2047.962</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>156</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="L18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>119</v>
       </c>
-      <c r="N18">
-        <v>1</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>314</v>
+      <c r="O18">
+        <v>1</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="90">
+        <v>378</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="90">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -2599,7 +2657,7 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D19">
         <v>2003</v>
@@ -2613,38 +2671,41 @@
       <c r="G19" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="I19" s="1">
         <v>1901.21</v>
       </c>
-      <c r="J19" t="s">
-        <v>255</v>
-      </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" t="s">
+        <v>403</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
+        <v>365</v>
+      </c>
+      <c r="N19" t="s">
         <v>366</v>
       </c>
-      <c r="M19" t="s">
-        <v>367</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>314</v>
+      <c r="O19">
+        <v>1</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="180">
+        <v>317</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="180">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2663,26 +2724,26 @@
       <c r="G20" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="H20" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>53</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="L20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>122</v>
       </c>
-      <c r="M20" t="s">
-        <v>368</v>
-      </c>
-      <c r="N20">
+      <c r="N20" t="s">
+        <v>367</v>
+      </c>
+      <c r="O20">
         <v>0</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="P20" s="1" t="s">
         <v>320</v>
@@ -2690,11 +2751,14 @@
       <c r="Q20" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="S20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="180">
+    <row r="21" spans="1:19" ht="180">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -2713,26 +2777,26 @@
       <c r="G21" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="H21" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="L21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>122</v>
       </c>
-      <c r="M21" t="s">
-        <v>368</v>
-      </c>
-      <c r="N21">
+      <c r="N21" t="s">
+        <v>367</v>
+      </c>
+      <c r="O21">
         <v>0</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="P21" s="1" t="s">
         <v>320</v>
@@ -2740,11 +2804,14 @@
       <c r="Q21" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="S21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="120">
+    <row r="22" spans="1:19" ht="120">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -2752,7 +2819,7 @@
         <v>38</v>
       </c>
       <c r="C22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D22">
         <v>2005</v>
@@ -2766,32 +2833,35 @@
       <c r="G22" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="J22" t="s">
+      <c r="H22" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="K22" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>120</v>
       </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>314</v>
+      <c r="O22">
+        <v>1</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R22">
+        <v>321</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="90">
+    <row r="23" spans="1:19" ht="90">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -2799,7 +2869,7 @@
         <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D23">
         <v>2005</v>
@@ -2813,32 +2883,35 @@
       <c r="G23" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="J23" t="s">
+      <c r="H23" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K23" t="s">
         <v>54</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="L23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>120</v>
       </c>
-      <c r="N23">
-        <v>1</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>314</v>
+      <c r="O23">
+        <v>1</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R23">
+        <v>321</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="105">
+    <row r="24" spans="1:19" ht="105">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -2846,7 +2919,7 @@
         <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D24">
         <v>2005</v>
@@ -2860,32 +2933,35 @@
       <c r="G24" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J24" t="s">
+      <c r="H24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K24" t="s">
         <v>54</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="L24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>120</v>
       </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>314</v>
+      <c r="O24">
+        <v>1</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R24">
+        <v>321</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="45">
+    <row r="25" spans="1:19" ht="45">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2904,38 +2980,41 @@
       <c r="G25" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I25" t="s">
+      <c r="H25" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J25" t="s">
         <v>176</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>56</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="L25" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="M25" t="s">
         <v>123</v>
       </c>
-      <c r="M25" t="s">
-        <v>368</v>
-      </c>
-      <c r="N25">
+      <c r="N25" t="s">
+        <v>367</v>
+      </c>
+      <c r="O25">
         <v>0</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="Q25" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="R25">
+        <v>354</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="S25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="165">
+    <row r="26" spans="1:19" ht="165">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2943,7 +3022,7 @@
         <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D26">
         <v>1979</v>
@@ -2954,38 +3033,41 @@
       <c r="G26" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="I26" t="s">
+      <c r="H26" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J26" t="s">
         <v>169</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
+        <v>386</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>124</v>
       </c>
-      <c r="M26" t="s">
-        <v>373</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-      <c r="O26" t="s">
+      <c r="N26" t="s">
+        <v>372</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="165">
+      <c r="S26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="165">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -2993,7 +3075,7 @@
         <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D27">
         <v>1986</v>
@@ -3004,38 +3086,41 @@
       <c r="G27" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I27" t="s">
+      <c r="H27" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="J27" t="s">
         <v>169</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
+        <v>386</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="K27" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>124</v>
       </c>
-      <c r="M27" t="s">
-        <v>371</v>
-      </c>
-      <c r="N27">
-        <v>1</v>
-      </c>
-      <c r="O27" t="s">
+      <c r="N27" t="s">
+        <v>370</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="165">
+      <c r="S27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="165">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -3043,7 +3128,7 @@
         <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D28">
         <v>1992</v>
@@ -3057,38 +3142,41 @@
       <c r="G28" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="H28" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
+        <v>386</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="K28" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="M28" t="s">
         <v>124</v>
       </c>
-      <c r="M28" t="s">
-        <v>374</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-      <c r="O28" t="s">
+      <c r="N28" t="s">
+        <v>373</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P28" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="105">
+      <c r="S28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="105">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -3096,7 +3184,7 @@
         <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D29">
         <v>2013</v>
@@ -3110,32 +3198,35 @@
       <c r="G29" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="J29" t="s">
+      <c r="H29" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K29" t="s">
         <v>68</v>
       </c>
-      <c r="K29" s="2" t="s">
+      <c r="L29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="L29" t="s">
+      <c r="M29" t="s">
         <v>125</v>
       </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-      <c r="O29" t="s">
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="P29" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P29" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R29">
+      <c r="S29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="120">
+    <row r="30" spans="1:19" ht="120">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -3143,7 +3234,7 @@
         <v>71</v>
       </c>
       <c r="C30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D30">
         <v>2007</v>
@@ -3157,35 +3248,38 @@
       <c r="G30" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I30" s="1">
         <v>2235.6489999999999</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>72</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="L30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L30" t="s">
-        <v>324</v>
-      </c>
-      <c r="N30">
-        <v>1</v>
-      </c>
-      <c r="O30" t="s">
+      <c r="M30" t="s">
+        <v>323</v>
+      </c>
+      <c r="O30">
+        <v>1</v>
+      </c>
+      <c r="P30" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="R30" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R30">
+      <c r="S30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:18" ht="120">
+    <row r="31" spans="1:19" ht="120">
       <c r="A31" t="s">
         <v>184</v>
       </c>
@@ -3201,32 +3295,35 @@
       <c r="G31" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="H31" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>74</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="L31" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="L31" t="s">
+      <c r="M31" t="s">
         <v>126</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>0</v>
       </c>
-      <c r="O31" t="s">
+      <c r="P31" t="s">
         <v>160</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="R31">
+      <c r="Q31" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="S31">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="75">
+    <row r="32" spans="1:19" ht="75">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -3234,7 +3331,7 @@
         <v>135</v>
       </c>
       <c r="C32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D32">
         <v>1990</v>
@@ -3248,35 +3345,38 @@
       <c r="G32" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="J32" t="s">
+      <c r="H32" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K32" t="s">
         <v>78</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="L32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" t="s">
         <v>127</v>
       </c>
-      <c r="M32" t="s">
-        <v>375</v>
-      </c>
-      <c r="N32">
-        <v>1</v>
-      </c>
-      <c r="O32" t="s">
-        <v>308</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>327</v>
+      <c r="N32" t="s">
+        <v>374</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
+        <v>307</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="S32">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="75">
+    <row r="33" spans="1:19" ht="75">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -3298,35 +3398,38 @@
       <c r="G33" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="J33" t="s">
+      <c r="H33" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="K33" t="s">
         <v>81</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="L33" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="L33" t="s">
+      <c r="M33" t="s">
         <v>128</v>
       </c>
-      <c r="M33" t="s">
-        <v>376</v>
-      </c>
-      <c r="N33">
-        <v>1</v>
-      </c>
-      <c r="O33" t="s">
-        <v>308</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>328</v>
+      <c r="N33" t="s">
+        <v>375</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+      <c r="P33" t="s">
+        <v>307</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="R33">
+        <v>327</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="S33">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" ht="135">
+    <row r="34" spans="1:19" ht="135">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -3334,7 +3437,7 @@
         <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D34">
         <v>1993</v>
@@ -3348,35 +3451,38 @@
       <c r="G34" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I34" s="1">
         <v>1934.5</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>85</v>
       </c>
-      <c r="K34" s="2" t="s">
+      <c r="L34" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" t="s">
         <v>129</v>
       </c>
-      <c r="N34">
-        <v>1</v>
-      </c>
-      <c r="O34" t="s">
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q34" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="P34" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="R34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="135">
+      <c r="R34" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="135">
       <c r="A35" t="s">
         <v>88</v>
       </c>
@@ -3384,7 +3490,7 @@
         <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D35">
         <v>1993</v>
@@ -3398,35 +3504,38 @@
       <c r="G35" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I35" s="1">
         <v>1928.4169999999999</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>85</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="L35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L35" t="s">
+      <c r="M35" t="s">
         <v>129</v>
       </c>
-      <c r="N35">
-        <v>1</v>
-      </c>
-      <c r="O35" t="s">
+      <c r="O35">
+        <v>1</v>
+      </c>
+      <c r="P35" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q35" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="P35" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="R35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="135">
+      <c r="R35" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="S35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="135">
       <c r="A36" t="s">
         <v>89</v>
       </c>
@@ -3434,7 +3543,7 @@
         <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D36">
         <v>1993</v>
@@ -3448,35 +3557,38 @@
       <c r="G36" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I36" s="1">
         <v>1925.375</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>85</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="L36" t="s">
+      <c r="M36" t="s">
         <v>129</v>
       </c>
-      <c r="N36">
-        <v>1</v>
-      </c>
-      <c r="O36" t="s">
+      <c r="O36">
+        <v>1</v>
+      </c>
+      <c r="P36" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q36" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="P36" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="R36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="120">
+      <c r="R36" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="S36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="120">
       <c r="A37" t="s">
         <v>90</v>
       </c>
@@ -3484,7 +3596,7 @@
         <v>91</v>
       </c>
       <c r="C37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D37">
         <v>2002</v>
@@ -3498,35 +3610,38 @@
       <c r="G37" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="I37" s="1">
         <v>1999.866</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>93</v>
       </c>
-      <c r="K37" s="2" t="s">
+      <c r="L37" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
         <v>130</v>
       </c>
-      <c r="N37">
-        <v>1</v>
-      </c>
-      <c r="O37" t="s">
-        <v>329</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>331</v>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37" t="s">
+        <v>328</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="R37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="135">
+        <v>330</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="135">
       <c r="A38" t="s">
         <v>106</v>
       </c>
@@ -3534,7 +3649,7 @@
         <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D38">
         <v>2006</v>
@@ -3548,35 +3663,38 @@
       <c r="G38" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="J38" t="s">
-        <v>381</v>
-      </c>
-      <c r="K38" s="2" t="s">
+      <c r="H38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K38" t="s">
+        <v>380</v>
+      </c>
+      <c r="L38" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="L38" t="s">
+      <c r="M38" t="s">
+        <v>376</v>
+      </c>
+      <c r="N38" t="s">
         <v>377</v>
       </c>
-      <c r="M38" t="s">
-        <v>378</v>
-      </c>
-      <c r="N38">
-        <v>1</v>
-      </c>
-      <c r="O38" t="s">
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="P38" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="R38" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P38" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R38">
+      <c r="S38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="75">
+    <row r="39" spans="1:19" ht="75">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -3584,7 +3702,7 @@
         <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D39">
         <v>2011</v>
@@ -3598,35 +3716,38 @@
       <c r="G39" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="I39" s="1">
         <v>1593.2249999999999</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="K39" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="K39" s="2" t="s">
+      <c r="L39" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L39" t="s">
+      <c r="M39" t="s">
         <v>131</v>
       </c>
-      <c r="N39">
-        <v>1</v>
-      </c>
-      <c r="O39" t="s">
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="P39" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="R39" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="P39" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="R39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="60">
+      <c r="S39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="60">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -3634,7 +3755,7 @@
         <v>101</v>
       </c>
       <c r="C40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D40">
         <v>2006</v>
@@ -3648,35 +3769,38 @@
       <c r="G40" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I40" s="1">
         <v>2624.9580000000001</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>254</v>
       </c>
-      <c r="K40" s="2" t="s">
+      <c r="L40" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L40" t="s">
+      <c r="M40" t="s">
         <v>133</v>
       </c>
-      <c r="N40">
-        <v>1</v>
-      </c>
-      <c r="O40" t="s">
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="P40" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="R40" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="P40" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="R40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" ht="90">
+      <c r="S40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="90">
       <c r="A41" t="s">
         <v>105</v>
       </c>
@@ -3694,37 +3818,40 @@
         <v>37.630000000000003</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="I41">
+        <v>2731</v>
+      </c>
+      <c r="K41" s="5" t="s">
         <v>395</v>
       </c>
-      <c r="H41">
-        <v>2731</v>
-      </c>
-      <c r="J41" s="5" t="s">
+      <c r="L41" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="M41" t="s">
         <v>396</v>
       </c>
-      <c r="K41" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="L41" t="s">
-        <v>397</v>
-      </c>
-      <c r="N41">
+      <c r="O41">
         <v>0</v>
       </c>
-      <c r="O41" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="P41" s="1" t="s">
-        <v>336</v>
+        <v>313</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" ht="195">
+        <v>335</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="195">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -3732,7 +3859,7 @@
         <v>110</v>
       </c>
       <c r="C42" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D42">
         <v>2001</v>
@@ -3746,35 +3873,38 @@
       <c r="G42" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="I42" s="1">
         <v>1278.2249999999999</v>
       </c>
-      <c r="J42" s="6" t="s">
+      <c r="K42" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="L42" t="s">
+      <c r="M42" t="s">
         <v>132</v>
       </c>
-      <c r="N42">
-        <v>1</v>
-      </c>
-      <c r="O42" t="s">
-        <v>305</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>339</v>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>304</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="R42">
+        <v>338</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="S42">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="90">
+    <row r="43" spans="1:19" ht="90">
       <c r="A43" t="s">
         <v>112</v>
       </c>
@@ -3782,7 +3912,7 @@
         <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D43">
         <v>2009</v>
@@ -3796,35 +3926,38 @@
       <c r="G43" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I43" s="1">
         <v>1543.018</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="K43" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="L43" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="K43" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="L43" t="s">
-        <v>399</v>
-      </c>
-      <c r="N43">
-        <v>1</v>
-      </c>
-      <c r="O43" t="s">
-        <v>305</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>369</v>
+      <c r="M43" t="s">
+        <v>398</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
+      </c>
+      <c r="P43" t="s">
+        <v>304</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="R43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="150">
+        <v>368</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="150">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -3832,7 +3965,7 @@
         <v>137</v>
       </c>
       <c r="C44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D44">
         <v>2005</v>
@@ -3846,35 +3979,38 @@
       <c r="G44" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I44" s="1">
         <v>2004.07</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>139</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="L44" t="s">
+      <c r="M44" t="s">
         <v>138</v>
       </c>
-      <c r="N44">
-        <v>1</v>
-      </c>
-      <c r="O44" t="s">
-        <v>329</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>402</v>
+      <c r="O44">
+        <v>1</v>
+      </c>
+      <c r="P44" t="s">
+        <v>328</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="105">
+        <v>401</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="105">
       <c r="A45" t="s">
         <v>143</v>
       </c>
@@ -3882,7 +4018,7 @@
         <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D45">
         <v>2012</v>
@@ -3896,35 +4032,38 @@
       <c r="G45" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I45" s="1">
         <v>994.59460000000001</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="K45" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="L45" t="s">
+      <c r="M45" t="s">
         <v>142</v>
       </c>
-      <c r="N45">
-        <v>1</v>
-      </c>
-      <c r="O45" t="s">
+      <c r="O45">
+        <v>1</v>
+      </c>
+      <c r="P45" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="R45" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P45" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" ht="135">
+      <c r="S45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" ht="135">
       <c r="A46" t="s">
         <v>145</v>
       </c>
@@ -3932,7 +4071,7 @@
         <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D46">
         <v>2012</v>
@@ -3946,39 +4085,42 @@
       <c r="G46" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="I46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>150</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>149</v>
       </c>
-      <c r="N46">
-        <v>1</v>
-      </c>
-      <c r="O46" t="s">
-        <v>341</v>
-      </c>
-      <c r="P46" s="1" t="s">
-        <v>357</v>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46" t="s">
+        <v>340</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="135">
+        <v>356</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="135">
       <c r="A47" t="s">
         <v>151</v>
       </c>
@@ -3986,7 +4128,7 @@
         <v>152</v>
       </c>
       <c r="C47" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D47">
         <v>2012</v>
@@ -4000,39 +4142,42 @@
       <c r="G47" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
         <v>2928.3125</v>
       </c>
-      <c r="I47" s="1" t="s">
+      <c r="J47" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>150</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="L47" t="s">
+      <c r="M47" t="s">
         <v>149</v>
       </c>
-      <c r="N47">
-        <v>1</v>
-      </c>
-      <c r="O47" t="s">
-        <v>341</v>
-      </c>
-      <c r="P47" s="1" t="s">
-        <v>357</v>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47" t="s">
+        <v>340</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="105">
+        <v>356</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="S47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" ht="105">
       <c r="A48" t="s">
         <v>231</v>
       </c>
@@ -4040,7 +4185,7 @@
         <v>232</v>
       </c>
       <c r="C48" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D48">
         <v>1967</v>
@@ -4054,36 +4199,39 @@
       <c r="G48" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="I48" s="1"/>
-      <c r="J48" t="s">
-        <v>345</v>
-      </c>
-      <c r="K48" s="2" t="s">
+      <c r="H48" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J48" s="1"/>
+      <c r="K48" t="s">
+        <v>344</v>
+      </c>
+      <c r="L48" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="L48" t="s">
-        <v>343</v>
-      </c>
-      <c r="M48" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="N48">
-        <v>1</v>
-      </c>
-      <c r="O48" t="s">
+      <c r="M48" t="s">
+        <v>342</v>
+      </c>
+      <c r="N48" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="P48" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="R48" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P48" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="Q48" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="120">
+      <c r="S48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" ht="120">
       <c r="A49" t="s">
         <v>235</v>
       </c>
@@ -4091,7 +4239,7 @@
         <v>234</v>
       </c>
       <c r="C49" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D49">
         <v>2003</v>
@@ -4105,35 +4253,38 @@
       <c r="G49" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J49" t="s">
-        <v>344</v>
-      </c>
-      <c r="K49" s="2" t="s">
+      <c r="H49" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="K49" t="s">
+        <v>343</v>
+      </c>
+      <c r="L49" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="L49" t="s">
-        <v>346</v>
-      </c>
       <c r="M49" t="s">
-        <v>373</v>
-      </c>
-      <c r="N49">
-        <v>1</v>
-      </c>
-      <c r="O49" t="s">
+        <v>345</v>
+      </c>
+      <c r="N49" t="s">
+        <v>372</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+      <c r="P49" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="R49" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P49" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="Q49" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="75">
+      <c r="S49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" ht="75">
       <c r="A50" t="s">
         <v>236</v>
       </c>
@@ -4141,7 +4292,7 @@
         <v>237</v>
       </c>
       <c r="C50" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D50">
         <v>1957</v>
@@ -4155,35 +4306,38 @@
       <c r="G50" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="J50" s="1" t="s">
+      <c r="H50" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="K50" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="L50" s="7" t="s">
-        <v>347</v>
-      </c>
       <c r="M50" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="N50">
-        <v>1</v>
-      </c>
-      <c r="O50" t="s">
-        <v>308</v>
-      </c>
-      <c r="P50" s="1" t="s">
-        <v>403</v>
+        <v>346</v>
+      </c>
+      <c r="N50" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+      <c r="P50" t="s">
+        <v>307</v>
       </c>
       <c r="Q50" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="R50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" ht="105">
+        <v>402</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="S50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="105">
       <c r="A51" t="s">
         <v>243</v>
       </c>
@@ -4191,7 +4345,7 @@
         <v>244</v>
       </c>
       <c r="C51" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D51">
         <v>2017</v>
@@ -4205,35 +4359,38 @@
       <c r="G51" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="J51" t="s">
+      <c r="H51" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K51" t="s">
         <v>242</v>
       </c>
-      <c r="K51" s="2" t="s">
+      <c r="L51" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="L51" t="s">
-        <v>348</v>
-      </c>
       <c r="M51" t="s">
-        <v>373</v>
-      </c>
-      <c r="N51">
-        <v>1</v>
-      </c>
-      <c r="O51" t="s">
+        <v>347</v>
+      </c>
+      <c r="N51" t="s">
+        <v>372</v>
+      </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="P51" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="R51" t="s">
         <v>305</v>
       </c>
-      <c r="P51" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>306</v>
-      </c>
-      <c r="R51">
+      <c r="S51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" ht="135">
+    <row r="52" spans="1:19" ht="135">
       <c r="A52" t="s">
         <v>246</v>
       </c>
@@ -4241,7 +4398,7 @@
         <v>247</v>
       </c>
       <c r="C52" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D52">
         <v>1978</v>
@@ -4255,67 +4412,70 @@
       <c r="G52" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="H52" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="K52" s="2" t="s">
+      <c r="L52" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="L52" s="7" t="s">
-        <v>349</v>
-      </c>
       <c r="M52" s="7" t="s">
-        <v>371</v>
-      </c>
-      <c r="N52">
-        <v>1</v>
-      </c>
-      <c r="O52" t="s">
+        <v>348</v>
+      </c>
+      <c r="N52" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
+      <c r="P52" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="R52" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="P52" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="Q52" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="R52">
+      <c r="S52">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K6" r:id="rId1"/>
-    <hyperlink ref="K7" r:id="rId2"/>
-    <hyperlink ref="K9" r:id="rId3"/>
-    <hyperlink ref="K8" r:id="rId4"/>
-    <hyperlink ref="K14" r:id="rId5"/>
-    <hyperlink ref="K15" r:id="rId6"/>
-    <hyperlink ref="K18" r:id="rId7"/>
-    <hyperlink ref="K19" r:id="rId8"/>
-    <hyperlink ref="K20" r:id="rId9"/>
-    <hyperlink ref="K21" r:id="rId10"/>
-    <hyperlink ref="K22" r:id="rId11"/>
-    <hyperlink ref="K23" r:id="rId12"/>
-    <hyperlink ref="K24" r:id="rId13"/>
-    <hyperlink ref="K25" r:id="rId14"/>
-    <hyperlink ref="K26" r:id="rId15"/>
-    <hyperlink ref="K29" r:id="rId16"/>
-    <hyperlink ref="K30" r:id="rId17"/>
-    <hyperlink ref="K31" r:id="rId18" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="K32" r:id="rId19" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
-    <hyperlink ref="K33" r:id="rId20" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
-    <hyperlink ref="K34" r:id="rId21"/>
-    <hyperlink ref="K37" r:id="rId22"/>
-    <hyperlink ref="K48" r:id="rId23"/>
-    <hyperlink ref="K49" r:id="rId24"/>
-    <hyperlink ref="K50" r:id="rId25"/>
-    <hyperlink ref="K51" r:id="rId26"/>
-    <hyperlink ref="K52" r:id="rId27"/>
-    <hyperlink ref="K27" r:id="rId28"/>
-    <hyperlink ref="K28" r:id="rId29"/>
-    <hyperlink ref="K41" r:id="rId30"/>
-    <hyperlink ref="K43" r:id="rId31"/>
+    <hyperlink ref="L6" r:id="rId1"/>
+    <hyperlink ref="L7" r:id="rId2"/>
+    <hyperlink ref="L9" r:id="rId3"/>
+    <hyperlink ref="L8" r:id="rId4"/>
+    <hyperlink ref="L14" r:id="rId5"/>
+    <hyperlink ref="L15" r:id="rId6"/>
+    <hyperlink ref="L18" r:id="rId7"/>
+    <hyperlink ref="L19" r:id="rId8"/>
+    <hyperlink ref="L20" r:id="rId9"/>
+    <hyperlink ref="L21" r:id="rId10"/>
+    <hyperlink ref="L22" r:id="rId11"/>
+    <hyperlink ref="L23" r:id="rId12"/>
+    <hyperlink ref="L24" r:id="rId13"/>
+    <hyperlink ref="L25" r:id="rId14"/>
+    <hyperlink ref="L26" r:id="rId15"/>
+    <hyperlink ref="L29" r:id="rId16"/>
+    <hyperlink ref="L30" r:id="rId17"/>
+    <hyperlink ref="L31" r:id="rId18" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="L32" r:id="rId19" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/_x000a_"/>
+    <hyperlink ref="L33" r:id="rId20" display="https://ideas.repec.org/a/eee/pubeco/v151y2017icp41-55.html;https://wid.world/"/>
+    <hyperlink ref="L34" r:id="rId21"/>
+    <hyperlink ref="L37" r:id="rId22"/>
+    <hyperlink ref="L48" r:id="rId23"/>
+    <hyperlink ref="L49" r:id="rId24"/>
+    <hyperlink ref="L50" r:id="rId25"/>
+    <hyperlink ref="L51" r:id="rId26"/>
+    <hyperlink ref="L52" r:id="rId27"/>
+    <hyperlink ref="L27" r:id="rId28"/>
+    <hyperlink ref="L28" r:id="rId29"/>
+    <hyperlink ref="L41" r:id="rId30"/>
+    <hyperlink ref="L43" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId32"/>

</xml_diff>

<commit_message>
* Deutsche Kurzbeschreibungen hinzugefügt
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7800"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="450">
   <si>
     <t>program_identifier</t>
   </si>
@@ -1253,6 +1253,142 @@
   </si>
   <si>
     <t>short_description_de</t>
+  </si>
+  <si>
+    <t>Im Jahr 1990 wurde der Spitzensteuersatz der deutschen Einkommenssteuer von 56% auf 53% gesenkt.</t>
+  </si>
+  <si>
+    <t>Zwischen 1999 and 2001 wurde der Spitzensteuersatz schrittweise von 53% auf 48,5% gesenkt. Dies war die erste einer Reihe von Absenkungen des Spitzensteuersatztes in der ersten Hälfte der 2000 Jahre.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2004 wurde der Spitzensteuersatz der Einkommenssteuer von 48,5% to 45% gesenkt. Die Reform war Teil einer Reihe von schrittweisen Absenkungen des Spitzensteuersatzes zwischen 1999 und 2005.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2005, wurde der Spitzensteuersatz von 45% auf 42% gesenkt. Mit Ausnahme der Einführung der oft als Reichensteuer bezeichneten Steuer für Einkommen die 250.000 Euro pro Jahr übsterigen war dies die bis heute letzte Anpassung des Spitzensteuersatzes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im Rahmen eines randomisierten Feldexperimentes wurde die Auswirkung eines Workshops zu den Chancen eines Hochschulstudiums auf die Wahrscheinlichkeit ein Studium aufzunehmen untersucht.
+</t>
+  </si>
+  <si>
+    <t>Grundschülern, die aus Familien mit niedrigem sozioökonomischem Status stammen, wurden im Rahmen des Programms “Balu und Du” einem Mentor zugewiesen. Teilnahme an "Balu und Du" erhöhte die Wahrscheinlichkeit die 10. Klasse eines Gymnasiums zu Besuchen um 10,3 Prozentpunkte.</t>
+  </si>
+  <si>
+    <t>In den Jahren 2007 bis 2013 verkürzten einige Bundesländer das Gymnasium von neun auf acht Jahre. Die G8 Reform reduzierte den Anteil der Schulabgänger die ein Studium aufnahmen.</t>
+  </si>
+  <si>
+    <t>In den Jahren 2006 and 2007 führten einige Bundesländer (darunter die fünf bevölkerungsreichsten Bundesländer) Studiengebühren von circa  1000 Euro pro Jahr ein. Die Studiengebühren wurden in allen Bundesländern wieder abgeschafft. Als Letztes geschah dies in Sachsen-Anhalt im Jahr 2015.</t>
+  </si>
+  <si>
+    <t>Unter lange Trainingsprogramme fallen meist in Vollzeit stattfindene Trainingsprogramme um  beruflichen Kenntnisse und andere Fähigkeiten zu erweitern damit Beschäftigungsaussichten verbessert werden können.</t>
+  </si>
+  <si>
+    <t>Kurze Trainingsprogramme umfassen eine Reihe von Weiterbildungsprogrammen für Beschäftigungssuchende deren Dauer niedriger als sechs Monate ist.</t>
+  </si>
+  <si>
+    <t>Durch die Beschäftigung in einer Übungsfirma wurden Tätigkeiten in einem bestimmten Berufsfeld simuliert. Dabei sollen die Fähigkeiten, die an einem echten Arbeitsplatz benötigt werden, erlernt und ausgebaut werden. Ziel ist es die Reintegration in den Arbeitsmarkt für Arbeitssuchende zu erleichtern.</t>
+  </si>
+  <si>
+    <t>Eine berufliche Neuausrichtung umfasst ein längerfristige Ausbildung von bis zu drei Jahre um einen Berufsabschluss in einem neuen Tätigkeitsbereich zu erlangen</t>
+  </si>
+  <si>
+    <t>Berufliche Weiterbildungen umfassen Aktivitäten zum Ausbau von beruflichen Kompetenzen. Sowohl Präsenzunterricht, Schulungen am Arbeitsplatz oder die Arbeit an einer Übungsfirma können Teil einer staatlich finanzierten beruflichen Weiterbildung für Arbeitssuchende sein.</t>
+  </si>
+  <si>
+    <t>Unter Trainingsmaßnahmen fallen eine Reihe von Trainingsprogrammen mit einer kurzen Laufzeit von zwei bis zwölf Wochen (Im Durchschnitt etwas mehr als 4 Wochen). Die Trainingsmaßnahmen sollen helfen den Wiedereinstieg in den Arbeitsmarkt zu ermöglichen.</t>
+  </si>
+  <si>
+    <t>Der Existenzgründungszuschuss war eine staatliche Subvention die für  3  Jahre Gründer unterstützte die sich zuvor in Arbeitslosigkeit befanden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Das Überbrückungsgeld war eine staatliche Transferleistung die an Gründer gezahlt wurde, die andernfalls Anspruch auf Arbeitslosengeld oder eine staatlich finanzierte Weiterbildungsmaßnahme hätten. The bridging allowance was paid for 6 months.</t>
+  </si>
+  <si>
+    <t>Der Gründungszuschuss löste im Jahr 2006 die beiden bisherigen Förderprogramme zur Existenzgründung um Arbeitslosugkeit zu vermeiden  (Überbrückungsgeld &amp; Existenzgründungszuschuss) ab. Die Höhe des Zuschuss belief sich auf die invidiuellen Arbeitslosengeldansprüche für 6 Monate und weitere 300 Euro für bis zu 15 Monate.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2003 wurde ein Gutscheinsystem für die Vergabe von öffentlich finanzierten Trainings- und Fortbildungsprogrammen eingeführt.</t>
+  </si>
+  <si>
+    <t>Arbeitsbeschaffungsmaßnahmen waren ein Element der aktiven Arbeitsmarktpolitik, das Arbeitssuchenden die Möglichkeit gab eine temporäre, meist auf 12 Monate befristete Tätigkeiten auszuüben, um die Chancen auf Wiedereingliederung in den Arbeitsmarkt zu verbessern.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein-Euro-Jobs, formal Arbeitsgelegenheiten mit Mehraufwandsentschädigung, sind Arbeitsplätze, die Langzeitarbeitslosen vermittelt werden, um sie bei der Wiedereingliederung in den Arbeitsmarkt zu unterstützen. </t>
+  </si>
+  <si>
+    <t>Arbeitsgelegenheiten, formal Arbeitsgelegenheiten in der Entgeltvariante, stellen neben den Ein-Euro-Jobs eine weitere von der Arbeitsagentur subventionierte und befristete Beschäftigungsmöglichkeit dar.</t>
+  </si>
+  <si>
+    <t>Im Jahr 1979 wurde das sogenannte Mutterschaftsurlaubsgeld eingeführt. Dieses umfasste eine gesetzlich garantierte Rückkehr zur bisherigen Arbeitsstelle und ein Mutterschaftsgeld in Höhe von 750 Mark für bis zu sechs Monate nach der Geburt.</t>
+  </si>
+  <si>
+    <t>Das Erziehungsgeld wurde im Jahr 1986 eingeführt und löste das Mutterschaftsurlaubsgeld ab.  Die Bezugsdauer und der Kündigungsschutz wurde um 4 Monate verlängert. Die Höhe des staatlichen Transfers wurde auf 600 Mark reduziert (von zuvor 750 Mark).</t>
+  </si>
+  <si>
+    <t>m Jahr 1992 wurde der besondere Kündigungsschutz für Mütter, welcher das Recht zur Rückkehr an den bisherigen Arbeitsplatz garantiert, von 18 Monate nach der Geburt auf 36 Monate nach der Geburt ausgeweitet. Staatliche Tranfers blieben unverändert.</t>
+  </si>
+  <si>
+    <t>Das Betreungsgeld wurde 2013 für Elterrn eingeführt die nicht nicht von staatlich subventionierter Kinderbetreung gebrauch machen. Es umfasste eine monatliche Zahlung von 100€ für bis zu 22 Monate. Im Jahr 2015 wurde das Betreuungsgeld in Folge eines Urteils des Bundesverfassungsgerichts wieder abgeschafft.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2007 löste das Elterngeld das Erziehungsgeld ab. Die Höhe des Elterngeldes orientiert sich am Nettoeinkommen des jeweiligen Elternteils der das Elterngeld in Anspruch nimmt. Die maximale Bezugsdauer wurde verglichen mit dem Erziehungsgeld auf 12 Monate halbiert. Dennoch ist die Summe der erhaltenen Leistungen für die meisten Eltern höher als unter dem alten System.</t>
+  </si>
+  <si>
+    <t>Im Jahr 1990  wurde das BAföG grundlegend reformiert. Zuvor musste das gesamte Darlehen zurückgezahlt werden. Seit 1990 wird im Regelfall etwa die Hälfte des Darlehens als Zuschuss gewährt und muss somit nicht zurückgezahlt werden.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2001 wurde die Einkommensgrenze der Eltern bis zu der Studienrende BAföG beziehen konnten um 20 Prozent angehoben. Dadruch stieg die Anzahl der BAföG Berechtigten um circa 50 Prozent.</t>
+  </si>
+  <si>
+    <t>Das deutsche Arbeitslosenversicherungssystem weist einige Sprungsstellen auf an welchen sich abhängig vom Alter die maximale Bezugsdauer ändert.  Dadurch lassen sich Rückschlüsse über den Anreizeffekt der Arbeitslosenversicherung schließen und es kann ein MVPF für die Ausweitung der Bezugsdauer im Alter von 42 berechnet werden.</t>
+  </si>
+  <si>
+    <t>Das deutsche Arbeitslosenversicherungssystem weist einige Sprungsstellen auf an welchen sich abhängig vom Alter die maximale Bezugsdauer ändert.  Dadurch lassen sich Rückschlüsse über den Anreizeffekt der Arbeitslosenversicherung schließen und es kann ein MVPF für die Ausweitung der Bezugsdauer im Alter von 44 berechnet werden.</t>
+  </si>
+  <si>
+    <t>Das deutsche Arbeitslosenversicherungssystem weist einige Sprungsstellen auf an welchen sich abhängig vom Alter die maximale Bezugsdauer ändert.  Dadurch lassen sich Rückschlüsse über den Anreizeffekt der Arbeitslosenversicherung schließen und es kann ein MVPF für die Ausweitung der Bezugsdauer im Alter von 49 berechnet werden.</t>
+  </si>
+  <si>
+    <t>Das deutsche Arbeitslosenversicherungssystem weist einige Sprungsstellen auf an welchen sich abhängig vom Alter die maximale Bezugsdauer ändert.  Dadurch lassen sich Rückschlüsse über den Anreizeffekt der Arbeitslosenversicherung schließen und es kann ein MVPF für die Ausweitung der Bezugsdauer im Alter von 45 berechnet werden.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2006 wurde die Bezugsdauer des Arbeitslosengeldes im Rahmen der Hartz-Reformen gekürzt. Zur Identfikation des Effekts wurden betroffene Altersgruppen mit nicht betroffenen Altersgruppen verglichen. Außerdem beschränkt sich der Effekt auf Personen mit gesundheitlichen Beeinträchtigungen.</t>
+  </si>
+  <si>
+    <t>Im Rahmen eines randomisierten Feldexperimentes wurde ine Informationsbroschüre, die über Strategien zur Jobsuche und die negativen Auswirkungen von Arbeitslosigkeit aufklärt, an neu registrierte Arbeitssuchende verschickt.</t>
+  </si>
+  <si>
+    <t>Arbeitssuchende die im lokalen Arbeitsmarkt keine Beschäftigung finden können entwerder Umzugskosten erstattet bekommen oder eine Subvention für eine Wohnung an ihrem neuen Arbeitsplatz erhalten.</t>
+  </si>
+  <si>
+    <t>An zwei Arbeitsagenturen in Deutschland wurden Arbeitssuchende entweder einem privaten Dienstleister oder einem internen Team zur Stellenvermittlung zugeordnet. Die interne Stellenvermittlung führte zu höhren Einkommen und höheren Kosten für die Arbeitsagentur.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2012 wurden lokale Jobcenter, die bisher im Zuständigkeitsbereich der Bundesagentur für Arbeit waren, dezentralisiert und dem Landkreis unterstellt.</t>
+  </si>
+  <si>
+    <t>Seit dem Jahr 2007 verschickt die deutsche Rentenversicherung Briefe, die über die gemäß der aktuell und zuvor geleisteten Beiträge über zu erwartende Rentenansprüche informiert. Da nur Personen die 27 oder älter sind einen solchen Brief erhielten, ließ sich der Effekt des Erhalts des Briefs  bestimmen.</t>
+  </si>
+  <si>
+    <t>In Deutschland wird Windstrom unter dem Erneuerbare Energien Gesetz (EEG) subventioniert. Auf Basis der implizierte CO2 Vermeidungskosten kann ein MVPF berechnet werden.</t>
+  </si>
+  <si>
+    <t>In Deutschland wird Solarstrom unter dem Erneuerbare Energien Gesetz (EEG) subventioniert. Auf Basis der implizierte CO2 Vermeidungskosten kann ein MVPF berechnet werden.</t>
+  </si>
+  <si>
+    <t>Zwischen 1946 und 1969 wurde in allen deutschen Bundesländern die Dauer der Haupt bzw. Mittelschule um ein Jahr ausgeweitet. Relevante Effekte treten lediglich eine Generation später auf.</t>
+  </si>
+  <si>
+    <t>Im Jahr 2000 wurde die Aufteilung von Real und Hauptschule in Bayern von der sechsten in die vierte Klasse vorverlegt. Es zeigte sich ein negativer Effekt auf PISA Scores.</t>
+  </si>
+  <si>
+    <t>In den Jahren 1947 bis 1962 wurden in allen Bundesländern Schulgebühren abgeschafft. Dies hatte einen positiven Effekt auf den Anteil der Schüler die das Gymnasium besuchen.</t>
+  </si>
+  <si>
+    <t>Rock your Life ist ein Mentoringprogramm für Schüler, die eine achte oder neunte Klasse der Haupt- oder Mittelschule besuchen. Das Mentoringprogramm wird an ausgewählten Schulen in tendenziell benachteiligten Stadtbezirken angeboten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zwischen 1965 und 1996 wurde in allen deutschen Bundesländern die mittlere Reife, also der Realschulabschluss als Zwischenabschluss des Gymnasiums eingeführt. Mit erfolgreicher Beendigung der 10. Klasse erhalten Schüler die mittlere Reife, auch wenn sie die Oberstufe des Gymnasiums nicht abschließen. </t>
   </si>
 </sst>
 </file>
@@ -1625,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H52"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1729,7 +1865,7 @@
         <v>186</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>186</v>
+        <v>405</v>
       </c>
       <c r="I2" s="1">
         <v>8868.6350000000002</v>
@@ -1765,7 +1901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="60">
+    <row r="3" spans="1:20" ht="75">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -1788,7 +1924,7 @@
         <v>211</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>211</v>
+        <v>406</v>
       </c>
       <c r="I3" s="1">
         <v>9056.3310000000001</v>
@@ -1824,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="60">
+    <row r="4" spans="1:20" ht="75">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1847,7 +1983,7 @@
         <v>187</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>187</v>
+        <v>407</v>
       </c>
       <c r="I4" s="1">
         <v>8886.7603079578239</v>
@@ -1883,7 +2019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="75">
+    <row r="5" spans="1:20" ht="90">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -1906,7 +2042,7 @@
         <v>212</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>212</v>
+        <v>408</v>
       </c>
       <c r="I5" s="1">
         <v>9022.8359999999993</v>
@@ -1965,7 +2101,7 @@
         <v>188</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>188</v>
+        <v>409</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" t="s">
@@ -2019,7 +2155,7 @@
         <v>215</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>215</v>
+        <v>410</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
@@ -2073,7 +2209,7 @@
         <v>192</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>192</v>
+        <v>411</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" t="s">
@@ -2104,7 +2240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="75">
+    <row r="9" spans="1:20" ht="105">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2127,7 +2263,7 @@
         <v>193</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>193</v>
+        <v>412</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" t="s">
@@ -2181,7 +2317,7 @@
         <v>197</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>197</v>
+        <v>414</v>
       </c>
       <c r="I10" s="1">
         <v>1672</v>
@@ -2213,7 +2349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="30">
+    <row r="11" spans="1:20" ht="75">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2236,7 +2372,7 @@
         <v>198</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>198</v>
+        <v>413</v>
       </c>
       <c r="I11" s="1">
         <v>1570</v>
@@ -2291,7 +2427,7 @@
         <v>216</v>
       </c>
       <c r="H12" t="s">
-        <v>216</v>
+        <v>415</v>
       </c>
       <c r="I12" s="1">
         <v>1434</v>
@@ -2323,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="45">
+    <row r="13" spans="1:20" ht="60">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2346,7 +2482,7 @@
         <v>357</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>357</v>
+        <v>416</v>
       </c>
       <c r="I13" s="1">
         <v>1558</v>
@@ -2378,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="75">
+    <row r="14" spans="1:20" ht="105">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2401,7 +2537,7 @@
         <v>213</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>213</v>
+        <v>417</v>
       </c>
       <c r="I14" s="1">
         <v>1559.6189999999999</v>
@@ -2433,7 +2569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="75">
+    <row r="15" spans="1:20" ht="90">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2456,7 +2592,7 @@
         <v>214</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>214</v>
+        <v>418</v>
       </c>
       <c r="I15" s="1">
         <v>1542.066</v>
@@ -2511,7 +2647,7 @@
         <v>200</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>200</v>
+        <v>419</v>
       </c>
       <c r="I16" s="1">
         <v>1459.3779999999999</v>
@@ -2565,7 +2701,7 @@
         <v>217</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>217</v>
+        <v>420</v>
       </c>
       <c r="I17" s="1">
         <v>2189.3620000000001</v>
@@ -2596,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="105">
+    <row r="18" spans="1:19" ht="120">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -2619,7 +2755,7 @@
         <v>218</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>218</v>
+        <v>421</v>
       </c>
       <c r="I18" s="1">
         <v>2047.962</v>
@@ -2672,7 +2808,7 @@
         <v>199</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>199</v>
+        <v>422</v>
       </c>
       <c r="I19" s="1">
         <v>1901.21</v>
@@ -2834,7 +2970,7 @@
         <v>194</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>194</v>
+        <v>423</v>
       </c>
       <c r="K22" t="s">
         <v>54</v>
@@ -2884,7 +3020,7 @@
         <v>157</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>157</v>
+        <v>424</v>
       </c>
       <c r="K23" t="s">
         <v>54</v>
@@ -2934,7 +3070,7 @@
         <v>203</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>203</v>
+        <v>425</v>
       </c>
       <c r="K24" t="s">
         <v>54</v>
@@ -3034,7 +3170,7 @@
         <v>195</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>195</v>
+        <v>426</v>
       </c>
       <c r="J26" t="s">
         <v>169</v>
@@ -3087,7 +3223,7 @@
         <v>196</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>196</v>
+        <v>427</v>
       </c>
       <c r="J27" t="s">
         <v>169</v>
@@ -3143,7 +3279,7 @@
         <v>208</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>208</v>
+        <v>428</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>168</v>
@@ -3199,7 +3335,7 @@
         <v>190</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>190</v>
+        <v>429</v>
       </c>
       <c r="K29" t="s">
         <v>68</v>
@@ -3226,7 +3362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="120">
+    <row r="30" spans="1:19" ht="135">
       <c r="A30" t="s">
         <v>70</v>
       </c>
@@ -3249,7 +3385,7 @@
         <v>158</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>158</v>
+        <v>430</v>
       </c>
       <c r="I30" s="1">
         <v>2235.6489999999999</v>
@@ -3323,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="75">
+    <row r="32" spans="1:19" ht="90">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -3346,7 +3482,7 @@
         <v>227</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>227</v>
+        <v>431</v>
       </c>
       <c r="K32" t="s">
         <v>78</v>
@@ -3399,7 +3535,7 @@
         <v>253</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>253</v>
+        <v>432</v>
       </c>
       <c r="K33" t="s">
         <v>81</v>
@@ -3452,7 +3588,7 @@
         <v>207</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>207</v>
+        <v>433</v>
       </c>
       <c r="I34" s="1">
         <v>1934.5</v>
@@ -3505,7 +3641,7 @@
         <v>206</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>206</v>
+        <v>434</v>
       </c>
       <c r="I35" s="1">
         <v>1928.4169999999999</v>
@@ -3558,7 +3694,7 @@
         <v>221</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>221</v>
+        <v>435</v>
       </c>
       <c r="I36" s="1">
         <v>1925.375</v>
@@ -3611,7 +3747,7 @@
         <v>222</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>222</v>
+        <v>436</v>
       </c>
       <c r="I37" s="1">
         <v>1999.866</v>
@@ -3664,7 +3800,7 @@
         <v>223</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>223</v>
+        <v>437</v>
       </c>
       <c r="K38" t="s">
         <v>380</v>
@@ -3694,7 +3830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="75">
+    <row r="39" spans="1:19" ht="90">
       <c r="A39" t="s">
         <v>98</v>
       </c>
@@ -3717,7 +3853,7 @@
         <v>191</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>191</v>
+        <v>438</v>
       </c>
       <c r="I39" s="1">
         <v>1593.2249999999999</v>
@@ -3747,7 +3883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="60">
+    <row r="40" spans="1:19" ht="75">
       <c r="A40" t="s">
         <v>100</v>
       </c>
@@ -3770,7 +3906,7 @@
         <v>159</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>159</v>
+        <v>439</v>
       </c>
       <c r="I40" s="1">
         <v>2624.9580000000001</v>
@@ -3927,7 +4063,7 @@
         <v>205</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>205</v>
+        <v>440</v>
       </c>
       <c r="I43" s="1">
         <v>1543.018</v>
@@ -3980,7 +4116,7 @@
         <v>225</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>225</v>
+        <v>442</v>
       </c>
       <c r="I44" s="1">
         <v>2004.07</v>
@@ -4033,7 +4169,7 @@
         <v>204</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>204</v>
+        <v>441</v>
       </c>
       <c r="I45" s="1">
         <v>994.59460000000001</v>
@@ -4086,7 +4222,7 @@
         <v>210</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>210</v>
+        <v>443</v>
       </c>
       <c r="I46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
@@ -4143,7 +4279,7 @@
         <v>209</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>209</v>
+        <v>444</v>
       </c>
       <c r="I47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
@@ -4200,7 +4336,7 @@
         <v>230</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>230</v>
+        <v>445</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" t="s">
@@ -4254,7 +4390,7 @@
         <v>233</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>233</v>
+        <v>446</v>
       </c>
       <c r="K49" t="s">
         <v>343</v>
@@ -4307,7 +4443,7 @@
         <v>240</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>240</v>
+        <v>447</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>239</v>
@@ -4360,7 +4496,7 @@
         <v>245</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>245</v>
+        <v>448</v>
       </c>
       <c r="K51" t="s">
         <v>242</v>
@@ -4413,7 +4549,7 @@
         <v>250</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>250</v>
+        <v>449</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
* added Introduction * fixed spelling mistakes in programs.xlsx
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -1337,9 +1337,6 @@
     <t>Im Jahr 1990  wurde das BAföG grundlegend reformiert. Zuvor musste das gesamte Darlehen zurückgezahlt werden. Seit 1990 wird im Regelfall etwa die Hälfte des Darlehens als Zuschuss gewährt und muss somit nicht zurückgezahlt werden.</t>
   </si>
   <si>
-    <t>Im Jahr 2001 wurde die Einkommensgrenze der Eltern bis zu der Studienrende BAföG beziehen konnten um 20 Prozent angehoben. Dadruch stieg die Anzahl der BAföG Berechtigten um circa 50 Prozent.</t>
-  </si>
-  <si>
     <t>Das deutsche Arbeitslosenversicherungssystem weist einige Sprungsstellen auf an welchen sich abhängig vom Alter die maximale Bezugsdauer ändert.  Dadurch lassen sich Rückschlüsse über den Anreizeffekt der Arbeitslosenversicherung schließen und es kann ein MVPF für die Ausweitung der Bezugsdauer im Alter von 42 berechnet werden.</t>
   </si>
   <si>
@@ -1389,6 +1386,9 @@
   </si>
   <si>
     <t xml:space="preserve">Zwischen 1965 und 1996 wurde in allen deutschen Bundesländern die mittlere Reife, also der Realschulabschluss als Zwischenabschluss des Gymnasiums eingeführt. Mit erfolgreicher Beendigung der 10. Klasse erhalten Schüler die mittlere Reife, auch wenn sie die Oberstufe des Gymnasiums nicht abschließen. </t>
+  </si>
+  <si>
+    <t>Im Jahr 2001 wurde die Einkommensgrenze der Eltern bis zu der Studierende BAföG beziehen konnten um 20 Prozent angehoben. Dadurch stieg die Anzahl der BAföG Berechtigten um circa 50 Prozent.</t>
   </si>
 </sst>
 </file>
@@ -1761,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3535,7 +3535,7 @@
         <v>253</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>432</v>
+        <v>449</v>
       </c>
       <c r="K33" t="s">
         <v>81</v>
@@ -3588,7 +3588,7 @@
         <v>207</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I34" s="1">
         <v>1934.5</v>
@@ -3641,7 +3641,7 @@
         <v>206</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I35" s="1">
         <v>1928.4169999999999</v>
@@ -3694,7 +3694,7 @@
         <v>221</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I36" s="1">
         <v>1925.375</v>
@@ -3747,7 +3747,7 @@
         <v>222</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I37" s="1">
         <v>1999.866</v>
@@ -3800,7 +3800,7 @@
         <v>223</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K38" t="s">
         <v>380</v>
@@ -3853,7 +3853,7 @@
         <v>191</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I39" s="1">
         <v>1593.2249999999999</v>
@@ -3906,7 +3906,7 @@
         <v>159</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I40" s="1">
         <v>2624.9580000000001</v>
@@ -4063,7 +4063,7 @@
         <v>205</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I43" s="1">
         <v>1543.018</v>
@@ -4116,7 +4116,7 @@
         <v>225</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I44" s="1">
         <v>2004.07</v>
@@ -4169,7 +4169,7 @@
         <v>204</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I45" s="1">
         <v>994.59460000000001</v>
@@ -4222,7 +4222,7 @@
         <v>210</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I46" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
@@ -4279,7 +4279,7 @@
         <v>209</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I47" s="1">
         <f>2811.18 * 10^9 /(80 * 10^6) / 12</f>
@@ -4336,7 +4336,7 @@
         <v>230</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" t="s">
@@ -4390,7 +4390,7 @@
         <v>233</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K49" t="s">
         <v>343</v>
@@ -4443,7 +4443,7 @@
         <v>240</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>239</v>
@@ -4496,7 +4496,7 @@
         <v>245</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="K51" t="s">
         <v>242</v>
@@ -4549,7 +4549,7 @@
         <v>250</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>249</v>

</xml_diff>